<commit_message>
Lots of Harlequin Content
</commit_message>
<xml_diff>
--- a/Balancing Sheet.xlsx
+++ b/Balancing Sheet.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Space Marines" sheetId="1" r:id="rId1"/>
     <sheet name="Chaos Space Marines" sheetId="2" r:id="rId2"/>
     <sheet name="Eldar" sheetId="4" r:id="rId3"/>
+    <sheet name="Harlequins" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="143">
   <si>
     <t>Name</t>
   </si>
@@ -432,6 +433,42 @@
   <si>
     <t>Lethal Weapon    .</t>
   </si>
+  <si>
+    <t>Harlequin’s Kiss</t>
+  </si>
+  <si>
+    <t>Harlequin’s Caress</t>
+  </si>
+  <si>
+    <t>Miststave</t>
+  </si>
+  <si>
+    <t>Harlequin’s Embrace</t>
+  </si>
+  <si>
+    <t>Neuro Disruptor</t>
+  </si>
+  <si>
+    <t>Shuriken Cannon</t>
+  </si>
+  <si>
+    <t>Haywire Cannon</t>
+  </si>
+  <si>
+    <t>Prism Cannon</t>
+  </si>
+  <si>
+    <t>Zephyrglaive 2H</t>
+  </si>
+  <si>
+    <t>Cleave, Wide Range</t>
+  </si>
+  <si>
+    <t>Burst</t>
+  </si>
+  <si>
+    <t>Stunned</t>
+  </si>
 </sst>
 </file>
 
@@ -508,7 +545,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -591,13 +628,512 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="94">
+  <dxfs count="124">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="180" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2166,60 +2702,60 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:AB38" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92" dataCellStyle="Percent">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:AB38" totalsRowShown="0" headerRowDxfId="123" dataDxfId="122" dataCellStyle="Percent">
   <autoFilter ref="B3:AB38"/>
   <tableColumns count="27">
-    <tableColumn id="1" name="Name" dataDxfId="91"/>
-    <tableColumn id="2" name="Damage" dataDxfId="90"/>
-    <tableColumn id="3" name="Attacks" dataDxfId="89"/>
-    <tableColumn id="5" name="Note" dataDxfId="88"/>
-    <tableColumn id="6" name="Penetration" dataDxfId="87"/>
-    <tableColumn id="23" name="MM      ." dataDxfId="86"/>
-    <tableColumn id="24" name="Crit       ." dataDxfId="85"/>
-    <tableColumn id="4" name="CB       ." dataDxfId="84"/>
-    <tableColumn id="26" name="Weak Spots" dataDxfId="83"/>
-    <tableColumn id="25" name="Cone      ." dataDxfId="82"/>
-    <tableColumn id="29" name="No Crits     ." dataDxfId="81"/>
-    <tableColumn id="32" name="2H        ." dataDxfId="80"/>
-    <tableColumn id="27" name="Column2" dataDxfId="79"/>
-    <tableColumn id="7" name="Hit%" dataDxfId="78" dataCellStyle="Percent">
+    <tableColumn id="1" name="Name" dataDxfId="121"/>
+    <tableColumn id="2" name="Damage" dataDxfId="120"/>
+    <tableColumn id="3" name="Attacks" dataDxfId="119"/>
+    <tableColumn id="5" name="Note" dataDxfId="118"/>
+    <tableColumn id="6" name="Penetration" dataDxfId="117"/>
+    <tableColumn id="23" name="MM      ." dataDxfId="116"/>
+    <tableColumn id="24" name="Crit       ." dataDxfId="115"/>
+    <tableColumn id="4" name="CB       ." dataDxfId="114"/>
+    <tableColumn id="26" name="Weak Spots" dataDxfId="113"/>
+    <tableColumn id="25" name="Cone      ." dataDxfId="112"/>
+    <tableColumn id="29" name="No Crits     ." dataDxfId="111"/>
+    <tableColumn id="32" name="2H        ." dataDxfId="110"/>
+    <tableColumn id="27" name="Column2" dataDxfId="109"/>
+    <tableColumn id="7" name="Hit%" dataDxfId="108" dataCellStyle="Percent">
       <calculatedColumnFormula>($AE$3 )/20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Wound%" dataDxfId="77" dataCellStyle="Percent">
+    <tableColumn id="8" name="Wound%" dataDxfId="107" dataCellStyle="Percent">
       <calculatedColumnFormula>(C4/20)*IF($AH$6=1,0.5,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Crit%" dataDxfId="76" dataCellStyle="Percent">
+    <tableColumn id="9" name="Crit%" dataDxfId="106" dataCellStyle="Percent">
       <calculatedColumnFormula>(IF(( L4="X"),0,($AE$6+H4))/20)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="WoundsÆ" dataDxfId="75">
+    <tableColumn id="11" name="WoundsÆ" dataDxfId="105">
       <calculatedColumnFormula>1*P4*(O4)*(1+Q4)*D4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="% Base" dataDxfId="74" dataCellStyle="Percent">
+    <tableColumn id="12" name="% Base" dataDxfId="104" dataCellStyle="Percent">
       <calculatedColumnFormula>R4/$R$27</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="To Kill" dataDxfId="73" dataCellStyle="Percent">
+    <tableColumn id="20" name="To Kill" dataDxfId="103" dataCellStyle="Percent">
       <calculatedColumnFormula>AH9/Table1[[#This Row],[WoundsÆ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Column3" dataDxfId="72"/>
-    <tableColumn id="14" name="Hit %" dataDxfId="71" dataCellStyle="Percent">
+    <tableColumn id="13" name="Column3" dataDxfId="102"/>
+    <tableColumn id="14" name="Hit %" dataDxfId="101" dataCellStyle="Percent">
       <calculatedColumnFormula>($AE$3)/20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Wound %" dataDxfId="70" dataCellStyle="Percent">
+    <tableColumn id="15" name="Wound %" dataDxfId="100" dataCellStyle="Percent">
       <calculatedColumnFormula>(C4/20)*IF($AH$6=1,IF(F4="X",1,0.5),1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Crit %" dataDxfId="69" dataCellStyle="Percent">
+    <tableColumn id="16" name="Crit %" dataDxfId="99" dataCellStyle="Percent">
       <calculatedColumnFormula>($AE$6/20)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="WoundÆ" dataDxfId="68">
+    <tableColumn id="18" name="WoundÆ" dataDxfId="98">
       <calculatedColumnFormula>1*W4*(V4)*(1+X4)*D4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="% Base2" dataDxfId="67" dataCellStyle="Percent">
+    <tableColumn id="19" name="% Base2" dataDxfId="97" dataCellStyle="Percent">
       <calculatedColumnFormula>Y4/$Y$27</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="To Kill2" dataDxfId="66" dataCellStyle="Percent">
+    <tableColumn id="21" name="To Kill2" dataDxfId="96" dataCellStyle="Percent">
       <calculatedColumnFormula>$AH$9/Table1[[#This Row],[WoundÆ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="Combo" dataDxfId="65" dataCellStyle="Percent">
+    <tableColumn id="22" name="Combo" dataDxfId="95" dataCellStyle="Percent">
       <calculatedColumnFormula>(Table1[[#This Row],[% Base]]+Table1[[#This Row],[% Base2]])/2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2228,64 +2764,64 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="B3:AF40" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63" dataCellStyle="Percent">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="B3:AF40" totalsRowShown="0" headerRowDxfId="94" dataDxfId="93" dataCellStyle="Percent">
   <autoFilter ref="B3:AF40"/>
   <tableColumns count="31">
-    <tableColumn id="1" name="Name" dataDxfId="62"/>
-    <tableColumn id="2" name="Damage" dataDxfId="61"/>
-    <tableColumn id="3" name="Attacks" dataDxfId="60"/>
-    <tableColumn id="5" name="Note" dataDxfId="59"/>
-    <tableColumn id="6" name="Penetration" dataDxfId="58"/>
-    <tableColumn id="23" name="MM      ." dataDxfId="57"/>
-    <tableColumn id="24" name="Crit       ." dataDxfId="56"/>
-    <tableColumn id="26" name="Weak Spots" dataDxfId="55"/>
-    <tableColumn id="25" name="Cone      ." dataDxfId="54"/>
-    <tableColumn id="29" name="No Crits     ." dataDxfId="53"/>
-    <tableColumn id="32" name="2H        ." dataDxfId="52"/>
-    <tableColumn id="33" name="Heavy Strikes      ." dataDxfId="51"/>
-    <tableColumn id="4" name="XAmmo       ." dataDxfId="50"/>
-    <tableColumn id="28" name="Lethal Weapon" dataDxfId="49"/>
-    <tableColumn id="27" name="Column2" dataDxfId="48"/>
-    <tableColumn id="7" name="Hit%" dataDxfId="47" dataCellStyle="Percent">
+    <tableColumn id="1" name="Name" dataDxfId="92"/>
+    <tableColumn id="2" name="Damage" dataDxfId="91"/>
+    <tableColumn id="3" name="Attacks" dataDxfId="90"/>
+    <tableColumn id="5" name="Note" dataDxfId="89"/>
+    <tableColumn id="6" name="Penetration" dataDxfId="88"/>
+    <tableColumn id="23" name="MM      ." dataDxfId="87"/>
+    <tableColumn id="24" name="Crit       ." dataDxfId="86"/>
+    <tableColumn id="26" name="Weak Spots" dataDxfId="85"/>
+    <tableColumn id="25" name="Cone      ." dataDxfId="84"/>
+    <tableColumn id="29" name="No Crits     ." dataDxfId="83"/>
+    <tableColumn id="32" name="2H        ." dataDxfId="82"/>
+    <tableColumn id="33" name="Heavy Strikes      ." dataDxfId="81"/>
+    <tableColumn id="4" name="XAmmo       ." dataDxfId="80"/>
+    <tableColumn id="28" name="Lethal Weapon" dataDxfId="79"/>
+    <tableColumn id="27" name="Column2" dataDxfId="78"/>
+    <tableColumn id="7" name="Hit%" dataDxfId="77" dataCellStyle="Percent">
       <calculatedColumnFormula>($AI$3 )/20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Wound%" dataDxfId="46" dataCellStyle="Percent">
+    <tableColumn id="8" name="Wound%" dataDxfId="76" dataCellStyle="Percent">
       <calculatedColumnFormula>(C4/20)*IF($AL$5=1,0.5,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Crit%" dataDxfId="45" dataCellStyle="Percent">
+    <tableColumn id="9" name="Crit%" dataDxfId="75" dataCellStyle="Percent">
       <calculatedColumnFormula>(IF(( K4="X"),0,($AI$5+H4))/20)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Block%" dataDxfId="44" dataCellStyle="Percent"/>
-    <tableColumn id="11" name="WoundsÆ" dataDxfId="43">
+    <tableColumn id="10" name="Block%" dataDxfId="74" dataCellStyle="Percent"/>
+    <tableColumn id="11" name="WoundsÆ" dataDxfId="73">
       <calculatedColumnFormula>1*R4*(Q4)*(1+S4)*D4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="% Base" dataDxfId="42" dataCellStyle="Percent">
+    <tableColumn id="12" name="% Base" dataDxfId="72" dataCellStyle="Percent">
       <calculatedColumnFormula>U4/$U$28</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="To Kill" dataDxfId="41" dataCellStyle="Percent">
+    <tableColumn id="20" name="To Kill" dataDxfId="71" dataCellStyle="Percent">
       <calculatedColumnFormula>AL9/Table14[[#This Row],[WoundsÆ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Column3" dataDxfId="40"/>
-    <tableColumn id="14" name="Hit %" dataDxfId="39" dataCellStyle="Percent">
+    <tableColumn id="13" name="Column3" dataDxfId="70"/>
+    <tableColumn id="14" name="Hit %" dataDxfId="69" dataCellStyle="Percent">
       <calculatedColumnFormula>($AI$3)/20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Wound %" dataDxfId="38" dataCellStyle="Percent">
+    <tableColumn id="15" name="Wound %" dataDxfId="68" dataCellStyle="Percent">
       <calculatedColumnFormula>(C4/20)*IF($AL$5=1,IF(F4="X",1,0.5),1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Crit %" dataDxfId="37" dataCellStyle="Percent">
+    <tableColumn id="16" name="Crit %" dataDxfId="67" dataCellStyle="Percent">
       <calculatedColumnFormula>($AI$5/20)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Block %" dataDxfId="36" dataCellStyle="Percent"/>
-    <tableColumn id="18" name="WoundÆ" dataDxfId="35">
+    <tableColumn id="17" name="Block %" dataDxfId="66" dataCellStyle="Percent"/>
+    <tableColumn id="18" name="WoundÆ" dataDxfId="65">
       <calculatedColumnFormula>1*Z4*(Y4)*(1+AA4)*D4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="% Base2" dataDxfId="34" dataCellStyle="Percent">
+    <tableColumn id="19" name="% Base2" dataDxfId="64" dataCellStyle="Percent">
       <calculatedColumnFormula>AC4/$AC$28</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="To Kill2" dataDxfId="33" dataCellStyle="Percent">
+    <tableColumn id="21" name="To Kill2" dataDxfId="63" dataCellStyle="Percent">
       <calculatedColumnFormula>$AL$9/Table14[[#This Row],[WoundÆ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="Combo" dataDxfId="32" dataCellStyle="Percent">
+    <tableColumn id="22" name="Combo" dataDxfId="62" dataCellStyle="Percent">
       <calculatedColumnFormula>(Table14[[#This Row],[% Base]]+Table14[[#This Row],[% Base2]])/2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2294,64 +2830,127 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="B3:AE35" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30" dataCellStyle="Percent">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="B3:AE35" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60" dataCellStyle="Percent">
   <autoFilter ref="B3:AE35"/>
   <tableColumns count="30">
-    <tableColumn id="1" name="Name" dataDxfId="29"/>
-    <tableColumn id="2" name="Damage" dataDxfId="28"/>
-    <tableColumn id="3" name="Attacks" dataDxfId="27"/>
-    <tableColumn id="5" name="Note" dataDxfId="26"/>
-    <tableColumn id="6" name="Penetration" dataDxfId="25"/>
-    <tableColumn id="30" name="Light Weapon    ." dataDxfId="24"/>
-    <tableColumn id="23" name="MM      ." dataDxfId="23"/>
-    <tableColumn id="24" name="Crit       ." dataDxfId="22"/>
-    <tableColumn id="26" name="Weak Spots" dataDxfId="21"/>
-    <tableColumn id="25" name="Cone      ." dataDxfId="20"/>
-    <tableColumn id="29" name="No Crits     ." dataDxfId="19"/>
-    <tableColumn id="32" name="2H        ." dataDxfId="18"/>
-    <tableColumn id="33" name="Heavy Strikes      ." dataDxfId="17"/>
+    <tableColumn id="1" name="Name" dataDxfId="59"/>
+    <tableColumn id="2" name="Damage" dataDxfId="58"/>
+    <tableColumn id="3" name="Attacks" dataDxfId="57"/>
+    <tableColumn id="5" name="Note" dataDxfId="56"/>
+    <tableColumn id="6" name="Penetration" dataDxfId="55"/>
+    <tableColumn id="30" name="Light Weapon    ." dataDxfId="54"/>
+    <tableColumn id="23" name="MM      ." dataDxfId="53"/>
+    <tableColumn id="24" name="Crit       ." dataDxfId="52"/>
+    <tableColumn id="26" name="Weak Spots" dataDxfId="51"/>
+    <tableColumn id="25" name="Cone      ." dataDxfId="50"/>
+    <tableColumn id="29" name="No Crits     ." dataDxfId="49"/>
+    <tableColumn id="32" name="2H        ." dataDxfId="48"/>
+    <tableColumn id="33" name="Heavy Strikes      ." dataDxfId="47"/>
+    <tableColumn id="4" name="Lethal Wounds    ." dataDxfId="46"/>
+    <tableColumn id="28" name="Lethal Weapon    ." dataDxfId="45"/>
+    <tableColumn id="27" name="Column2" dataDxfId="44"/>
+    <tableColumn id="7" name="Hit%" dataDxfId="43" dataCellStyle="Percent">
+      <calculatedColumnFormula>($AH$3 )/20</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" name="Wound%" dataDxfId="42" dataCellStyle="Percent">
+      <calculatedColumnFormula>(C4/20)*IF($AK$6=1,0.5,1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" name="Crit%" dataDxfId="41" dataCellStyle="Percent">
+      <calculatedColumnFormula>(IF(( L4="X"),0,($AH$5+I4))/20)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" name="WoundsÆ" dataDxfId="40">
+      <calculatedColumnFormula>1*S4*(R4)*(1+T4)*D4</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="12" name="% Base" dataDxfId="39" dataCellStyle="Percent">
+      <calculatedColumnFormula>U4/$U$25</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="20" name="To Kill" dataDxfId="38" dataCellStyle="Percent">
+      <calculatedColumnFormula>AK9/Table145[[#This Row],[WoundsÆ]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" name="Column3" dataDxfId="37"/>
+    <tableColumn id="14" name="Hit %" dataDxfId="36" dataCellStyle="Percent">
+      <calculatedColumnFormula>($AH$3)/20</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="15" name="Wound %" dataDxfId="35" dataCellStyle="Percent">
+      <calculatedColumnFormula>(C4/20)*IF($AK$6=1,IF(F4="X",1,0.5),1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="16" name="Crit %" dataDxfId="34" dataCellStyle="Percent">
+      <calculatedColumnFormula>($AH$5/20)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="18" name="WoundÆ" dataDxfId="33">
+      <calculatedColumnFormula>1*Z4*(Y4)*(1+AA4)*D4</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="19" name="% Base2" dataDxfId="32" dataCellStyle="Percent">
+      <calculatedColumnFormula>AB4/$AB$25</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="21" name="To Kill2" dataDxfId="31" dataCellStyle="Percent">
+      <calculatedColumnFormula>$AK$9/Table145[[#This Row],[WoundÆ]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="22" name="Combo" dataDxfId="30" dataCellStyle="Percent">
+      <calculatedColumnFormula>(Table145[[#This Row],[% Base]]+Table145[[#This Row],[% Base2]])/2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table1453" displayName="Table1453" ref="B3:AC35" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" dataCellStyle="Percent">
+  <autoFilter ref="B3:AC35"/>
+  <tableColumns count="28">
+    <tableColumn id="1" name="Name" dataDxfId="27"/>
+    <tableColumn id="2" name="Damage" dataDxfId="26"/>
+    <tableColumn id="3" name="Attacks" dataDxfId="25"/>
+    <tableColumn id="5" name="Note" dataDxfId="24"/>
+    <tableColumn id="6" name="Penetration" dataDxfId="23"/>
+    <tableColumn id="30" name="Light Weapon    ." dataDxfId="22"/>
+    <tableColumn id="23" name="MM      ." dataDxfId="21"/>
+    <tableColumn id="24" name="Crit       ." dataDxfId="20"/>
+    <tableColumn id="26" name="Weak Spots" dataDxfId="19"/>
+    <tableColumn id="25" name="Cone      ." dataDxfId="18"/>
+    <tableColumn id="29" name="No Crits     ." dataDxfId="17"/>
     <tableColumn id="4" name="Lethal Wounds    ." dataDxfId="16"/>
     <tableColumn id="28" name="Lethal Weapon    ." dataDxfId="15"/>
     <tableColumn id="27" name="Column2" dataDxfId="14"/>
     <tableColumn id="7" name="Hit%" dataDxfId="13" dataCellStyle="Percent">
-      <calculatedColumnFormula>($AH$3 )/20</calculatedColumnFormula>
+      <calculatedColumnFormula>($AF$3 )/20</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" name="Wound%" dataDxfId="12" dataCellStyle="Percent">
-      <calculatedColumnFormula>(C4/20)*IF($AK$6=1,0.5,1)</calculatedColumnFormula>
+      <calculatedColumnFormula>(C4/20)*IF($AI$6=1,0.5,1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" name="Crit%" dataDxfId="11" dataCellStyle="Percent">
-      <calculatedColumnFormula>(IF(( L4="X"),0,($AH$5+I4))/20)</calculatedColumnFormula>
+      <calculatedColumnFormula>(IF(( L4="X"),0,($AF$5+I4))/20)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" name="WoundsÆ" dataDxfId="10">
-      <calculatedColumnFormula>1*S4*(R4)*(1+T4)*D4</calculatedColumnFormula>
+      <calculatedColumnFormula>1*Q4*(P4)*(1+R4)*D4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="12" name="% Base" dataDxfId="9" dataCellStyle="Percent">
-      <calculatedColumnFormula>U4/$U$25</calculatedColumnFormula>
+      <calculatedColumnFormula>S4/$S$25</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="20" name="To Kill" dataDxfId="8" dataCellStyle="Percent">
-      <calculatedColumnFormula>AK9/Table145[[#This Row],[WoundsÆ]]</calculatedColumnFormula>
+      <calculatedColumnFormula>AI9/Table1453[[#This Row],[WoundsÆ]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" name="Column3" dataDxfId="7"/>
     <tableColumn id="14" name="Hit %" dataDxfId="6" dataCellStyle="Percent">
-      <calculatedColumnFormula>($AH$3)/20</calculatedColumnFormula>
+      <calculatedColumnFormula>($AF$3)/20</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="15" name="Wound %" dataDxfId="5" dataCellStyle="Percent">
-      <calculatedColumnFormula>(C4/20)*IF($AK$6=1,IF(F4="X",1,0.5),1)</calculatedColumnFormula>
+      <calculatedColumnFormula>(C4/20)*IF($AI$6=1,IF(F4="X",1,0.5),1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="16" name="Crit %" dataDxfId="4" dataCellStyle="Percent">
-      <calculatedColumnFormula>($AH$5/20)</calculatedColumnFormula>
+      <calculatedColumnFormula>($AF$5/20)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="18" name="WoundÆ" dataDxfId="3">
-      <calculatedColumnFormula>1*Z4*(Y4)*(1+AA4)*D4</calculatedColumnFormula>
+      <calculatedColumnFormula>1*X4*(W4)*(1+Y4)*D4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="19" name="% Base2" dataDxfId="2" dataCellStyle="Percent">
-      <calculatedColumnFormula>AB4/$AB$25</calculatedColumnFormula>
+      <calculatedColumnFormula>Z4/$Z$25</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="21" name="To Kill2" dataDxfId="1" dataCellStyle="Percent">
-      <calculatedColumnFormula>$AK$9/Table145[[#This Row],[WoundÆ]]</calculatedColumnFormula>
+      <calculatedColumnFormula>$AI$9/Table1453[[#This Row],[WoundÆ]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="22" name="Combo" dataDxfId="0" dataCellStyle="Percent">
-      <calculatedColumnFormula>(Table145[[#This Row],[% Base]]+Table145[[#This Row],[% Base2]])/2</calculatedColumnFormula>
+      <calculatedColumnFormula>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2657,8 +3256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AH66"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2678,24 +3277,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="O2" s="31" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="O2" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="V2" s="31" t="s">
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="V2" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="31"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
       <c r="Z2" s="1"/>
       <c r="AA2" s="2"/>
       <c r="AD2" t="s">
@@ -6339,26 +6938,26 @@
   <sheetData>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="Q2" s="31" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="Q2" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
-      <c r="Y2" s="31" t="s">
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="Y2" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="Z2" s="31"/>
-      <c r="AA2" s="31"/>
-      <c r="AB2" s="31"/>
-      <c r="AC2" s="31"/>
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="32"/>
       <c r="AD2" s="25"/>
       <c r="AE2" s="25"/>
       <c r="AH2" t="s">
@@ -9456,7 +10055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AK43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
@@ -9469,24 +10068,24 @@
   <sheetData>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="R2" s="31" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="R2" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
-      <c r="Y2" s="31" t="s">
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="Y2" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="Z2" s="31"/>
-      <c r="AA2" s="31"/>
-      <c r="AB2" s="31"/>
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
       <c r="AC2" s="28"/>
       <c r="AD2" s="28"/>
       <c r="AG2" t="s">
@@ -9496,7 +10095,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:37" ht="88.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" ht="87.75" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
         <v>0</v>
@@ -11428,23 +12027,23 @@
       <c r="P31" s="3"/>
       <c r="Q31" s="3"/>
       <c r="R31" s="5">
-        <f t="shared" ref="R30:R32" si="16">($AH$3 )/20</f>
+        <f t="shared" ref="R31:R32" si="16">($AH$3 )/20</f>
         <v>0.5</v>
       </c>
       <c r="S31" s="5">
-        <f t="shared" ref="S30:S32" si="17">(C31/20)*IF($AK$6=1,0.5,1)</f>
+        <f t="shared" ref="S31:S32" si="17">(C31/20)*IF($AK$6=1,0.5,1)</f>
         <v>0.75</v>
       </c>
       <c r="T31" s="5">
-        <f t="shared" ref="T30:T32" si="18">(IF(( L31="X"),0,($AH$5+I31))/20)</f>
+        <f t="shared" ref="T31:T32" si="18">(IF(( L31="X"),0,($AH$5+I31))/20)</f>
         <v>0.1</v>
       </c>
       <c r="U31" s="8">
-        <f t="shared" ref="U30:U32" si="19">1*S31*(R31)*(1+T31)*D31</f>
+        <f t="shared" ref="U31:U32" si="19">1*S31*(R31)*(1+T31)*D31</f>
         <v>1.6500000000000001</v>
       </c>
       <c r="V31" s="5">
-        <f t="shared" ref="V30:V32" si="20">U31/$U$25</f>
+        <f t="shared" ref="V31:V32" si="20">U31/$U$25</f>
         <v>0.83018867924528306</v>
       </c>
       <c r="W31" s="23">
@@ -11453,23 +12052,23 @@
       </c>
       <c r="X31" s="6"/>
       <c r="Y31" s="5">
-        <f t="shared" ref="Y30:Y32" si="21">($AH$3)/20</f>
+        <f t="shared" ref="Y31:Y32" si="21">($AH$3)/20</f>
         <v>0.5</v>
       </c>
       <c r="Z31" s="5">
-        <f t="shared" ref="Z30:Z32" si="22">(C31/20)*IF($AK$6=1,IF(F31="X",1,0.5),1)</f>
+        <f t="shared" ref="Z31:Z32" si="22">(C31/20)*IF($AK$6=1,IF(F31="X",1,0.5),1)</f>
         <v>0.75</v>
       </c>
       <c r="AA31" s="5">
-        <f t="shared" ref="AA30:AA32" si="23">($AH$5/20)</f>
+        <f t="shared" ref="AA31:AA32" si="23">($AH$5/20)</f>
         <v>0.1</v>
       </c>
       <c r="AB31" s="8">
-        <f t="shared" ref="AB30:AB32" si="24">1*Z31*(Y31)*(1+AA31)*D31</f>
+        <f t="shared" ref="AB31:AB32" si="24">1*Z31*(Y31)*(1+AA31)*D31</f>
         <v>1.6500000000000001</v>
       </c>
       <c r="AC31" s="5">
-        <f t="shared" ref="AC30:AC32" si="25">AB31/$AB$25</f>
+        <f t="shared" ref="AC31:AC32" si="25">AB31/$AB$25</f>
         <v>1.6603773584905661</v>
       </c>
       <c r="AD31" s="24">
@@ -11687,23 +12286,23 @@
       <c r="P35" s="11"/>
       <c r="Q35" s="11"/>
       <c r="R35" s="5">
-        <f t="shared" ref="R33:R35" si="35">($AH$3 )/20</f>
+        <f t="shared" ref="R35" si="35">($AH$3 )/20</f>
         <v>0.5</v>
       </c>
       <c r="S35" s="5">
-        <f t="shared" ref="S33:S35" si="36">(C35/20)*IF($AK$6=1,0.5,1)</f>
+        <f t="shared" ref="S35" si="36">(C35/20)*IF($AK$6=1,0.5,1)</f>
         <v>0</v>
       </c>
       <c r="T35" s="5">
-        <f t="shared" ref="T33:T35" si="37">(IF(( L35="X"),0,($AH$5+I35))/20)</f>
+        <f t="shared" ref="T35" si="37">(IF(( L35="X"),0,($AH$5+I35))/20)</f>
         <v>0.1</v>
       </c>
       <c r="U35" s="8">
-        <f t="shared" ref="U33:U35" si="38">1*S35*(R35)*(1+T35)*D35</f>
+        <f t="shared" ref="U35" si="38">1*S35*(R35)*(1+T35)*D35</f>
         <v>0</v>
       </c>
       <c r="V35" s="5">
-        <f t="shared" ref="V33:V35" si="39">U35/$U$25</f>
+        <f t="shared" ref="V35" si="39">U35/$U$25</f>
         <v>0</v>
       </c>
       <c r="W35" s="23" t="e">
@@ -11712,23 +12311,23 @@
       </c>
       <c r="X35" s="6"/>
       <c r="Y35" s="5">
-        <f t="shared" ref="Y33:Y35" si="40">($AH$3)/20</f>
+        <f t="shared" ref="Y35" si="40">($AH$3)/20</f>
         <v>0.5</v>
       </c>
       <c r="Z35" s="5">
-        <f t="shared" ref="Z33:Z35" si="41">(C35/20)*IF($AK$6=1,IF(F35="X",1,0.5),1)</f>
+        <f t="shared" ref="Z35" si="41">(C35/20)*IF($AK$6=1,IF(F35="X",1,0.5),1)</f>
         <v>0</v>
       </c>
       <c r="AA35" s="5">
-        <f t="shared" ref="AA33:AA35" si="42">($AH$5/20)</f>
+        <f t="shared" ref="AA35" si="42">($AH$5/20)</f>
         <v>0.1</v>
       </c>
       <c r="AB35" s="8">
-        <f t="shared" ref="AB33:AB35" si="43">1*Z35*(Y35)*(1+AA35)*D35</f>
+        <f t="shared" ref="AB35" si="43">1*Z35*(Y35)*(1+AA35)*D35</f>
         <v>0</v>
       </c>
       <c r="AC35" s="5">
-        <f t="shared" ref="AC33:AC35" si="44">AB35/$AB$25</f>
+        <f t="shared" ref="AC35" si="44">AB35/$AB$25</f>
         <v>0</v>
       </c>
       <c r="AD35" s="24" t="e">
@@ -12048,7 +12647,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD30 W30">
+  <conditionalFormatting sqref="W30 AD30">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -12060,7 +12659,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC30 V30">
+  <conditionalFormatting sqref="V30 AC30">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -12084,7 +12683,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD34 W34">
+  <conditionalFormatting sqref="W34 AD34">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -12096,7 +12695,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC34 V34">
+  <conditionalFormatting sqref="V34 AC34">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -12126,4 +12725,2657 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:AI43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Z5" sqref="Z5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="14" width="3.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A2" s="26"/>
+      <c r="B2" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="P2" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="W2" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="31"/>
+      <c r="AB2" s="31"/>
+      <c r="AE2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" ht="88.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="P3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="R3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="S3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="T3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="U3" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="V3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="W3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="X3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z3" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA3" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB3" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC3" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF3">
+        <v>10</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="3">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="5">
+        <f>(10+$AF$4-$AI$5)/20</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q4" s="5">
+        <f>(C4/20)*IF($AI$6=1,IF(F4="X",1,0.5),1)</f>
+        <v>0.5</v>
+      </c>
+      <c r="R4" s="5">
+        <f>(IF(( L4="X"),0,($AF$5+I4))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S4" s="8">
+        <f>1*Q4*P4*(1+R4)*D4 + IF(N4="X",D4*P4*0.25,0) + IF(M4="X",D4*P4*Q4*0.5,0)</f>
+        <v>0.82500000000000007</v>
+      </c>
+      <c r="T4" s="5">
+        <f>S4/$S$4</f>
+        <v>1</v>
+      </c>
+      <c r="U4" s="10">
+        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]/2</f>
+        <v>2.4242424242424239</v>
+      </c>
+      <c r="V4" s="6"/>
+      <c r="W4" s="5">
+        <f>(10+$AF$4-$AI$5)/20</f>
+        <v>0.5</v>
+      </c>
+      <c r="X4" s="5">
+        <f>(C4/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Y4" s="5">
+        <f>(IF((OR(K4="X", L4="X")),0,($AF$5+I4))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z4" s="8">
+        <f>IF(G4="X",0,1*X4*W4*(1+Y4)*D4) * IF($AI$13=1,IF(F4="X",1,0.5),1) + IF(N4="X",D4*P4*0.25,0)</f>
+        <v>0.41250000000000003</v>
+      </c>
+      <c r="AA4" s="5">
+        <f>Z4/$Z$4</f>
+        <v>1</v>
+      </c>
+      <c r="AB4" s="10">
+        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]/2</f>
+        <v>4.8484848484848477</v>
+      </c>
+      <c r="AC4" s="5">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>1</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF4">
+        <v>10</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AI4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="3">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="5">
+        <f>(10+$AF$4-$AI$5)/20</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q5" s="5">
+        <f>(C5/20)*IF($AI$6=1,IF(F5="X",1,0.5),1)</f>
+        <v>0.75</v>
+      </c>
+      <c r="R5" s="5">
+        <f>(IF(( L5="X"),0,($AF$5+I5))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S5" s="8">
+        <f>1*Q5*P5*(1+R5)*D5 + IF(N5="X",D5*P5*0.25,0) + IF(M5="X",D5*P5*Q5*0.5,0)</f>
+        <v>1.8</v>
+      </c>
+      <c r="T5" s="5">
+        <f>S5/$S$4</f>
+        <v>2.1818181818181817</v>
+      </c>
+      <c r="U5" s="10">
+        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]/2</f>
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="V5" s="6"/>
+      <c r="W5" s="5">
+        <f t="shared" ref="W5:W8" si="0">(10+$AF$4-$AI$5)/20</f>
+        <v>0.5</v>
+      </c>
+      <c r="X5" s="5">
+        <f>(C5/20)*IF($AI$13=1,IF(F5="X",1,0.5),1)</f>
+        <v>0.375</v>
+      </c>
+      <c r="Y5" s="5">
+        <f>(IF((OR(K5="X", L5="X")),0,($AF$5+I5))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z5" s="8">
+        <f>IF(G5="X",0,1*X5*W5*(1+Y5)*D5) * IF($AI$13=1,IF(F5="X",1,0.5),1) + IF(N5="X",D5*P5*0.25,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA5" s="5">
+        <f>Z5/$Z$4</f>
+        <v>0</v>
+      </c>
+      <c r="AB5" s="10" t="e">
+        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]/2</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC5" s="5">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>1.0909090909090908</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF5">
+        <v>2</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>99</v>
+      </c>
+      <c r="AI5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="4">
+        <v>16</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="5">
+        <f>(10+$AF$4-$AI$5)/20</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q6" s="5">
+        <f>(C6/20)*IF($AI$6=1,IF(F6="X",1,0.5),1)</f>
+        <v>0.8</v>
+      </c>
+      <c r="R6" s="5">
+        <f>(IF(( L6="X"),0,($AF$5+I6))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S6" s="8">
+        <f t="shared" ref="S6:S8" si="1">1*Q6*P6*(1+R6)*D6 + IF(N6="X",D6*P6*0.25,0) + IF(M6="X",D6*P6*Q6*0.5,0)</f>
+        <v>0.88000000000000012</v>
+      </c>
+      <c r="T6" s="5">
+        <f t="shared" ref="T6:T7" si="2">S6/$S$4</f>
+        <v>1.0666666666666667</v>
+      </c>
+      <c r="U6" s="10">
+        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]/2</f>
+        <v>2.2727272727272725</v>
+      </c>
+      <c r="V6" s="6"/>
+      <c r="W6" s="5">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="X6" s="5">
+        <f>(C6/20)*IF($AI$13=1,IF(F6="X",1,0.5),1)</f>
+        <v>0.8</v>
+      </c>
+      <c r="Y6" s="5">
+        <f>(IF((OR(K6="X", L6="X")),0,($AF$5+I6))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z6" s="8">
+        <f>IF(G6="X",0,1*X6*W6*(1+Y6)*D6) * IF($AI$13=1,IF(F6="X",1,0.5),1) + IF(N6="X",D6*P6*0.25,0)</f>
+        <v>0.88000000000000012</v>
+      </c>
+      <c r="AA6" s="5">
+        <f t="shared" ref="AA6:AA7" si="3">Z6/$Z$4</f>
+        <v>2.1333333333333333</v>
+      </c>
+      <c r="AB6" s="10">
+        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]/2</f>
+        <v>2.2727272727272725</v>
+      </c>
+      <c r="AC6" s="5">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>1.6</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>124</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" s="3">
+        <v>14</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="5">
+        <f>(10+$AF$4-$AI$5)/20</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q7" s="5">
+        <f>(C7/20)*IF($AI$6=1,IF(F7="X",1,0.5),1)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R7" s="5">
+        <f>(IF(( L7="X"),0,($AF$5+I7))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S7" s="8">
+        <f t="shared" si="1"/>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="T7" s="5">
+        <f t="shared" si="2"/>
+        <v>1.3575757575757577</v>
+      </c>
+      <c r="U7" s="10">
+        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]/2</f>
+        <v>1.7857142857142856</v>
+      </c>
+      <c r="V7" s="6"/>
+      <c r="W7" s="5">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="X7" s="5">
+        <f>(C7/20)*IF($AI$13=1,IF(F7="X",1,0.5),1)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Y7" s="5">
+        <f>(IF((OR(K7="X", L7="X")),0,($AF$5+I7))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z7" s="8">
+        <f>IF(G7="X",0,1*X7*W7*(1+Y7)*D7) * IF($AI$13=1,IF(F7="X",1,0.5),1) + IF(N7="X",D7*P7*0.25,0)</f>
+        <v>0.1925</v>
+      </c>
+      <c r="AA7" s="5">
+        <f t="shared" si="3"/>
+        <v>0.46666666666666662</v>
+      </c>
+      <c r="AB7" s="10">
+        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]/2</f>
+        <v>10.38961038961039</v>
+      </c>
+      <c r="AC7" s="5">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>0.91212121212121211</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="3">
+        <v>12</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O8" s="3"/>
+      <c r="P8" s="5">
+        <f>(10+$AF$4-$AI$5)/20</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q8" s="5">
+        <f>(C8/20)*IF($AI$6=1,IF(F8="X",1,0.5),1)</f>
+        <v>0.6</v>
+      </c>
+      <c r="R8" s="5">
+        <f>(IF(( L8="X"),0,($AF$5+I8))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S8" s="8">
+        <f t="shared" si="1"/>
+        <v>0.91</v>
+      </c>
+      <c r="T8" s="5">
+        <f t="shared" ref="T8" si="4">S8/$S$4</f>
+        <v>1.103030303030303</v>
+      </c>
+      <c r="U8" s="10">
+        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]/2</f>
+        <v>2.1978021978021975</v>
+      </c>
+      <c r="V8" s="6"/>
+      <c r="W8" s="5">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="X8" s="5">
+        <f>(C8/20)*IF($AI$13=1,IF(F8="X",1,0.5),1)</f>
+        <v>0.3</v>
+      </c>
+      <c r="Y8" s="5">
+        <f>(IF((OR(K8="X", L8="X")),0,($AF$5+I8))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z8" s="8">
+        <f>IF(G8="X",0,1*X8*W8*(1+Y8)*D8) * IF($AI$13=1,IF(F8="X",1,0.5),1) + IF(N8="X",D8*P8*0.25,0)</f>
+        <v>0.41500000000000004</v>
+      </c>
+      <c r="AA8" s="5">
+        <f t="shared" ref="AA8" si="5">Z8/$Z$4</f>
+        <v>1.0060606060606061</v>
+      </c>
+      <c r="AB8" s="10">
+        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]/2</f>
+        <v>4.8192771084337345</v>
+      </c>
+      <c r="AC8" s="5">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>1.0545454545454547</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
+      <c r="Z9" s="8"/>
+      <c r="AA9" s="5"/>
+      <c r="AB9" s="10"/>
+      <c r="AC9" s="5"/>
+      <c r="AH9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="4">
+        <v>15</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="5">
+        <f>IF(K10="X",1,($AF$3+H10)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q10" s="5">
+        <f>(C10/20)*IF($AI$6=1,IF(F10="X",1,0.5),1)</f>
+        <v>0.75</v>
+      </c>
+      <c r="R10" s="5">
+        <f>(IF(( L10="X"),0,($AF$5+I10))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S10" s="8">
+        <f>((1*Q10*(P10)*D10   +   (IF(J10="X",2,1)*R10*D10)      + IF(N10="X",D10*P10*0.25,0)     ) * IF(M10="X",1.5,1) ) *      IF($AI$6="1",0.5,1)</f>
+        <v>0.95</v>
+      </c>
+      <c r="T10" s="5">
+        <f>S10/$S$10</f>
+        <v>1</v>
+      </c>
+      <c r="U10" s="10">
+        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]/2</f>
+        <v>2.1052631578947367</v>
+      </c>
+      <c r="V10" s="6"/>
+      <c r="W10" s="5">
+        <f t="shared" ref="W10:W24" si="6">IF(K10="X",1,($AF$3+H10)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="X10" s="5">
+        <f>(C10/20)*IF($AI$13=1,IF(F10="X",1,0.5),1)</f>
+        <v>0.375</v>
+      </c>
+      <c r="Y10" s="5">
+        <f>(IF((OR(K10="X", L10="X")),0,($AF$5+I10))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z10" s="8">
+        <f>IF(G10="X",0,((1*Q10*(P10)*D10   +   (IF(J10="X",2,1)*R10*D10)      + IF(N10="X",D10*P10*0.5,0)     ) * IF(M10="X",1.5,1) ) *      IF($AI$13=1,IF(F10="X",1,0.5),1))</f>
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="AA10" s="5">
+        <f>Z10/$Z$10</f>
+        <v>1</v>
+      </c>
+      <c r="AB10" s="24">
+        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]/2</f>
+        <v>4.2105263157894735</v>
+      </c>
+      <c r="AC10" s="23">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>1</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" s="4">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="5">
+        <f>IF(K11="X",1,($AF$3+H11)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q11" s="5">
+        <f>(C11/20)*IF($AI$6=1,IF(F11="X",1,0.5),1)</f>
+        <v>0.4</v>
+      </c>
+      <c r="R11" s="5">
+        <f>(IF(( L11="X"),0,($AF$5+I11))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S11" s="8">
+        <f>((1*Q11*(P11)*D11   +   (IF(J11="X",2,1)*R11*D11)      + IF(N11="X",D11*P11*0.25,0)     ) * IF(M11="X",1.5,1) ) *      IF($AI$6="1",0.5,1)</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="T11" s="5">
+        <f>S11/$S$10</f>
+        <v>0.63157894736842113</v>
+      </c>
+      <c r="U11" s="10">
+        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]/2</f>
+        <v>3.333333333333333</v>
+      </c>
+      <c r="V11" s="6"/>
+      <c r="W11" s="5">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="X11" s="5">
+        <f>(C11/20)*IF($AI$13=1,IF(F11="X",1,0.5),1)</f>
+        <v>0.2</v>
+      </c>
+      <c r="Y11" s="5">
+        <f>(IF((OR(K11="X", L11="X")),0,($AF$5+I11))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z11" s="8">
+        <f>IF(G11="X",0,((1*Q11*(P11)*D11   +   (IF(J11="X",2,1)*R11*D11)      + IF(N11="X",D11*P11*0.5,0)     ) * IF(M11="X",1.5,1) ) *      IF($AI$13=1,IF(F11="X",1,0.5),1))</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="AA11" s="5">
+        <f>Z11/$Z$10</f>
+        <v>0.63157894736842113</v>
+      </c>
+      <c r="AB11" s="24">
+        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]/2</f>
+        <v>6.6666666666666661</v>
+      </c>
+      <c r="AC11" s="23">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>0.63157894736842113</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>98</v>
+      </c>
+      <c r="AI11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="C12" s="4">
+        <v>8</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="5">
+        <f>IF(K12="X",1,($AF$3+H12)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q12" s="5">
+        <f>(C12/20)*IF($AI$6=1,IF(F12="X",1,0.5),1)</f>
+        <v>0.4</v>
+      </c>
+      <c r="R12" s="5">
+        <f>(IF(( L12="X"),0,($AF$5+I12))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S12" s="8">
+        <f>((1*Q12*(P12)*D12   +   (IF(J12="X",2,1)*R12*D12)      + IF(N12="X",D12*P12*0.25,0)     ) * IF(M12="X",1.5,1) ) *      IF($AI$6="1",0.5,1)</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="T12" s="5">
+        <f>S12/$S$10</f>
+        <v>0.63157894736842113</v>
+      </c>
+      <c r="U12" s="10">
+        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]/2</f>
+        <v>3.333333333333333</v>
+      </c>
+      <c r="V12" s="6"/>
+      <c r="W12" s="5">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="X12" s="5">
+        <f>(C12/20)*IF($AI$13=1,IF(F12="X",1,0.5),1)</f>
+        <v>0.4</v>
+      </c>
+      <c r="Y12" s="5">
+        <f>(IF((OR(K12="X", L12="X")),0,($AF$5+I12))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z12" s="8">
+        <f>IF(G12="X",0,((1*Q12*(P12)*D12   +   (IF(J12="X",2,1)*R12*D12)      + IF(N12="X",D12*P12*0.5,0)     ) * IF(M12="X",1.5,1) ) *      IF($AI$13=1,IF(F12="X",1,0.5),1))</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AA12" s="5">
+        <f>Z12/$Z$10</f>
+        <v>1.2631578947368423</v>
+      </c>
+      <c r="AB12" s="24">
+        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]/2</f>
+        <v>3.333333333333333</v>
+      </c>
+      <c r="AC12" s="23">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>0.94736842105263164</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>99</v>
+      </c>
+      <c r="AI12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="8"/>
+      <c r="AA13" s="5"/>
+      <c r="AB13" s="24"/>
+      <c r="AC13" s="23"/>
+      <c r="AH13" t="s">
+        <v>124</v>
+      </c>
+      <c r="AI13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="8"/>
+      <c r="AA14" s="5"/>
+      <c r="AB14" s="24"/>
+      <c r="AC14" s="23"/>
+    </row>
+    <row r="15" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="C15" s="4">
+        <v>8</v>
+      </c>
+      <c r="D15" s="3">
+        <v>3</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O15" s="3"/>
+      <c r="P15" s="5">
+        <f>IF(K15="X",1,($AF$3+H15)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q15" s="5">
+        <f>(C15/20)*IF($AI$6=1,0.5,1)</f>
+        <v>0.4</v>
+      </c>
+      <c r="R15" s="5">
+        <f>(IF(( L15="X"),0,($AF$5+I15))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S15" s="8">
+        <f>((1*Q15*(P15)*D15   +   (IF(J15="X",2,1)*R15*D15)      + IF(N15="X",D15*P15*0.25,0)     ) * IF(M15="X",1.5,1) ) *      IF($AI$6="1",0.5,1)</f>
+        <v>1.2750000000000001</v>
+      </c>
+      <c r="T15" s="5">
+        <f>S15/$S$15</f>
+        <v>1</v>
+      </c>
+      <c r="U15" s="10">
+        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]</f>
+        <v>3.1372549019607838</v>
+      </c>
+      <c r="V15" s="6"/>
+      <c r="W15" s="5">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="X15" s="5">
+        <f>(C15/20)*IF($AI$13=1,IF(F15="X",1,0.5),1)</f>
+        <v>0.2</v>
+      </c>
+      <c r="Y15" s="5">
+        <f>(IF((OR(K15="X", L15="X")),0,($AF$5+I15))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z15" s="8">
+        <f t="shared" ref="Z15:Z24" si="7">IF(G15="X",0,((1*X15*(W15)*D15   +   (IF(J15="X",2,1)*Y15*D15)      + IF(N15="X",D15*W15*0.25,0)     ) * IF(M15="X",1.5,1) ) *      IF($AI$13=1,IF(F15="X",1,0.5),1))</f>
+        <v>0</v>
+      </c>
+      <c r="AA15" s="5" t="e">
+        <f t="shared" ref="AA15:AA23" si="8">Z15/$Z$15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB15" s="24" t="e">
+        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC15" s="23" t="e">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="C16" s="4">
+        <v>8</v>
+      </c>
+      <c r="D16" s="3">
+        <v>2</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="5">
+        <f>IF(K16="X",1,($AF$3+H16)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q16" s="5">
+        <f>(C16/20)*IF($AI$6=1,0.5,1)</f>
+        <v>0.4</v>
+      </c>
+      <c r="R16" s="5">
+        <f>(IF(( L16="X"),0,($AF$5+I16))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S16" s="8">
+        <f>((1*Q16*(P16)*D16   +   (IF(J16="X",2,1)*R16*D16)      + IF(N16="X",D16*P16*0.25,0)     ) * IF(M16="X",1.5,1) ) *      IF($AI$6="1",0.5,1)</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="T16" s="5">
+        <f t="shared" ref="T16:T23" si="9">S16/$S$15</f>
+        <v>0.47058823529411764</v>
+      </c>
+      <c r="U16" s="10">
+        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]</f>
+        <v>6.6666666666666661</v>
+      </c>
+      <c r="V16" s="6"/>
+      <c r="W16" s="5">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="X16" s="5">
+        <f>(C16/20)*IF($AI$13=1,IF(F16="X",1,0.5),1)</f>
+        <v>0.2</v>
+      </c>
+      <c r="Y16" s="5">
+        <f>(IF((OR(K16="X", L16="X")),0,($AF$5+I16))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z16" s="8">
+        <f t="shared" si="7"/>
+        <v>0.2</v>
+      </c>
+      <c r="AA16" s="5" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB16" s="24">
+        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
+        <v>20</v>
+      </c>
+      <c r="AC16" s="23" t="e">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="C17" s="4">
+        <v>14</v>
+      </c>
+      <c r="D17" s="3">
+        <v>2</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="5">
+        <f>IF(K17="X",1,($AF$3+H17)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q17" s="5">
+        <f>(C17/20)*IF($AI$6=1,0.5,1)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R17" s="5">
+        <f>(IF(( L17="X"),0,($AF$5+I17))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S17" s="8">
+        <f>((1*Q17*(P17)*D17   +   (IF(J17="X",2,1)*R17*D17)      + IF(N17="X",D17*P17*0.25,0)     ) * IF(M17="X",1.5,1) ) *      IF($AI$6="1",0.5,1)</f>
+        <v>1.3499999999999999</v>
+      </c>
+      <c r="T17" s="5">
+        <f t="shared" si="9"/>
+        <v>1.0588235294117645</v>
+      </c>
+      <c r="U17" s="10">
+        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]</f>
+        <v>2.9629629629629632</v>
+      </c>
+      <c r="V17" s="6"/>
+      <c r="W17" s="5">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="X17" s="5">
+        <f>(C17/20)*IF($AI$13=1,IF(F17="X",1,0.5),1)</f>
+        <v>0.7</v>
+      </c>
+      <c r="Y17" s="5">
+        <f>(IF((OR(K17="X", L17="X")),0,($AF$5+I17))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z17" s="8">
+        <f t="shared" si="7"/>
+        <v>1.3499999999999999</v>
+      </c>
+      <c r="AA17" s="5" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB17" s="24">
+        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
+        <v>2.9629629629629632</v>
+      </c>
+      <c r="AC17" s="23" t="e">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="5">
+        <f>IF(K18="X",1,($AF$3+H18)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q18" s="5">
+        <f>(C18/20)*IF($AI$6=1,0.5,1)</f>
+        <v>0</v>
+      </c>
+      <c r="R18" s="5">
+        <f>(IF(( L18="X"),0,($AF$5+I18))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S18" s="8">
+        <f>((1*Q18*(P18)*D18   +   (IF(J18="X",2,1)*R18*D18)      + IF(N18="X",D18*P18*0.25,0)     ) * IF(M18="X",1.5,1) ) *      IF($AI$6="1",0.5,1)</f>
+        <v>0</v>
+      </c>
+      <c r="T18" s="5">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U18" s="10" t="e">
+        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V18" s="6"/>
+      <c r="W18" s="5">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="X18" s="5">
+        <f>(C18/20)*IF($AI$13=1,IF(F18="X",1,0.5),1)</f>
+        <v>0</v>
+      </c>
+      <c r="Y18" s="5">
+        <f>(IF((OR(K18="X", L18="X")),0,($AF$5+I18))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z18" s="8">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AA18" s="5" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB18" s="24" t="e">
+        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC18" s="23" t="e">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="5">
+        <f>IF(K19="X",1,($AF$3+H19)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q19" s="5">
+        <f>(C19/20)*IF($AI$6=1,0.5,1)</f>
+        <v>0</v>
+      </c>
+      <c r="R19" s="5">
+        <f>(IF(( L19="X"),0,($AF$5+I19))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S19" s="8">
+        <f>((1*Q19*(P19)*D19   +   (IF(J19="X",2,1)*R19*D19)      + IF(N19="X",D19*P19*0.25,0)     ) * IF(M19="X",1.5,1) ) *      IF($AI$6="1",0.5,1)</f>
+        <v>0</v>
+      </c>
+      <c r="T19" s="5">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U19" s="10" t="e">
+        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V19" s="6"/>
+      <c r="W19" s="5">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="X19" s="5">
+        <f>(C19/20)*IF($AI$13=1,IF(F19="X",1,0.5),1)</f>
+        <v>0</v>
+      </c>
+      <c r="Y19" s="5">
+        <f>(IF((OR(K19="X", L19="X")),0,($AF$5+I19))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z19" s="8">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AA19" s="5" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB19" s="24" t="e">
+        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC19" s="23" t="e">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="5">
+        <f>IF(K20="X",1,($AF$3+H20)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q20" s="5">
+        <f>(C20/20)*IF($AI$6=1,0.5,1)</f>
+        <v>0</v>
+      </c>
+      <c r="R20" s="5">
+        <f>(IF(( L20="X"),0,($AF$5+I20))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S20" s="8">
+        <f>((1*Q20*(P20)*D20   +   (IF(J20="X",2,1)*R20*D20)      + IF(N20="X",D20*P20*0.25,0)     ) * IF(M20="X",1.5,1) ) *      IF($AI$6="1",0.5,1)</f>
+        <v>0</v>
+      </c>
+      <c r="T20" s="5">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U20" s="10" t="e">
+        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V20" s="6"/>
+      <c r="W20" s="5">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="X20" s="5">
+        <f>(C20/20)*IF($AI$13=1,IF(F20="X",1,0.5),1)</f>
+        <v>0</v>
+      </c>
+      <c r="Y20" s="5">
+        <f>(IF((OR(K20="X", L20="X")),0,($AF$5+I20))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z20" s="8">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AA20" s="5" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB20" s="24" t="e">
+        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC20" s="23" t="e">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="5">
+        <f>IF(K21="X",1,($AF$3+H21)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q21" s="5">
+        <f>(C21/20)*IF($AI$6=1,0.5,1)</f>
+        <v>0</v>
+      </c>
+      <c r="R21" s="5">
+        <f>(IF(( L21="X"),0,($AF$5+I21))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S21" s="8">
+        <f>((1*Q21*(P21)*D21   +   (IF(J21="X",2,1)*R21*D21)      + IF(N21="X",D21*P21*0.25,0)     ) * IF(M21="X",1.5,1) ) *      IF($AI$6="1",0.5,1)</f>
+        <v>0</v>
+      </c>
+      <c r="T21" s="5">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U21" s="10" t="e">
+        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V21" s="6"/>
+      <c r="W21" s="5">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="X21" s="5">
+        <f>(C21/20)*IF($AI$13=1,IF(F21="X",1,0.5),1)</f>
+        <v>0</v>
+      </c>
+      <c r="Y21" s="5">
+        <f>(IF((OR(K21="X", L21="X")),0,($AF$5+I21))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z21" s="8">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AA21" s="5" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB21" s="24" t="e">
+        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC21" s="23" t="e">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="5">
+        <f>IF(K22="X",1,($AF$3+H22)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q22" s="5">
+        <f>(C22/20)*IF($AI$6=1,0.5,1)</f>
+        <v>0</v>
+      </c>
+      <c r="R22" s="5">
+        <f>(IF(( L22="X"),0,($AF$5+I22))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S22" s="8">
+        <f>((1*Q22*(P22)*D22   +   (IF(J22="X",2,1)*R22*D22)      + IF(N22="X",D22*P22*0.25,0)     ) * IF(M22="X",1.5,1) ) *      IF($AI$6="1",0.5,1)</f>
+        <v>0</v>
+      </c>
+      <c r="T22" s="5">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U22" s="10" t="e">
+        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V22" s="6"/>
+      <c r="W22" s="5">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="X22" s="5">
+        <f>(C22/20)*IF($AI$13=1,IF(F22="X",1,0.5),1)</f>
+        <v>0</v>
+      </c>
+      <c r="Y22" s="5">
+        <f>(IF((OR(K22="X", L22="X")),0,($AF$5+I22))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z22" s="8">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AA22" s="5" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB22" s="24" t="e">
+        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC22" s="23" t="e">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="5">
+        <f>IF(K23="X",1,($AF$3+H23)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q23" s="5">
+        <f>(C23/20)*IF($AI$6=1,0.5,1)</f>
+        <v>0</v>
+      </c>
+      <c r="R23" s="5">
+        <f>(IF(( L23="X"),0,($AF$5+I23))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S23" s="8">
+        <f>((1*Q23*(P23)*D23   +   (IF(J23="X",2,1)*R23*D23)      + IF(N23="X",D23*P23*0.25,0)     ) * IF(M23="X",1.5,1) ) *      IF($AI$6="1",0.5,1)</f>
+        <v>0</v>
+      </c>
+      <c r="T23" s="5">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U23" s="10" t="e">
+        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V23" s="6"/>
+      <c r="W23" s="5">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="X23" s="5">
+        <f>(C23/20)*IF($AI$13=1,IF(F23="X",1,0.5),1)</f>
+        <v>0</v>
+      </c>
+      <c r="Y23" s="5">
+        <f>(IF((OR(K23="X", L23="X")),0,($AF$5+I23))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z23" s="8">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AA23" s="5" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB23" s="24" t="e">
+        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC23" s="23" t="e">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="5"/>
+      <c r="U24" s="10"/>
+      <c r="V24" s="6"/>
+      <c r="W24" s="5"/>
+      <c r="X24" s="5"/>
+      <c r="Y24" s="5"/>
+      <c r="Z24" s="8"/>
+      <c r="AA24" s="5"/>
+      <c r="AB24" s="24"/>
+      <c r="AC24" s="23"/>
+    </row>
+    <row r="25" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" s="4">
+        <v>12</v>
+      </c>
+      <c r="D25" s="3">
+        <v>3</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O25" s="3"/>
+      <c r="P25" s="5">
+        <f>IF(K25="X",1,($AF$3+H25)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q25" s="5">
+        <f>(C25/20)*IF($AI$6=1,0.5,1)</f>
+        <v>0.6</v>
+      </c>
+      <c r="R25" s="5">
+        <f>(IF(( L25="X"),0,($AF$5+I25))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S25" s="8">
+        <f>((1*Q25*(P25)*D25   +   (IF(J25="X",2,1)*R25*D25)      + IF(N25="X",D25*P25*0.25,0)     ) * IF(M25="X",1.5,1) ) *      IF($AI$6="1",0.5,1)</f>
+        <v>1.575</v>
+      </c>
+      <c r="T25" s="5">
+        <f>S25/$S$25</f>
+        <v>1</v>
+      </c>
+      <c r="U25" s="10">
+        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]</f>
+        <v>2.5396825396825395</v>
+      </c>
+      <c r="V25" s="6"/>
+      <c r="W25" s="5">
+        <f>IF(K25="X",1,($AF$3+H25)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="X25" s="5">
+        <f>(C25/20)*IF($AI$13=1,IF(F25="X",1,0.5),1)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Y25" s="5">
+        <f>(IF((OR(K25="X", L25="X")),0,($AF$5+I25))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z25" s="8">
+        <f>IF(G25="X",0,((1*X25*(W25)*D25   +   (IF(J25="X",2,1)*Y25*D25)      + IF(N25="X",D25*W25*0.25,0)     ) * IF(M25="X",1.5,1) ) *      IF($AI$13=1,IF(F25="X",1,0.5),1))</f>
+        <v>1.575</v>
+      </c>
+      <c r="AA25" s="5">
+        <f>Z25/$Z$25</f>
+        <v>1</v>
+      </c>
+      <c r="AB25" s="24">
+        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
+        <v>2.5396825396825395</v>
+      </c>
+      <c r="AC25" s="23">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="5">
+        <f>IF(K26="X",1,($AF$3+H26)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q26" s="5">
+        <f>(C26/20)*IF($AI$6=1,0.5,1)</f>
+        <v>0</v>
+      </c>
+      <c r="R26" s="5">
+        <f>(IF(( L26="X"),0,($AF$5+I26))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S26" s="8">
+        <f>((1*Q26*(P26)*D26   +   (IF(J26="X",2,1)*R26*D26)      + IF(N26="X",D26*P26*0.25,0)     ) * IF(M26="X",1.5,1) ) *      IF($AI$6="1",0.5,1)</f>
+        <v>0</v>
+      </c>
+      <c r="T26" s="5">
+        <f>S26/$S$25</f>
+        <v>0</v>
+      </c>
+      <c r="U26" s="10" t="e">
+        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V26" s="6"/>
+      <c r="W26" s="5">
+        <f>IF(K26="X",1,($AF$3+IF(F26="X",2,0)+H26)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="X26" s="5">
+        <f>(C26/20)*IF($AI$13=1,IF(F26="X",1,0.5),1)</f>
+        <v>0</v>
+      </c>
+      <c r="Y26" s="5">
+        <f>(IF((OR(K26="X", L26="X")),0,($AF$5+I26))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z26" s="8">
+        <f>IF(G26="X",0,((1*Q26*(P26)*D26   +   (IF(J26="X",2,1)*R26*D26)      + IF(N26="X",D26*P26*0.5,0)     ) * IF(M26="X",1.5,1) ) *      IF($AI$13=1,IF(F26="X",1,0.5),1))</f>
+        <v>0</v>
+      </c>
+      <c r="AA26" s="5">
+        <f>Z26/$Z$25</f>
+        <v>0</v>
+      </c>
+      <c r="AB26" s="24" t="e">
+        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC26" s="23">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="5">
+        <f>IF(K27="X",1,($AF$3+H27)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q27" s="5">
+        <f>(C27/20)*IF($AI$6=1,0.5,1)</f>
+        <v>0</v>
+      </c>
+      <c r="R27" s="5">
+        <f>(IF(( L27="X"),0,($AF$5+I27))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S27" s="8">
+        <f>((1*Q27*(P27)*D27   +   (IF(J27="X",2,1)*R27*D27)      + IF(N27="X",D27*P27*0.25,0)     ) * IF(M27="X",1.5,1) ) *      IF($AI$6="1",0.5,1)</f>
+        <v>0</v>
+      </c>
+      <c r="T27" s="5">
+        <f>S27/$S$25</f>
+        <v>0</v>
+      </c>
+      <c r="U27" s="10" t="e">
+        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V27" s="6"/>
+      <c r="W27" s="5">
+        <f>IF(K27="X",1,($AF$3+IF(F27="X",2,0)+H27)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="X27" s="5">
+        <f>(C27/20)*IF($AI$13=1,IF(F27="X",1,0.5),1)</f>
+        <v>0</v>
+      </c>
+      <c r="Y27" s="5">
+        <f>(IF((OR(K27="X", L27="X")),0,($AF$5+I27))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z27" s="8">
+        <f>IF(G27="X",0,((1*Q27*(P27)*D27   +   (IF(J27="X",2,1)*R27*D27)      + IF(N27="X",D27*P27*0.5,0)     ) * IF(M27="X",1.5,1) ) *      IF($AI$13=1,IF(F27="X",1,0.5),1))</f>
+        <v>0</v>
+      </c>
+      <c r="AA27" s="5">
+        <f>Z27/$Z$25</f>
+        <v>0</v>
+      </c>
+      <c r="AB27" s="24" t="e">
+        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC27" s="23">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="8"/>
+      <c r="T28" s="5"/>
+      <c r="U28" s="10"/>
+      <c r="V28" s="6"/>
+      <c r="W28" s="6"/>
+      <c r="X28" s="5"/>
+      <c r="Y28" s="5"/>
+      <c r="Z28" s="8"/>
+      <c r="AA28" s="5"/>
+      <c r="AB28" s="10"/>
+      <c r="AC28" s="5"/>
+    </row>
+    <row r="29" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="8"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="23"/>
+      <c r="V29" s="6"/>
+      <c r="W29" s="5"/>
+      <c r="X29" s="5"/>
+      <c r="Y29" s="5"/>
+      <c r="Z29" s="8"/>
+      <c r="AA29" s="5"/>
+      <c r="AB29" s="24"/>
+      <c r="AC29" s="23"/>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="5">
+        <f>(10+$AF$4-$AI$5)/20</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q30" s="5">
+        <f>(C30/20)*IF($AI$6=1,IF(F30="X",1,0.5),1)</f>
+        <v>0</v>
+      </c>
+      <c r="R30" s="5">
+        <f>(IF(( L30="X"),0,($AF$5+I30))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S30" s="8">
+        <f>1*Q30*P30*(1+R30)*D30 + IF(N30="X",D30*P30*0.25,0)</f>
+        <v>0</v>
+      </c>
+      <c r="T30" s="5">
+        <f>S30/$S$4</f>
+        <v>0</v>
+      </c>
+      <c r="U30" s="10" t="e">
+        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]/2</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V30" s="6"/>
+      <c r="W30" s="5">
+        <f>(10+$AF$4-$AI$5)/20</f>
+        <v>0.5</v>
+      </c>
+      <c r="X30" s="5">
+        <f>(C30/20)</f>
+        <v>0</v>
+      </c>
+      <c r="Y30" s="5">
+        <f>(IF((OR(K30="X", L30="X")),0,($AF$5+I30))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z30" s="8">
+        <f>IF(G30="X",0,1*X30*W30*(1+Y30)*D30) * IF($AI$13=1,IF(F30="X",1,0.5),1) + IF(N30="X",D30*P30*0.25,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA30" s="5">
+        <f>Z30/$Z$4</f>
+        <v>0</v>
+      </c>
+      <c r="AB30" s="10" t="e">
+        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]/2</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC30" s="5">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="5">
+        <f t="shared" ref="P31:P32" si="10">($AF$3 )/20</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q31" s="5">
+        <f>(C31/20)*IF($AI$6=1,0.5,1)</f>
+        <v>0</v>
+      </c>
+      <c r="R31" s="5">
+        <f>(IF(( L31="X"),0,($AF$5+I31))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S31" s="8">
+        <f>1*Q31*(P31)*(1+R31)*D31</f>
+        <v>0</v>
+      </c>
+      <c r="T31" s="5">
+        <f t="shared" ref="T31:T32" si="11">S31/$S$25</f>
+        <v>0</v>
+      </c>
+      <c r="U31" s="23" t="e">
+        <f>AI36/Table1453[[#This Row],[WoundsÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V31" s="6"/>
+      <c r="W31" s="5">
+        <f t="shared" ref="W31:W32" si="12">($AF$3)/20</f>
+        <v>0.5</v>
+      </c>
+      <c r="X31" s="5">
+        <f>(C31/20)*IF($AI$6=1,IF(F31="X",1,0.5),1)</f>
+        <v>0</v>
+      </c>
+      <c r="Y31" s="5">
+        <f t="shared" ref="Y31:Y32" si="13">($AF$5/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z31" s="8">
+        <f>1*X31*(W31)*(1+Y31)*D31</f>
+        <v>0</v>
+      </c>
+      <c r="AA31" s="5">
+        <f t="shared" ref="AA31:AA32" si="14">Z31/$Z$25</f>
+        <v>0</v>
+      </c>
+      <c r="AB31" s="24" t="e">
+        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC31" s="23">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="5">
+        <f t="shared" si="10"/>
+        <v>0.5</v>
+      </c>
+      <c r="Q32" s="5">
+        <f>(C32/20)*IF($AI$6=1,0.5,1)</f>
+        <v>0</v>
+      </c>
+      <c r="R32" s="5">
+        <f>(IF(( L32="X"),0,($AF$5+I32))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S32" s="8">
+        <f>1*Q32*(P32)*(1+R32)*D32</f>
+        <v>0</v>
+      </c>
+      <c r="T32" s="5">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="U32" s="23" t="e">
+        <f>AI37/Table1453[[#This Row],[WoundsÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V32" s="6"/>
+      <c r="W32" s="5">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="X32" s="5">
+        <f>(C32/20)*IF($AI$6=1,IF(F32="X",1,0.5),1)</f>
+        <v>0</v>
+      </c>
+      <c r="Y32" s="5">
+        <f t="shared" si="13"/>
+        <v>0.1</v>
+      </c>
+      <c r="Z32" s="8">
+        <f>1*X32*(W32)*(1+Y32)*D32</f>
+        <v>0</v>
+      </c>
+      <c r="AA32" s="5">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AB32" s="24" t="e">
+        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC32" s="23">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="8"/>
+      <c r="T33" s="5"/>
+      <c r="U33" s="23"/>
+      <c r="V33" s="6"/>
+      <c r="W33" s="5"/>
+      <c r="X33" s="5"/>
+      <c r="Y33" s="5"/>
+      <c r="Z33" s="8"/>
+      <c r="AA33" s="5"/>
+      <c r="AB33" s="24"/>
+      <c r="AC33" s="23"/>
+      <c r="AD33" s="18"/>
+    </row>
+    <row r="34" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="11"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="5">
+        <f>IF(K34="X",1,($AF$3+H34)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q34" s="5">
+        <f>(C34/20)*IF($AI$6=1,0.5,1)</f>
+        <v>0</v>
+      </c>
+      <c r="R34" s="5">
+        <f>(IF(( L34="X"),0,($AF$5+I34))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S34" s="8">
+        <f>((1*Q34*(P34)*D34   +   (IF(J34="X",2,1)*R34*D34)      + IF(N34="X",D34*P34*0.25,0)     ) * IF(M34="X",1.5,1) ) *      IF($AI$6="1",0.5,1)</f>
+        <v>0</v>
+      </c>
+      <c r="T34" s="5">
+        <f>S34/$S$15</f>
+        <v>0</v>
+      </c>
+      <c r="U34" s="10" t="e">
+        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V34" s="6"/>
+      <c r="W34" s="5">
+        <f>IF(K34="X",1,($AF$3+IF(F34="X",2,0)+H34)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="X34" s="5">
+        <f>(C34/20)*IF($AI$13=1,IF(F34="X",1,0.5),1)</f>
+        <v>0</v>
+      </c>
+      <c r="Y34" s="5">
+        <f>(IF((OR(K34="X", L34="X")),0,($AF$5+I34))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z34" s="8">
+        <f>IF(G34="X",0,((1*Q34*(P34)*D34   +   (IF(J34="X",2,1)*R34*D34)      + IF(N34="X",D34*P34*0.5,0)     ) * IF(M34="X",1.5,1) ) *      IF($AI$13=1,IF(F34="X",1,0.5),1))</f>
+        <v>0</v>
+      </c>
+      <c r="AA34" s="5" t="e">
+        <f t="shared" ref="AA34" si="15">Z34/$Z$15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB34" s="24" t="e">
+        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC34" s="23" t="e">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD34" s="18"/>
+    </row>
+    <row r="35" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="11"/>
+      <c r="P35" s="5">
+        <f t="shared" ref="P35" si="16">($AF$3 )/20</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q35" s="5">
+        <f>(C35/20)*IF($AI$6=1,0.5,1)</f>
+        <v>0</v>
+      </c>
+      <c r="R35" s="5">
+        <f>(IF(( L35="X"),0,($AF$5+I35))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S35" s="8">
+        <f>1*Q35*(P35)*(1+R35)*D35</f>
+        <v>0</v>
+      </c>
+      <c r="T35" s="5">
+        <f t="shared" ref="T35" si="17">S35/$S$25</f>
+        <v>0</v>
+      </c>
+      <c r="U35" s="23" t="e">
+        <f>AI40/Table1453[[#This Row],[WoundsÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V35" s="6"/>
+      <c r="W35" s="5">
+        <f t="shared" ref="W35" si="18">($AF$3)/20</f>
+        <v>0.5</v>
+      </c>
+      <c r="X35" s="5">
+        <f>(C35/20)*IF($AI$6=1,IF(F35="X",1,0.5),1)</f>
+        <v>0</v>
+      </c>
+      <c r="Y35" s="5">
+        <f t="shared" ref="Y35" si="19">($AF$5/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z35" s="8">
+        <f>1*X35*(W35)*(1+Y35)*D35</f>
+        <v>0</v>
+      </c>
+      <c r="AA35" s="5">
+        <f t="shared" ref="AA35" si="20">Z35/$Z$25</f>
+        <v>0</v>
+      </c>
+      <c r="AB35" s="24" t="e">
+        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC35" s="23">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>0</v>
+      </c>
+      <c r="AD35" s="18"/>
+    </row>
+    <row r="36" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="5"/>
+      <c r="Q36" s="5"/>
+      <c r="R36" s="5"/>
+      <c r="S36" s="8"/>
+      <c r="T36" s="5"/>
+      <c r="U36" s="10"/>
+      <c r="V36" s="6"/>
+      <c r="W36" s="5"/>
+      <c r="X36" s="5"/>
+      <c r="Y36" s="5"/>
+      <c r="Z36" s="8"/>
+      <c r="AA36" s="5"/>
+      <c r="AB36" s="24"/>
+      <c r="AC36" s="23"/>
+      <c r="AD36" s="18"/>
+    </row>
+    <row r="37" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="11"/>
+      <c r="P37" s="5"/>
+      <c r="Q37" s="5"/>
+      <c r="R37" s="5"/>
+      <c r="S37" s="8"/>
+      <c r="T37" s="5"/>
+      <c r="U37" s="10"/>
+      <c r="V37" s="6"/>
+      <c r="W37" s="5"/>
+      <c r="X37" s="5"/>
+      <c r="Y37" s="5"/>
+      <c r="Z37" s="8"/>
+      <c r="AA37" s="5"/>
+      <c r="AB37" s="24"/>
+      <c r="AC37" s="23"/>
+      <c r="AD37" s="18"/>
+    </row>
+    <row r="38" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11"/>
+      <c r="M38" s="11"/>
+      <c r="N38" s="11"/>
+      <c r="O38" s="11"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="5"/>
+      <c r="R38" s="5"/>
+      <c r="S38" s="8"/>
+      <c r="T38" s="5"/>
+      <c r="U38" s="10"/>
+      <c r="V38" s="6"/>
+      <c r="W38" s="5"/>
+      <c r="X38" s="5"/>
+      <c r="Y38" s="5"/>
+      <c r="Z38" s="8"/>
+      <c r="AA38" s="5"/>
+      <c r="AB38" s="24"/>
+      <c r="AC38" s="23"/>
+      <c r="AD38" s="18"/>
+    </row>
+    <row r="39" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="11"/>
+      <c r="O39" s="11"/>
+      <c r="P39" s="5"/>
+      <c r="Q39" s="5"/>
+      <c r="R39" s="5"/>
+      <c r="S39" s="8"/>
+      <c r="T39" s="5"/>
+      <c r="U39" s="10"/>
+      <c r="V39" s="6"/>
+      <c r="W39" s="5"/>
+      <c r="X39" s="5"/>
+      <c r="Y39" s="5"/>
+      <c r="Z39" s="8"/>
+      <c r="AA39" s="5"/>
+      <c r="AB39" s="24"/>
+      <c r="AC39" s="23"/>
+    </row>
+    <row r="40" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="11"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+      <c r="P40" s="5"/>
+      <c r="Q40" s="5"/>
+      <c r="R40" s="5"/>
+      <c r="S40" s="8"/>
+      <c r="T40" s="5"/>
+      <c r="U40" s="23"/>
+      <c r="V40" s="6"/>
+      <c r="W40" s="5"/>
+      <c r="X40" s="5"/>
+      <c r="Y40" s="5"/>
+      <c r="Z40" s="8"/>
+      <c r="AA40" s="5"/>
+      <c r="AB40" s="24"/>
+      <c r="AC40" s="23"/>
+    </row>
+    <row r="41" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="11"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="11"/>
+      <c r="M41" s="11"/>
+      <c r="N41" s="11"/>
+      <c r="O41" s="13"/>
+      <c r="P41" s="13"/>
+      <c r="Q41" s="13"/>
+      <c r="R41" s="13"/>
+      <c r="S41" s="13"/>
+      <c r="T41" s="15"/>
+      <c r="U41" s="16"/>
+      <c r="V41" s="13"/>
+      <c r="W41" s="13"/>
+      <c r="X41" s="13"/>
+      <c r="Y41" s="13"/>
+      <c r="Z41" s="13"/>
+      <c r="AA41" s="15"/>
+      <c r="AB41" s="13"/>
+      <c r="AC41" s="18"/>
+    </row>
+    <row r="42" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B42" s="12"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="11"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11"/>
+      <c r="N42" s="11"/>
+      <c r="O42" s="13"/>
+      <c r="P42" s="13"/>
+      <c r="Q42" s="13"/>
+      <c r="R42" s="13"/>
+      <c r="S42" s="13"/>
+      <c r="T42" s="15"/>
+      <c r="U42" s="16"/>
+      <c r="V42" s="13"/>
+      <c r="W42" s="13"/>
+      <c r="X42" s="13"/>
+      <c r="Y42" s="13"/>
+      <c r="Z42" s="13"/>
+      <c r="AA42" s="15"/>
+      <c r="AB42" s="13"/>
+      <c r="AC42" s="18"/>
+    </row>
+    <row r="43" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B43" s="12"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="11"/>
+      <c r="N43" s="11"/>
+      <c r="O43" s="13"/>
+      <c r="P43" s="13"/>
+      <c r="Q43" s="13"/>
+      <c r="R43" s="13"/>
+      <c r="S43" s="13"/>
+      <c r="T43" s="15"/>
+      <c r="U43" s="16"/>
+      <c r="V43" s="13"/>
+      <c r="W43" s="13"/>
+      <c r="X43" s="13"/>
+      <c r="Y43" s="13"/>
+      <c r="Z43" s="13"/>
+      <c r="AA43" s="15"/>
+      <c r="AB43" s="13"/>
+      <c r="AC43" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="W2:Z2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="AA41:AA43 T41:T43 U31:U33 AB31:AB33 AB35:AB39 U35:U39 AB4:AB28 U4:U28">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="2"/>
+        <cfvo type="num" val="8"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z41:Z43 S41:S43 T31:T33 AA31:AA33 AA35:AA39 T35:T39 AA4:AA28 T4:T28">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="2"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB41:AB43 AC31:AC33 AC35:AC39 AC4:AC28">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="num" val="2"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U30 AB30">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="2"/>
+        <cfvo type="num" val="8"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T30 AA30">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="2"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC30">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="num" val="2"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U34 AB34">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="2"/>
+        <cfvo type="num" val="8"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T34 AA34">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="2"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC34">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="num" val="2"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Harlequin Heroes + More
also: Salamanders reworked, added "Terms" to rules and added a Token
list
</commit_message>
<xml_diff>
--- a/Balancing Sheet.xlsx
+++ b/Balancing Sheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Space Marines" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="142">
   <si>
     <t>Name</t>
   </si>
@@ -460,6 +460,12 @@
   <si>
     <t>Stunned</t>
   </si>
+  <si>
+    <t>Shadowblade</t>
+  </si>
+  <si>
+    <t>Hero</t>
+  </si>
 </sst>
 </file>
 
@@ -536,7 +542,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -613,6 +619,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -620,445 +627,6 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="125">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2622,6 +2190,445 @@
       <alignment horizontal="general" vertical="bottom" textRotation="180" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2719,94 +2726,94 @@
     <tableColumn id="2" name="Damage" dataDxfId="121"/>
     <tableColumn id="3" name="Attacks" dataDxfId="120"/>
     <tableColumn id="5" name="Note" dataDxfId="119"/>
-    <tableColumn id="6" name="Penetration" dataDxfId="23"/>
-    <tableColumn id="23" name="Light Weapon    ." dataDxfId="22"/>
-    <tableColumn id="24" name="MM      ." dataDxfId="21"/>
-    <tableColumn id="4" name="Crit       ." dataDxfId="20"/>
-    <tableColumn id="26" name="Weak Spots" dataDxfId="19"/>
-    <tableColumn id="25" name="Cone      ." dataDxfId="18"/>
-    <tableColumn id="29" name="No Crits     ." dataDxfId="17"/>
-    <tableColumn id="32" name="Lethal Wounds    ." dataDxfId="16"/>
-    <tableColumn id="27" name="Lethal Weapon    ." dataDxfId="15"/>
-    <tableColumn id="7" name="Column2" dataDxfId="14" dataCellStyle="Percent"/>
-    <tableColumn id="8" name="Hit%" dataDxfId="13" dataCellStyle="Percent"/>
-    <tableColumn id="9" name="Wound%" dataDxfId="12" dataCellStyle="Percent"/>
-    <tableColumn id="11" name="Crit%" dataDxfId="11" dataCellStyle="Percent"/>
-    <tableColumn id="12" name="WoundsÆ" dataDxfId="10" dataCellStyle="Percent"/>
-    <tableColumn id="20" name="% Base" dataDxfId="9" dataCellStyle="Percent"/>
-    <tableColumn id="13" name="To Kill" dataDxfId="8" dataCellStyle="Comma"/>
-    <tableColumn id="14" name="Column3" dataDxfId="7" dataCellStyle="Percent"/>
-    <tableColumn id="15" name="Hit %" dataDxfId="6" dataCellStyle="Percent"/>
-    <tableColumn id="16" name="Wound %" dataDxfId="5" dataCellStyle="Percent"/>
-    <tableColumn id="18" name="Crit %" dataDxfId="4" dataCellStyle="Percent"/>
-    <tableColumn id="19" name="WoundÆ" dataDxfId="3" dataCellStyle="Percent"/>
-    <tableColumn id="21" name="% Base2" dataDxfId="2" dataCellStyle="Percent"/>
-    <tableColumn id="22" name="To Kill2" dataDxfId="1" dataCellStyle="Percent"/>
-    <tableColumn id="10" name="Combo" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="6" name="Penetration" dataDxfId="118"/>
+    <tableColumn id="23" name="Light Weapon    ." dataDxfId="117"/>
+    <tableColumn id="24" name="MM      ." dataDxfId="116"/>
+    <tableColumn id="4" name="Crit       ." dataDxfId="115"/>
+    <tableColumn id="26" name="Weak Spots" dataDxfId="114"/>
+    <tableColumn id="25" name="Cone      ." dataDxfId="113"/>
+    <tableColumn id="29" name="No Crits     ." dataDxfId="112"/>
+    <tableColumn id="32" name="Lethal Wounds    ." dataDxfId="111"/>
+    <tableColumn id="27" name="Lethal Weapon    ." dataDxfId="110"/>
+    <tableColumn id="7" name="Column2" dataDxfId="109" dataCellStyle="Percent"/>
+    <tableColumn id="8" name="Hit%" dataDxfId="108" dataCellStyle="Percent"/>
+    <tableColumn id="9" name="Wound%" dataDxfId="107" dataCellStyle="Percent"/>
+    <tableColumn id="11" name="Crit%" dataDxfId="106" dataCellStyle="Percent"/>
+    <tableColumn id="12" name="WoundsÆ" dataDxfId="105" dataCellStyle="Percent"/>
+    <tableColumn id="20" name="% Base" dataDxfId="104" dataCellStyle="Percent"/>
+    <tableColumn id="13" name="To Kill" dataDxfId="103" dataCellStyle="Comma"/>
+    <tableColumn id="14" name="Column3" dataDxfId="102" dataCellStyle="Percent"/>
+    <tableColumn id="15" name="Hit %" dataDxfId="101" dataCellStyle="Percent"/>
+    <tableColumn id="16" name="Wound %" dataDxfId="100" dataCellStyle="Percent"/>
+    <tableColumn id="18" name="Crit %" dataDxfId="99" dataCellStyle="Percent"/>
+    <tableColumn id="19" name="WoundÆ" dataDxfId="98" dataCellStyle="Percent"/>
+    <tableColumn id="21" name="% Base2" dataDxfId="97" dataCellStyle="Percent"/>
+    <tableColumn id="22" name="To Kill2" dataDxfId="96" dataCellStyle="Percent"/>
+    <tableColumn id="10" name="Combo" dataDxfId="95" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="B3:AF40" totalsRowShown="0" headerRowDxfId="118" dataDxfId="117" dataCellStyle="Percent">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="B3:AF40" totalsRowShown="0" headerRowDxfId="94" dataDxfId="93" dataCellStyle="Percent">
   <autoFilter ref="B3:AF40"/>
   <tableColumns count="31">
-    <tableColumn id="1" name="Name" dataDxfId="116"/>
-    <tableColumn id="2" name="Damage" dataDxfId="115"/>
-    <tableColumn id="3" name="Attacks" dataDxfId="114"/>
-    <tableColumn id="5" name="Note" dataDxfId="113"/>
-    <tableColumn id="6" name="Penetration" dataDxfId="112"/>
-    <tableColumn id="23" name="MM      ." dataDxfId="111"/>
-    <tableColumn id="24" name="Crit       ." dataDxfId="110"/>
-    <tableColumn id="26" name="Weak Spots" dataDxfId="109"/>
-    <tableColumn id="25" name="Cone      ." dataDxfId="108"/>
-    <tableColumn id="29" name="No Crits     ." dataDxfId="107"/>
-    <tableColumn id="32" name="2H        ." dataDxfId="106"/>
-    <tableColumn id="33" name="Heavy Strikes      ." dataDxfId="105"/>
-    <tableColumn id="4" name="XAmmo       ." dataDxfId="104"/>
-    <tableColumn id="28" name="Lethal Weapon" dataDxfId="103"/>
-    <tableColumn id="27" name="Column2" dataDxfId="102"/>
-    <tableColumn id="7" name="Hit%" dataDxfId="101" dataCellStyle="Percent">
+    <tableColumn id="1" name="Name" dataDxfId="92"/>
+    <tableColumn id="2" name="Damage" dataDxfId="91"/>
+    <tableColumn id="3" name="Attacks" dataDxfId="90"/>
+    <tableColumn id="5" name="Note" dataDxfId="89"/>
+    <tableColumn id="6" name="Penetration" dataDxfId="88"/>
+    <tableColumn id="23" name="MM      ." dataDxfId="87"/>
+    <tableColumn id="24" name="Crit       ." dataDxfId="86"/>
+    <tableColumn id="26" name="Weak Spots" dataDxfId="85"/>
+    <tableColumn id="25" name="Cone      ." dataDxfId="84"/>
+    <tableColumn id="29" name="No Crits     ." dataDxfId="83"/>
+    <tableColumn id="32" name="2H        ." dataDxfId="82"/>
+    <tableColumn id="33" name="Heavy Strikes      ." dataDxfId="81"/>
+    <tableColumn id="4" name="XAmmo       ." dataDxfId="80"/>
+    <tableColumn id="28" name="Lethal Weapon" dataDxfId="79"/>
+    <tableColumn id="27" name="Column2" dataDxfId="78"/>
+    <tableColumn id="7" name="Hit%" dataDxfId="77" dataCellStyle="Percent">
       <calculatedColumnFormula>($AI$3 )/20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Wound%" dataDxfId="100" dataCellStyle="Percent">
+    <tableColumn id="8" name="Wound%" dataDxfId="76" dataCellStyle="Percent">
       <calculatedColumnFormula>(C4/20)*IF($AL$5=1,0.5,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Crit%" dataDxfId="99" dataCellStyle="Percent">
+    <tableColumn id="9" name="Crit%" dataDxfId="75" dataCellStyle="Percent">
       <calculatedColumnFormula>(IF(( K4="X"),0,($AI$5+H4))/20)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Block%" dataDxfId="98" dataCellStyle="Percent"/>
-    <tableColumn id="11" name="WoundsÆ" dataDxfId="97">
+    <tableColumn id="10" name="Block%" dataDxfId="74" dataCellStyle="Percent"/>
+    <tableColumn id="11" name="WoundsÆ" dataDxfId="73">
       <calculatedColumnFormula>1*R4*(Q4)*(1+S4)*D4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="% Base" dataDxfId="96" dataCellStyle="Percent">
+    <tableColumn id="12" name="% Base" dataDxfId="72" dataCellStyle="Percent">
       <calculatedColumnFormula>U4/$U$28</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="To Kill" dataDxfId="95" dataCellStyle="Percent">
+    <tableColumn id="20" name="To Kill" dataDxfId="71" dataCellStyle="Percent">
       <calculatedColumnFormula>AL9/Table14[[#This Row],[WoundsÆ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Column3" dataDxfId="94"/>
-    <tableColumn id="14" name="Hit %" dataDxfId="93" dataCellStyle="Percent">
+    <tableColumn id="13" name="Column3" dataDxfId="70"/>
+    <tableColumn id="14" name="Hit %" dataDxfId="69" dataCellStyle="Percent">
       <calculatedColumnFormula>($AI$3)/20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Wound %" dataDxfId="92" dataCellStyle="Percent">
+    <tableColumn id="15" name="Wound %" dataDxfId="68" dataCellStyle="Percent">
       <calculatedColumnFormula>(C4/20)*IF($AL$5=1,IF(F4="X",1,0.5),1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Crit %" dataDxfId="91" dataCellStyle="Percent">
+    <tableColumn id="16" name="Crit %" dataDxfId="67" dataCellStyle="Percent">
       <calculatedColumnFormula>($AI$5/20)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Block %" dataDxfId="90" dataCellStyle="Percent"/>
-    <tableColumn id="18" name="WoundÆ" dataDxfId="89">
+    <tableColumn id="17" name="Block %" dataDxfId="66" dataCellStyle="Percent"/>
+    <tableColumn id="18" name="WoundÆ" dataDxfId="65">
       <calculatedColumnFormula>1*Z4*(Y4)*(1+AA4)*D4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="% Base2" dataDxfId="88" dataCellStyle="Percent">
+    <tableColumn id="19" name="% Base2" dataDxfId="64" dataCellStyle="Percent">
       <calculatedColumnFormula>AC4/$AC$28</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="To Kill2" dataDxfId="87" dataCellStyle="Percent">
+    <tableColumn id="21" name="To Kill2" dataDxfId="63" dataCellStyle="Percent">
       <calculatedColumnFormula>$AL$9/Table14[[#This Row],[WoundÆ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="Combo" dataDxfId="86" dataCellStyle="Percent">
+    <tableColumn id="22" name="Combo" dataDxfId="62" dataCellStyle="Percent">
       <calculatedColumnFormula>(Table14[[#This Row],[% Base]]+Table14[[#This Row],[% Base2]])/2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2815,63 +2822,63 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="B3:AE35" totalsRowShown="0" headerRowDxfId="85" dataDxfId="84" dataCellStyle="Percent">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="B3:AE35" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60" dataCellStyle="Percent">
   <autoFilter ref="B3:AE35"/>
   <tableColumns count="30">
-    <tableColumn id="1" name="Name" dataDxfId="83"/>
-    <tableColumn id="2" name="Damage" dataDxfId="82"/>
-    <tableColumn id="3" name="Attacks" dataDxfId="81"/>
-    <tableColumn id="5" name="Note" dataDxfId="80"/>
-    <tableColumn id="6" name="Penetration" dataDxfId="79"/>
-    <tableColumn id="30" name="Light Weapon    ." dataDxfId="78"/>
-    <tableColumn id="23" name="MM      ." dataDxfId="77"/>
-    <tableColumn id="24" name="Crit       ." dataDxfId="76"/>
-    <tableColumn id="26" name="Weak Spots" dataDxfId="75"/>
-    <tableColumn id="25" name="Cone      ." dataDxfId="74"/>
-    <tableColumn id="29" name="No Crits     ." dataDxfId="73"/>
-    <tableColumn id="32" name="2H        ." dataDxfId="72"/>
-    <tableColumn id="33" name="Heavy Strikes      ." dataDxfId="71"/>
-    <tableColumn id="4" name="Lethal Wounds    ." dataDxfId="70"/>
-    <tableColumn id="28" name="Lethal Weapon    ." dataDxfId="69"/>
-    <tableColumn id="27" name="Column2" dataDxfId="68"/>
-    <tableColumn id="7" name="Hit%" dataDxfId="67" dataCellStyle="Percent">
+    <tableColumn id="1" name="Name" dataDxfId="59"/>
+    <tableColumn id="2" name="Damage" dataDxfId="58"/>
+    <tableColumn id="3" name="Attacks" dataDxfId="57"/>
+    <tableColumn id="5" name="Note" dataDxfId="56"/>
+    <tableColumn id="6" name="Penetration" dataDxfId="55"/>
+    <tableColumn id="30" name="Light Weapon    ." dataDxfId="54"/>
+    <tableColumn id="23" name="MM      ." dataDxfId="53"/>
+    <tableColumn id="24" name="Crit       ." dataDxfId="52"/>
+    <tableColumn id="26" name="Weak Spots" dataDxfId="51"/>
+    <tableColumn id="25" name="Cone      ." dataDxfId="50"/>
+    <tableColumn id="29" name="No Crits     ." dataDxfId="49"/>
+    <tableColumn id="32" name="2H        ." dataDxfId="48"/>
+    <tableColumn id="33" name="Heavy Strikes      ." dataDxfId="47"/>
+    <tableColumn id="4" name="Lethal Wounds    ." dataDxfId="46"/>
+    <tableColumn id="28" name="Lethal Weapon    ." dataDxfId="45"/>
+    <tableColumn id="27" name="Column2" dataDxfId="44"/>
+    <tableColumn id="7" name="Hit%" dataDxfId="43" dataCellStyle="Percent">
       <calculatedColumnFormula>($AH$3 )/20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Wound%" dataDxfId="66" dataCellStyle="Percent">
+    <tableColumn id="8" name="Wound%" dataDxfId="42" dataCellStyle="Percent">
       <calculatedColumnFormula>(C4/20)*IF($AK$6=1,0.5,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Crit%" dataDxfId="65" dataCellStyle="Percent">
+    <tableColumn id="9" name="Crit%" dataDxfId="41" dataCellStyle="Percent">
       <calculatedColumnFormula>(IF(( L4="X"),0,($AH$5+I4))/20)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="WoundsÆ" dataDxfId="64">
+    <tableColumn id="11" name="WoundsÆ" dataDxfId="40">
       <calculatedColumnFormula>1*S4*(R4)*(1+T4)*D4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="% Base" dataDxfId="63" dataCellStyle="Percent">
+    <tableColumn id="12" name="% Base" dataDxfId="39" dataCellStyle="Percent">
       <calculatedColumnFormula>U4/$U$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="To Kill" dataDxfId="62" dataCellStyle="Percent">
+    <tableColumn id="20" name="To Kill" dataDxfId="38" dataCellStyle="Percent">
       <calculatedColumnFormula>AK9/Table145[[#This Row],[WoundsÆ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Column3" dataDxfId="61"/>
-    <tableColumn id="14" name="Hit %" dataDxfId="60" dataCellStyle="Percent">
+    <tableColumn id="13" name="Column3" dataDxfId="37"/>
+    <tableColumn id="14" name="Hit %" dataDxfId="36" dataCellStyle="Percent">
       <calculatedColumnFormula>($AH$3)/20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Wound %" dataDxfId="59" dataCellStyle="Percent">
+    <tableColumn id="15" name="Wound %" dataDxfId="35" dataCellStyle="Percent">
       <calculatedColumnFormula>(C4/20)*IF($AK$6=1,IF(F4="X",1,0.5),1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Crit %" dataDxfId="58" dataCellStyle="Percent">
+    <tableColumn id="16" name="Crit %" dataDxfId="34" dataCellStyle="Percent">
       <calculatedColumnFormula>($AH$5/20)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="WoundÆ" dataDxfId="57">
+    <tableColumn id="18" name="WoundÆ" dataDxfId="33">
       <calculatedColumnFormula>1*Z4*(Y4)*(1+AA4)*D4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="% Base2" dataDxfId="56" dataCellStyle="Percent">
+    <tableColumn id="19" name="% Base2" dataDxfId="32" dataCellStyle="Percent">
       <calculatedColumnFormula>AB4/$AB$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="To Kill2" dataDxfId="55" dataCellStyle="Percent">
+    <tableColumn id="21" name="To Kill2" dataDxfId="31" dataCellStyle="Percent">
       <calculatedColumnFormula>$AK$9/Table145[[#This Row],[WoundÆ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="Combo" dataDxfId="54" dataCellStyle="Percent">
+    <tableColumn id="22" name="Combo" dataDxfId="30" dataCellStyle="Percent">
       <calculatedColumnFormula>(Table145[[#This Row],[% Base]]+Table145[[#This Row],[% Base2]])/2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2880,61 +2887,61 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table1453" displayName="Table1453" ref="B3:AC35" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52" dataCellStyle="Percent">
-  <autoFilter ref="B3:AC35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table1453" displayName="Table1453" ref="B3:AC36" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" dataCellStyle="Percent">
+  <autoFilter ref="B3:AC36"/>
   <tableColumns count="28">
-    <tableColumn id="1" name="Name" dataDxfId="51"/>
-    <tableColumn id="2" name="Damage" dataDxfId="50"/>
-    <tableColumn id="3" name="Attacks" dataDxfId="49"/>
-    <tableColumn id="5" name="Note" dataDxfId="48"/>
-    <tableColumn id="6" name="Penetration" dataDxfId="47"/>
-    <tableColumn id="30" name="Light Weapon    ." dataDxfId="46"/>
-    <tableColumn id="23" name="MM      ." dataDxfId="45"/>
-    <tableColumn id="24" name="Crit       ." dataDxfId="44"/>
-    <tableColumn id="26" name="Weak Spots" dataDxfId="43"/>
-    <tableColumn id="25" name="Cone      ." dataDxfId="42"/>
-    <tableColumn id="29" name="No Crits     ." dataDxfId="41"/>
-    <tableColumn id="4" name="Lethal Wounds    ." dataDxfId="40"/>
-    <tableColumn id="28" name="Lethal Weapon    ." dataDxfId="39"/>
-    <tableColumn id="27" name="Column2" dataDxfId="38"/>
-    <tableColumn id="7" name="Hit%" dataDxfId="37" dataCellStyle="Percent">
+    <tableColumn id="1" name="Name" dataDxfId="27"/>
+    <tableColumn id="2" name="Damage" dataDxfId="26"/>
+    <tableColumn id="3" name="Attacks" dataDxfId="25"/>
+    <tableColumn id="5" name="Note" dataDxfId="24"/>
+    <tableColumn id="6" name="Penetration" dataDxfId="23"/>
+    <tableColumn id="30" name="Light Weapon    ." dataDxfId="22"/>
+    <tableColumn id="23" name="MM      ." dataDxfId="21"/>
+    <tableColumn id="24" name="Crit       ." dataDxfId="20"/>
+    <tableColumn id="26" name="Weak Spots" dataDxfId="19"/>
+    <tableColumn id="25" name="Cone      ." dataDxfId="18"/>
+    <tableColumn id="29" name="No Crits     ." dataDxfId="17"/>
+    <tableColumn id="4" name="Lethal Wounds    ." dataDxfId="16"/>
+    <tableColumn id="28" name="Lethal Weapon    ." dataDxfId="15"/>
+    <tableColumn id="27" name="Column2" dataDxfId="14"/>
+    <tableColumn id="7" name="Hit%" dataDxfId="13" dataCellStyle="Percent">
       <calculatedColumnFormula>($AF$3 )/20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Wound%" dataDxfId="36" dataCellStyle="Percent">
+    <tableColumn id="8" name="Wound%" dataDxfId="12" dataCellStyle="Percent">
       <calculatedColumnFormula>(C4/20)*IF($AI$6=1,0.5,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Crit%" dataDxfId="35" dataCellStyle="Percent">
+    <tableColumn id="9" name="Crit%" dataDxfId="11" dataCellStyle="Percent">
       <calculatedColumnFormula>(IF(( L4="X"),0,($AF$5+I4))/20)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="WoundsÆ" dataDxfId="34">
+    <tableColumn id="11" name="WoundsÆ" dataDxfId="10">
       <calculatedColumnFormula>1*Q4*(P4)*(1+R4)*D4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="% Base" dataDxfId="33" dataCellStyle="Percent">
-      <calculatedColumnFormula>S4/$S$25</calculatedColumnFormula>
+    <tableColumn id="12" name="% Base" dataDxfId="9" dataCellStyle="Percent">
+      <calculatedColumnFormula>S4/$S$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="To Kill" dataDxfId="32" dataCellStyle="Percent">
-      <calculatedColumnFormula>AI9/Table1453[[#This Row],[WoundsÆ]]</calculatedColumnFormula>
+    <tableColumn id="20" name="To Kill" dataDxfId="8" dataCellStyle="Percent">
+      <calculatedColumnFormula>AI10/Table1453[[#This Row],[WoundsÆ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Column3" dataDxfId="31"/>
-    <tableColumn id="14" name="Hit %" dataDxfId="30" dataCellStyle="Percent">
+    <tableColumn id="13" name="Column3" dataDxfId="7"/>
+    <tableColumn id="14" name="Hit %" dataDxfId="6" dataCellStyle="Percent">
       <calculatedColumnFormula>($AF$3)/20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Wound %" dataDxfId="29" dataCellStyle="Percent">
+    <tableColumn id="15" name="Wound %" dataDxfId="5" dataCellStyle="Percent">
       <calculatedColumnFormula>(C4/20)*IF($AI$6=1,IF(F4="X",1,0.5),1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Crit %" dataDxfId="28" dataCellStyle="Percent">
+    <tableColumn id="16" name="Crit %" dataDxfId="4" dataCellStyle="Percent">
       <calculatedColumnFormula>($AF$5/20)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="WoundÆ" dataDxfId="27">
+    <tableColumn id="18" name="WoundÆ" dataDxfId="3">
       <calculatedColumnFormula>1*X4*(W4)*(1+Y4)*D4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="% Base2" dataDxfId="26" dataCellStyle="Percent">
-      <calculatedColumnFormula>Z4/$Z$25</calculatedColumnFormula>
+    <tableColumn id="19" name="% Base2" dataDxfId="2" dataCellStyle="Percent">
+      <calculatedColumnFormula>Z4/$Z$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="To Kill2" dataDxfId="25" dataCellStyle="Percent">
-      <calculatedColumnFormula>$AI$9/Table1453[[#This Row],[WoundÆ]]</calculatedColumnFormula>
+    <tableColumn id="21" name="To Kill2" dataDxfId="1" dataCellStyle="Percent">
+      <calculatedColumnFormula>$AI$10/Table1453[[#This Row],[WoundÆ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="Combo" dataDxfId="24" dataCellStyle="Percent">
+    <tableColumn id="22" name="Combo" dataDxfId="0" dataCellStyle="Percent">
       <calculatedColumnFormula>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3241,7 +3248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AI66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -4129,7 +4136,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="T13" s="3">
-        <f t="shared" ref="T13:T25" si="19">S13/$S$12</f>
+        <f t="shared" ref="T13:T16" si="19">S13/$S$12</f>
         <v>0.91666666666666663</v>
       </c>
       <c r="U13" s="8">
@@ -5153,7 +5160,7 @@
         <v>1</v>
       </c>
       <c r="U27" s="8">
-        <f t="shared" ref="U5:U35" si="28">$AI$9/S27</f>
+        <f t="shared" ref="U27" si="28">$AI$9/S27</f>
         <v>2.5</v>
       </c>
       <c r="V27" s="4"/>
@@ -12045,7 +12052,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD30 W30">
+  <conditionalFormatting sqref="W30 AD30">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -12057,7 +12064,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC30 V30">
+  <conditionalFormatting sqref="V30 AC30">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -12081,7 +12088,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD34 W34">
+  <conditionalFormatting sqref="W34 AD34">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -12093,7 +12100,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC34 V34">
+  <conditionalFormatting sqref="V34 AC34">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -12127,10 +12134,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AI43"/>
+  <dimension ref="A2:AI44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:AC1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12311,7 +12318,7 @@
         <v>1</v>
       </c>
       <c r="U4" s="8">
-        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]/2</f>
+        <f>$AI$10/Table1453[[#This Row],[WoundsÆ]]/2</f>
         <v>2.4242424242424239</v>
       </c>
       <c r="V4" s="4"/>
@@ -12328,7 +12335,7 @@
         <v>0.1</v>
       </c>
       <c r="Z4" s="6">
-        <f>IF(G4="X",0,1*X4*W4*(1+Y4)*D4) * IF($AI$13=1,IF(F4="X",1,0.5),1) + IF(N4="X",D4*P4*0.25,0)</f>
+        <f>IF(G4="X",0,1*X4*W4*(1+Y4)*D4) * IF($AI$14=1,IF(F4="X",1,0.5),1) + IF(N4="X",D4*P4*0.25,0)</f>
         <v>0.41250000000000003</v>
       </c>
       <c r="AA4" s="3">
@@ -12336,7 +12343,7 @@
         <v>1</v>
       </c>
       <c r="AB4" s="8">
-        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]/2</f>
+        <f>$AI$10/Table1453[[#This Row],[WoundÆ]]/2</f>
         <v>4.8484848484848477</v>
       </c>
       <c r="AC4" s="3">
@@ -12403,16 +12410,16 @@
         <v>2.1818181818181817</v>
       </c>
       <c r="U5" s="8">
-        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]/2</f>
+        <f>$AI$10/Table1453[[#This Row],[WoundsÆ]]/2</f>
         <v>1.1111111111111112</v>
       </c>
       <c r="V5" s="4"/>
       <c r="W5" s="3">
-        <f t="shared" ref="W5:W8" si="0">(10+$AF$4-$AI$5)/20</f>
+        <f t="shared" ref="W5:W9" si="0">(10+$AF$4-$AI$5)/20</f>
         <v>0.5</v>
       </c>
       <c r="X5" s="3">
-        <f>(C5/20)*IF($AI$13=1,IF(F5="X",1,0.5),1)</f>
+        <f>(C5/20)*IF($AI$14=1,IF(F5="X",1,0.5),1)</f>
         <v>0.375</v>
       </c>
       <c r="Y5" s="3">
@@ -12420,7 +12427,7 @@
         <v>0.1</v>
       </c>
       <c r="Z5" s="6">
-        <f>IF(G5="X",0,1*X5*W5*(1+Y5)*D5) * IF($AI$13=1,IF(F5="X",1,0.5),1) + IF(N5="X",D5*P5*0.25,0)</f>
+        <f>IF(G5="X",0,1*X5*W5*(1+Y5)*D5) * IF($AI$14=1,IF(F5="X",1,0.5),1) + IF(N5="X",D5*P5*0.25,0)</f>
         <v>0</v>
       </c>
       <c r="AA5" s="3">
@@ -12428,7 +12435,7 @@
         <v>0</v>
       </c>
       <c r="AB5" s="8" t="e">
-        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]/2</f>
+        <f>$AI$10/Table1453[[#This Row],[WoundÆ]]/2</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AC5" s="3">
@@ -12493,7 +12500,7 @@
         <v>1.0666666666666667</v>
       </c>
       <c r="U6" s="8">
-        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]/2</f>
+        <f>$AI$10/Table1453[[#This Row],[WoundsÆ]]/2</f>
         <v>2.2727272727272725</v>
       </c>
       <c r="V6" s="4"/>
@@ -12502,7 +12509,7 @@
         <v>0.5</v>
       </c>
       <c r="X6" s="3">
-        <f>(C6/20)*IF($AI$13=1,IF(F6="X",1,0.5),1)</f>
+        <f>(C6/20)*IF($AI$14=1,IF(F6="X",1,0.5),1)</f>
         <v>0.8</v>
       </c>
       <c r="Y6" s="3">
@@ -12510,7 +12517,7 @@
         <v>0.1</v>
       </c>
       <c r="Z6" s="6">
-        <f>IF(G6="X",0,1*X6*W6*(1+Y6)*D6) * IF($AI$13=1,IF(F6="X",1,0.5),1) + IF(N6="X",D6*P6*0.25,0)</f>
+        <f>IF(G6="X",0,1*X6*W6*(1+Y6)*D6) * IF($AI$14=1,IF(F6="X",1,0.5),1) + IF(N6="X",D6*P6*0.25,0)</f>
         <v>0.88000000000000012</v>
       </c>
       <c r="AA6" s="3">
@@ -12518,7 +12525,7 @@
         <v>2.1333333333333333</v>
       </c>
       <c r="AB6" s="8">
-        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]/2</f>
+        <f>$AI$10/Table1453[[#This Row],[WoundÆ]]/2</f>
         <v>2.2727272727272725</v>
       </c>
       <c r="AC6" s="3">
@@ -12579,7 +12586,7 @@
         <v>1.3575757575757577</v>
       </c>
       <c r="U7" s="8">
-        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]/2</f>
+        <f>$AI$10/Table1453[[#This Row],[WoundsÆ]]/2</f>
         <v>1.7857142857142856</v>
       </c>
       <c r="V7" s="4"/>
@@ -12588,7 +12595,7 @@
         <v>0.5</v>
       </c>
       <c r="X7" s="3">
-        <f>(C7/20)*IF($AI$13=1,IF(F7="X",1,0.5),1)</f>
+        <f>(C7/20)*IF($AI$14=1,IF(F7="X",1,0.5),1)</f>
         <v>0.35</v>
       </c>
       <c r="Y7" s="3">
@@ -12596,7 +12603,7 @@
         <v>0.1</v>
       </c>
       <c r="Z7" s="6">
-        <f>IF(G7="X",0,1*X7*W7*(1+Y7)*D7) * IF($AI$13=1,IF(F7="X",1,0.5),1) + IF(N7="X",D7*P7*0.25,0)</f>
+        <f>IF(G7="X",0,1*X7*W7*(1+Y7)*D7) * IF($AI$14=1,IF(F7="X",1,0.5),1) + IF(N7="X",D7*P7*0.25,0)</f>
         <v>0.1925</v>
       </c>
       <c r="AA7" s="3">
@@ -12604,7 +12611,7 @@
         <v>0.46666666666666662</v>
       </c>
       <c r="AB7" s="8">
-        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]/2</f>
+        <f>$AI$10/Table1453[[#This Row],[WoundÆ]]/2</f>
         <v>10.38961038961039</v>
       </c>
       <c r="AC7" s="3">
@@ -12657,7 +12664,7 @@
         <v>1.103030303030303</v>
       </c>
       <c r="U8" s="8">
-        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]/2</f>
+        <f>$AI$10/Table1453[[#This Row],[WoundsÆ]]/2</f>
         <v>2.1978021978021975</v>
       </c>
       <c r="V8" s="4"/>
@@ -12666,7 +12673,7 @@
         <v>0.5</v>
       </c>
       <c r="X8" s="3">
-        <f>(C8/20)*IF($AI$13=1,IF(F8="X",1,0.5),1)</f>
+        <f>(C8/20)*IF($AI$14=1,IF(F8="X",1,0.5),1)</f>
         <v>0.3</v>
       </c>
       <c r="Y8" s="3">
@@ -12674,7 +12681,7 @@
         <v>0.1</v>
       </c>
       <c r="Z8" s="6">
-        <f>IF(G8="X",0,1*X8*W8*(1+Y8)*D8) * IF($AI$13=1,IF(F8="X",1,0.5),1) + IF(N8="X",D8*P8*0.25,0)</f>
+        <f>IF(G8="X",0,1*X8*W8*(1+Y8)*D8) * IF($AI$14=1,IF(F8="X",1,0.5),1) + IF(N8="X",D8*P8*0.25,0)</f>
         <v>0.41500000000000004</v>
       </c>
       <c r="AA8" s="3">
@@ -12682,7 +12689,7 @@
         <v>1.0060606060606061</v>
       </c>
       <c r="AB8" s="8">
-        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]/2</f>
+        <f>$AI$10/Table1453[[#This Row],[WoundÆ]]/2</f>
         <v>4.8192771084337345</v>
       </c>
       <c r="AC8" s="3">
@@ -12693,12 +12700,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="B9" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" s="2">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -12706,44 +12721,71 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
+      <c r="M9" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="8"/>
+      <c r="P9" s="3">
+        <f>(10+$AF$4-$AI$5)/20</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q9" s="3">
+        <f>(C9/20)*IF($AI$6=1,IF(F9="X",1,0.5),1)</f>
+        <v>0.6</v>
+      </c>
+      <c r="R9" s="3">
+        <f>(IF(( L9="X"),0,($AF$5+I9))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S9" s="6">
+        <f t="shared" ref="S9" si="6">1*Q9*P9*(1+R9)*D9 + IF(N9="X",D9*P9*0.25,0) + IF(M9="X",D9*P9*Q9*0.5,0)</f>
+        <v>0.96</v>
+      </c>
+      <c r="T9" s="3">
+        <f t="shared" ref="T9" si="7">S9/$S$4</f>
+        <v>1.1636363636363636</v>
+      </c>
+      <c r="U9" s="8">
+        <f>$AI$10/Table1453[[#This Row],[WoundsÆ]]/2</f>
+        <v>2.0833333333333335</v>
+      </c>
       <c r="V9" s="4"/>
-      <c r="W9" s="4"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="6"/>
-      <c r="AA9" s="3"/>
-      <c r="AB9" s="8"/>
-      <c r="AC9" s="3"/>
-      <c r="AH9" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="W9" s="3">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="X9" s="3">
+        <f>(C9/20)*IF($AI$14=1,IF(F9="X",1,0.5),1)</f>
+        <v>0.3</v>
+      </c>
+      <c r="Y9" s="3">
+        <f>(IF((OR(K9="X", L9="X")),0,($AF$5+I9))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z9" s="6">
+        <f>IF(G9="X",0,1*X9*W9*(1+Y9)*D9) * IF($AI$14=1,IF(F9="X",1,0.5),1) + IF(N9="X",D9*P9*0.25,0)</f>
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="AA9" s="3">
+        <f t="shared" ref="AA9" si="8">Z9/$Z$4</f>
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="AB9" s="8">
+        <f>$AI$10/Table1453[[#This Row],[WoundÆ]]/2</f>
+        <v>12.121212121212121</v>
+      </c>
+      <c r="AC9" s="3">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>0.78181818181818175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="C10" s="2">
-        <v>15</v>
-      </c>
-      <c r="D10" s="1">
-        <v>2</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>109</v>
-      </c>
+      <c r="B10" s="22"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -12754,79 +12796,40 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
-      <c r="P10" s="3">
-        <f>IF(K10="X",1,($AF$3+H10)/20)</f>
-        <v>0.5</v>
-      </c>
-      <c r="Q10" s="3">
-        <f>(C10/20)*IF($AI$6=1,IF(F10="X",1,0.5),1)</f>
-        <v>0.75</v>
-      </c>
-      <c r="R10" s="3">
-        <f>(IF(( L10="X"),0,($AF$5+I10))/20)</f>
-        <v>0.1</v>
-      </c>
-      <c r="S10" s="6">
-        <f>((1*Q10*(P10)*D10   +   (IF(J10="X",2,1)*R10*D10)      + IF(N10="X",D10*P10*0.25,0)     ) * IF(M10="X",1.5,1) ) *      IF($AI$6="1",0.5,1)</f>
-        <v>0.95</v>
-      </c>
-      <c r="T10" s="3">
-        <f>S10/$S$10</f>
-        <v>1</v>
-      </c>
-      <c r="U10" s="8">
-        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]/2</f>
-        <v>2.1052631578947367</v>
-      </c>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="8"/>
       <c r="V10" s="4"/>
-      <c r="W10" s="3">
-        <f t="shared" ref="W10:W23" si="6">IF(K10="X",1,($AF$3+H10)/20)</f>
-        <v>0.5</v>
-      </c>
-      <c r="X10" s="3">
-        <f>(C10/20)*IF($AI$13=1,IF(F10="X",1,0.5),1)</f>
-        <v>0.375</v>
-      </c>
-      <c r="Y10" s="3">
-        <f>(IF((OR(K10="X", L10="X")),0,($AF$5+I10))/20)</f>
-        <v>0.1</v>
-      </c>
-      <c r="Z10" s="6">
-        <f>IF(G10="X",0,((1*Q10*(P10)*D10   +   (IF(J10="X",2,1)*R10*D10)      + IF(N10="X",D10*P10*0.5,0)     ) * IF(M10="X",1.5,1) ) *      IF($AI$13=1,IF(F10="X",1,0.5),1))</f>
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="AA10" s="3">
-        <f>Z10/$Z$10</f>
-        <v>1</v>
-      </c>
-      <c r="AB10" s="20">
-        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]/2</f>
-        <v>4.2105263157894735</v>
-      </c>
-      <c r="AC10" s="19">
-        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
-        <v>1</v>
-      </c>
+      <c r="W10" s="4"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="8"/>
+      <c r="AC10" s="3"/>
       <c r="AH10" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="AI10">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="22" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="C11" s="2">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D11" s="1">
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>138</v>
+        <v>109</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -12844,7 +12847,7 @@
       </c>
       <c r="Q11" s="3">
         <f>(C11/20)*IF($AI$6=1,IF(F11="X",1,0.5),1)</f>
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="R11" s="3">
         <f>(IF(( L11="X"),0,($AF$5+I11))/20)</f>
@@ -12852,47 +12855,47 @@
       </c>
       <c r="S11" s="6">
         <f>((1*Q11*(P11)*D11   +   (IF(J11="X",2,1)*R11*D11)      + IF(N11="X",D11*P11*0.25,0)     ) * IF(M11="X",1.5,1) ) *      IF($AI$6="1",0.5,1)</f>
-        <v>0.60000000000000009</v>
+        <v>0.95</v>
       </c>
       <c r="T11" s="3">
-        <f>S11/$S$10</f>
-        <v>0.63157894736842113</v>
+        <f>S11/$S$11</f>
+        <v>1</v>
       </c>
       <c r="U11" s="8">
-        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]/2</f>
-        <v>3.333333333333333</v>
+        <f>$AI$10/Table1453[[#This Row],[WoundsÆ]]/2</f>
+        <v>2.1052631578947367</v>
       </c>
       <c r="V11" s="4"/>
       <c r="W11" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="W11:W24" si="9">IF(K11="X",1,($AF$3+H11)/20)</f>
         <v>0.5</v>
       </c>
       <c r="X11" s="3">
-        <f>(C11/20)*IF($AI$13=1,IF(F11="X",1,0.5),1)</f>
-        <v>0.2</v>
+        <f>(C11/20)*IF($AI$14=1,IF(F11="X",1,0.5),1)</f>
+        <v>0.375</v>
       </c>
       <c r="Y11" s="3">
         <f>(IF((OR(K11="X", L11="X")),0,($AF$5+I11))/20)</f>
         <v>0.1</v>
       </c>
       <c r="Z11" s="6">
-        <f>IF(G11="X",0,((1*Q11*(P11)*D11   +   (IF(J11="X",2,1)*R11*D11)      + IF(N11="X",D11*P11*0.5,0)     ) * IF(M11="X",1.5,1) ) *      IF($AI$13=1,IF(F11="X",1,0.5),1))</f>
-        <v>0.30000000000000004</v>
+        <f>IF(G11="X",0,((1*Q11*(P11)*D11   +   (IF(J11="X",2,1)*R11*D11)      + IF(N11="X",D11*P11*0.5,0)     ) * IF(M11="X",1.5,1) ) *      IF($AI$14=1,IF(F11="X",1,0.5),1))</f>
+        <v>0.47499999999999998</v>
       </c>
       <c r="AA11" s="3">
-        <f>Z11/$Z$10</f>
-        <v>0.63157894736842113</v>
+        <f>Z11/$Z$11</f>
+        <v>1</v>
       </c>
       <c r="AB11" s="20">
-        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]/2</f>
-        <v>6.6666666666666661</v>
+        <f>$AI$10/Table1453[[#This Row],[WoundÆ]]/2</f>
+        <v>4.2105263157894735</v>
       </c>
       <c r="AC11" s="19">
         <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
-        <v>0.63157894736842113</v>
+        <v>1</v>
       </c>
       <c r="AH11" t="s">
-        <v>98</v>
+        <v>10</v>
       </c>
       <c r="AI11">
         <v>10</v>
@@ -12901,7 +12904,7 @@
     <row r="12" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C12" s="2">
         <v>8</v>
@@ -12910,11 +12913,9 @@
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -12941,44 +12942,44 @@
         <v>0.60000000000000009</v>
       </c>
       <c r="T12" s="3">
-        <f>S12/$S$10</f>
+        <f>S12/$S$11</f>
         <v>0.63157894736842113</v>
       </c>
       <c r="U12" s="8">
-        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]/2</f>
+        <f>$AI$10/Table1453[[#This Row],[WoundsÆ]]/2</f>
         <v>3.333333333333333</v>
       </c>
       <c r="V12" s="4"/>
       <c r="W12" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="X12" s="3">
-        <f>(C12/20)*IF($AI$13=1,IF(F12="X",1,0.5),1)</f>
-        <v>0.4</v>
+        <f>(C12/20)*IF($AI$14=1,IF(F12="X",1,0.5),1)</f>
+        <v>0.2</v>
       </c>
       <c r="Y12" s="3">
         <f>(IF((OR(K12="X", L12="X")),0,($AF$5+I12))/20)</f>
         <v>0.1</v>
       </c>
       <c r="Z12" s="6">
-        <f>IF(G12="X",0,((1*Q12*(P12)*D12   +   (IF(J12="X",2,1)*R12*D12)      + IF(N12="X",D12*P12*0.5,0)     ) * IF(M12="X",1.5,1) ) *      IF($AI$13=1,IF(F12="X",1,0.5),1))</f>
-        <v>0.60000000000000009</v>
+        <f>IF(G12="X",0,((1*Q12*(P12)*D12   +   (IF(J12="X",2,1)*R12*D12)      + IF(N12="X",D12*P12*0.5,0)     ) * IF(M12="X",1.5,1) ) *      IF($AI$14=1,IF(F12="X",1,0.5),1))</f>
+        <v>0.30000000000000004</v>
       </c>
       <c r="AA12" s="3">
-        <f>Z12/$Z$10</f>
-        <v>1.2631578947368423</v>
+        <f>Z12/$Z$11</f>
+        <v>0.63157894736842113</v>
       </c>
       <c r="AB12" s="20">
-        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]/2</f>
-        <v>3.333333333333333</v>
+        <f>$AI$10/Table1453[[#This Row],[WoundÆ]]/2</f>
+        <v>6.6666666666666661</v>
       </c>
       <c r="AC12" s="19">
         <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
-        <v>0.94736842105263164</v>
+        <v>0.63157894736842113</v>
       </c>
       <c r="AH12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AI12">
         <v>10</v>
@@ -12986,11 +12987,21 @@
     </row>
     <row r="13" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="B13" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="2">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -13000,25 +13011,64 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="8"/>
+      <c r="P13" s="3">
+        <f>IF(K13="X",1,($AF$3+H13)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q13" s="3">
+        <f>(C13/20)*IF($AI$6=1,IF(F13="X",1,0.5),1)</f>
+        <v>0.4</v>
+      </c>
+      <c r="R13" s="3">
+        <f>(IF(( L13="X"),0,($AF$5+I13))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S13" s="6">
+        <f>((1*Q13*(P13)*D13   +   (IF(J13="X",2,1)*R13*D13)      + IF(N13="X",D13*P13*0.25,0)     ) * IF(M13="X",1.5,1) ) *      IF($AI$6="1",0.5,1)</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="T13" s="3">
+        <f>S13/$S$11</f>
+        <v>0.63157894736842113</v>
+      </c>
+      <c r="U13" s="8">
+        <f>$AI$10/Table1453[[#This Row],[WoundsÆ]]/2</f>
+        <v>3.333333333333333</v>
+      </c>
       <c r="V13" s="4"/>
-      <c r="W13" s="3"/>
-      <c r="X13" s="3"/>
-      <c r="Y13" s="3"/>
-      <c r="Z13" s="6"/>
-      <c r="AA13" s="3"/>
-      <c r="AB13" s="20"/>
-      <c r="AC13" s="19"/>
+      <c r="W13" s="3">
+        <f t="shared" si="9"/>
+        <v>0.5</v>
+      </c>
+      <c r="X13" s="3">
+        <f>(C13/20)*IF($AI$14=1,IF(F13="X",1,0.5),1)</f>
+        <v>0.4</v>
+      </c>
+      <c r="Y13" s="3">
+        <f>(IF((OR(K13="X", L13="X")),0,($AF$5+I13))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z13" s="6">
+        <f>IF(G13="X",0,((1*Q13*(P13)*D13   +   (IF(J13="X",2,1)*R13*D13)      + IF(N13="X",D13*P13*0.5,0)     ) * IF(M13="X",1.5,1) ) *      IF($AI$14=1,IF(F13="X",1,0.5),1))</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AA13" s="3">
+        <f>Z13/$Z$11</f>
+        <v>1.2631578947368423</v>
+      </c>
+      <c r="AB13" s="20">
+        <f>$AI$10/Table1453[[#This Row],[WoundÆ]]/2</f>
+        <v>3.333333333333333</v>
+      </c>
+      <c r="AC13" s="19">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>0.94736842105263164</v>
+      </c>
       <c r="AH13" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="AI13">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
@@ -13051,159 +13101,118 @@
       <c r="AA14" s="3"/>
       <c r="AB14" s="20"/>
       <c r="AC14" s="19"/>
+      <c r="AH14" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="C15" s="2">
-        <v>8</v>
-      </c>
-      <c r="D15" s="1">
-        <v>3</v>
-      </c>
+      <c r="B15" s="22"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-      <c r="N15" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="3">
-        <f t="shared" ref="P15:P23" si="7">IF(K15="X",1,($AF$3+H15)/20)</f>
-        <v>0.5</v>
-      </c>
-      <c r="Q15" s="3">
-        <f t="shared" ref="Q15:Q23" si="8">(C15/20)*IF($AI$6=1,0.5,1)</f>
-        <v>0.4</v>
-      </c>
-      <c r="R15" s="3">
-        <f t="shared" ref="R15:R23" si="9">(IF(( L15="X"),0,($AF$5+I15))/20)</f>
-        <v>0.1</v>
-      </c>
-      <c r="S15" s="6">
-        <f t="shared" ref="S15:S23" si="10">((1*Q15*(P15)*D15   +   (IF(J15="X",2,1)*R15*D15)      + IF(N15="X",D15*P15*0.25,0)     ) * IF(M15="X",1.5,1) ) *      IF($AI$6="1",0.5,1)</f>
-        <v>1.2750000000000001</v>
-      </c>
-      <c r="T15" s="3">
-        <f>S15/$S$15</f>
-        <v>1</v>
-      </c>
-      <c r="U15" s="8">
-        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]</f>
-        <v>3.1372549019607838</v>
-      </c>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="8"/>
       <c r="V15" s="4"/>
-      <c r="W15" s="3">
-        <f t="shared" si="6"/>
-        <v>0.5</v>
-      </c>
-      <c r="X15" s="3">
-        <f t="shared" ref="X15:X23" si="11">(C15/20)*IF($AI$13=1,IF(F15="X",1,0.5),1)</f>
-        <v>0.2</v>
-      </c>
-      <c r="Y15" s="3">
-        <f t="shared" ref="Y15:Y23" si="12">(IF((OR(K15="X", L15="X")),0,($AF$5+I15))/20)</f>
-        <v>0.1</v>
-      </c>
-      <c r="Z15" s="6">
-        <f t="shared" ref="Z15:Z23" si="13">IF(G15="X",0,((1*X15*(W15)*D15   +   (IF(J15="X",2,1)*Y15*D15)      + IF(N15="X",D15*W15*0.25,0)     ) * IF(M15="X",1.5,1) ) *      IF($AI$13=1,IF(F15="X",1,0.5),1))</f>
-        <v>0</v>
-      </c>
-      <c r="AA15" s="3" t="e">
-        <f t="shared" ref="AA15:AA23" si="14">Z15/$Z$15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AB15" s="20" t="e">
-        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC15" s="19" t="e">
-        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="W15" s="3"/>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="3"/>
+      <c r="AB15" s="20"/>
+      <c r="AC15" s="19"/>
     </row>
     <row r="16" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C16" s="2">
         <v>8</v>
       </c>
       <c r="D16" s="1">
-        <v>2</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>139</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="G16" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
+      <c r="N16" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="O16" s="1"/>
       <c r="P16" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="P16:P24" si="10">IF(K16="X",1,($AF$3+H16)/20)</f>
         <v>0.5</v>
       </c>
       <c r="Q16" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="Q16:Q24" si="11">(C16/20)*IF($AI$6=1,0.5,1)</f>
         <v>0.4</v>
       </c>
       <c r="R16" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="R16:R24" si="12">(IF(( L16="X"),0,($AF$5+I16))/20)</f>
         <v>0.1</v>
       </c>
       <c r="S16" s="6">
-        <f t="shared" si="10"/>
-        <v>0.60000000000000009</v>
+        <f t="shared" ref="S16:S24" si="13">((1*Q16*(P16)*D16   +   (IF(J16="X",2,1)*R16*D16)      + IF(N16="X",D16*P16*0.25,0)     ) * IF(M16="X",1.5,1) ) *      IF($AI$6="1",0.5,1)</f>
+        <v>1.2750000000000001</v>
       </c>
       <c r="T16" s="3">
-        <f t="shared" ref="T16:T23" si="15">S16/$S$15</f>
-        <v>0.47058823529411764</v>
+        <f>S16/$S$16</f>
+        <v>1</v>
       </c>
       <c r="U16" s="8">
-        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]</f>
-        <v>6.6666666666666661</v>
+        <f>$AI$10/Table1453[[#This Row],[WoundsÆ]]</f>
+        <v>3.1372549019607838</v>
       </c>
       <c r="V16" s="4"/>
       <c r="W16" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="X16" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="X16:X24" si="14">(C16/20)*IF($AI$14=1,IF(F16="X",1,0.5),1)</f>
         <v>0.2</v>
       </c>
       <c r="Y16" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="Y16:Y24" si="15">(IF((OR(K16="X", L16="X")),0,($AF$5+I16))/20)</f>
         <v>0.1</v>
       </c>
       <c r="Z16" s="6">
-        <f t="shared" si="13"/>
-        <v>0.2</v>
+        <f t="shared" ref="Z16:Z24" si="16">IF(G16="X",0,((1*X16*(W16)*D16   +   (IF(J16="X",2,1)*Y16*D16)      + IF(N16="X",D16*W16*0.25,0)     ) * IF(M16="X",1.5,1) ) *      IF($AI$14=1,IF(F16="X",1,0.5),1))</f>
+        <v>0</v>
       </c>
       <c r="AA16" s="3" t="e">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="AA16:AA24" si="17">Z16/$Z$16</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AB16" s="20">
-        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
-        <v>20</v>
+      <c r="AB16" s="20" t="e">
+        <f>$AI$10/Table1453[[#This Row],[WoundÆ]]</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="AC16" s="19" t="e">
         <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
@@ -13213,77 +13222,75 @@
     <row r="17" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C17" s="2">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D17" s="1">
         <v>2</v>
       </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="E17" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.5</v>
       </c>
       <c r="Q17" s="3">
-        <f t="shared" si="8"/>
-        <v>0.7</v>
+        <f t="shared" si="11"/>
+        <v>0.4</v>
       </c>
       <c r="R17" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.1</v>
       </c>
       <c r="S17" s="6">
-        <f t="shared" si="10"/>
-        <v>1.3499999999999999</v>
+        <f t="shared" si="13"/>
+        <v>0.60000000000000009</v>
       </c>
       <c r="T17" s="3">
-        <f t="shared" si="15"/>
-        <v>1.0588235294117645</v>
+        <f t="shared" ref="T17:T24" si="18">S17/$S$16</f>
+        <v>0.47058823529411764</v>
       </c>
       <c r="U17" s="8">
-        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]</f>
-        <v>2.9629629629629632</v>
+        <f>$AI$10/Table1453[[#This Row],[WoundsÆ]]</f>
+        <v>6.6666666666666661</v>
       </c>
       <c r="V17" s="4"/>
       <c r="W17" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="X17" s="3">
-        <f t="shared" si="11"/>
-        <v>0.7</v>
+        <f t="shared" si="14"/>
+        <v>0.2</v>
       </c>
       <c r="Y17" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.1</v>
       </c>
       <c r="Z17" s="6">
-        <f t="shared" si="13"/>
-        <v>1.3499999999999999</v>
+        <f t="shared" si="16"/>
+        <v>0.2</v>
       </c>
       <c r="AA17" s="3" t="e">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB17" s="20">
-        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
-        <v>2.9629629629629632</v>
+        <f>$AI$10/Table1453[[#This Row],[WoundÆ]]</f>
+        <v>20</v>
       </c>
       <c r="AC17" s="19" t="e">
         <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
@@ -13292,68 +13299,78 @@
     </row>
     <row r="18" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="1"/>
+      <c r="B18" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" s="2">
+        <v>14</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2</v>
+      </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
+      <c r="M18" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.5</v>
       </c>
       <c r="Q18" s="3">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>0.7</v>
       </c>
       <c r="R18" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.1</v>
       </c>
       <c r="S18" s="6">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>1.3499999999999999</v>
       </c>
       <c r="T18" s="3">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="U18" s="8" t="e">
-        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="18"/>
+        <v>1.0588235294117645</v>
+      </c>
+      <c r="U18" s="8">
+        <f>$AI$10/Table1453[[#This Row],[WoundsÆ]]</f>
+        <v>2.9629629629629632</v>
       </c>
       <c r="V18" s="4"/>
       <c r="W18" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="X18" s="3">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>0.7</v>
       </c>
       <c r="Y18" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.1</v>
       </c>
       <c r="Z18" s="6">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="16"/>
+        <v>1.3499999999999999</v>
       </c>
       <c r="AA18" s="3" t="e">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AB18" s="20" t="e">
-        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
-        <v>#DIV/0!</v>
+      <c r="AB18" s="20">
+        <f>$AI$10/Table1453[[#This Row],[WoundÆ]]</f>
+        <v>2.9629629629629632</v>
       </c>
       <c r="AC18" s="19" t="e">
         <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
@@ -13377,52 +13394,52 @@
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.5</v>
       </c>
       <c r="Q19" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="R19" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.1</v>
       </c>
       <c r="S19" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="T19" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="U19" s="8" t="e">
-        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]</f>
+        <f>$AI$10/Table1453[[#This Row],[WoundsÆ]]</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V19" s="4"/>
       <c r="W19" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="X19" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Y19" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.1</v>
       </c>
       <c r="Z19" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AA19" s="3" t="e">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB19" s="20" t="e">
-        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
+        <f>$AI$10/Table1453[[#This Row],[WoundÆ]]</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AC19" s="19" t="e">
@@ -13447,52 +13464,52 @@
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.5</v>
       </c>
       <c r="Q20" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="R20" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.1</v>
       </c>
       <c r="S20" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="T20" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="U20" s="8" t="e">
-        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]</f>
+        <f>$AI$10/Table1453[[#This Row],[WoundsÆ]]</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V20" s="4"/>
       <c r="W20" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="X20" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Y20" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.1</v>
       </c>
       <c r="Z20" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AA20" s="3" t="e">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB20" s="20" t="e">
-        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
+        <f>$AI$10/Table1453[[#This Row],[WoundÆ]]</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AC20" s="19" t="e">
@@ -13517,52 +13534,52 @@
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.5</v>
       </c>
       <c r="Q21" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="R21" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.1</v>
       </c>
       <c r="S21" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="T21" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="U21" s="8" t="e">
-        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]</f>
+        <f>$AI$10/Table1453[[#This Row],[WoundsÆ]]</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V21" s="4"/>
       <c r="W21" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="X21" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Y21" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.1</v>
       </c>
       <c r="Z21" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AA21" s="3" t="e">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB21" s="20" t="e">
-        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
+        <f>$AI$10/Table1453[[#This Row],[WoundÆ]]</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AC21" s="19" t="e">
@@ -13587,52 +13604,52 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.5</v>
       </c>
       <c r="Q22" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="R22" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.1</v>
       </c>
       <c r="S22" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="T22" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="U22" s="8" t="e">
-        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]</f>
+        <f>$AI$10/Table1453[[#This Row],[WoundsÆ]]</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V22" s="4"/>
       <c r="W22" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="X22" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Y22" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.1</v>
       </c>
       <c r="Z22" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AA22" s="3" t="e">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB22" s="20" t="e">
-        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
+        <f>$AI$10/Table1453[[#This Row],[WoundÆ]]</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AC22" s="19" t="e">
@@ -13657,52 +13674,52 @@
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.5</v>
       </c>
       <c r="Q23" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="R23" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.1</v>
       </c>
       <c r="S23" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="T23" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="U23" s="8" t="e">
-        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]</f>
+        <f>$AI$10/Table1453[[#This Row],[WoundsÆ]]</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V23" s="4"/>
       <c r="W23" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="X23" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Y23" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.1</v>
       </c>
       <c r="Z23" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AA23" s="3" t="e">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB23" s="20" t="e">
-        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
+        <f>$AI$10/Table1453[[#This Row],[WoundÆ]]</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AC23" s="19" t="e">
@@ -13726,36 +13743,67 @@
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
-      <c r="S24" s="6"/>
-      <c r="T24" s="3"/>
-      <c r="U24" s="8"/>
+      <c r="P24" s="3">
+        <f t="shared" si="10"/>
+        <v>0.5</v>
+      </c>
+      <c r="Q24" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="R24" s="3">
+        <f t="shared" si="12"/>
+        <v>0.1</v>
+      </c>
+      <c r="S24" s="6">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="T24" s="3">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="U24" s="8" t="e">
+        <f>$AI$10/Table1453[[#This Row],[WoundsÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="V24" s="4"/>
-      <c r="W24" s="3"/>
-      <c r="X24" s="3"/>
-      <c r="Y24" s="3"/>
-      <c r="Z24" s="6"/>
-      <c r="AA24" s="3"/>
-      <c r="AB24" s="20"/>
-      <c r="AC24" s="19"/>
+      <c r="W24" s="3">
+        <f t="shared" si="9"/>
+        <v>0.5</v>
+      </c>
+      <c r="X24" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="Y24" s="3">
+        <f t="shared" si="15"/>
+        <v>0.1</v>
+      </c>
+      <c r="Z24" s="6">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AA24" s="3" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB24" s="20" t="e">
+        <f>$AI$10/Table1453[[#This Row],[WoundÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC24" s="19" t="e">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="25" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="C25" s="2">
-        <v>12</v>
-      </c>
-      <c r="D25" s="1">
-        <v>3</v>
-      </c>
+      <c r="B25" s="22"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -13763,71 +13811,38 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
-      <c r="N25" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="N25" s="1"/>
       <c r="O25" s="1"/>
-      <c r="P25" s="3">
-        <f>IF(K25="X",1,($AF$3+H25)/20)</f>
-        <v>0.5</v>
-      </c>
-      <c r="Q25" s="3">
-        <f>(C25/20)*IF($AI$6=1,0.5,1)</f>
-        <v>0.6</v>
-      </c>
-      <c r="R25" s="3">
-        <f>(IF(( L25="X"),0,($AF$5+I25))/20)</f>
-        <v>0.1</v>
-      </c>
-      <c r="S25" s="6">
-        <f>((1*Q25*(P25)*D25   +   (IF(J25="X",2,1)*R25*D25)      + IF(N25="X",D25*P25*0.25,0)     ) * IF(M25="X",1.5,1) ) *      IF($AI$6="1",0.5,1)</f>
-        <v>1.575</v>
-      </c>
-      <c r="T25" s="3">
-        <f>S25/$S$25</f>
-        <v>1</v>
-      </c>
-      <c r="U25" s="8">
-        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]</f>
-        <v>2.5396825396825395</v>
-      </c>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="8"/>
       <c r="V25" s="4"/>
-      <c r="W25" s="3">
-        <f>IF(K25="X",1,($AF$3+H25)/20)</f>
-        <v>0.5</v>
-      </c>
-      <c r="X25" s="3">
-        <f>(C25/20)*IF($AI$13=1,IF(F25="X",1,0.5),1)</f>
-        <v>0.6</v>
-      </c>
-      <c r="Y25" s="3">
-        <f>(IF((OR(K25="X", L25="X")),0,($AF$5+I25))/20)</f>
-        <v>0.1</v>
-      </c>
-      <c r="Z25" s="6">
-        <f>IF(G25="X",0,((1*X25*(W25)*D25   +   (IF(J25="X",2,1)*Y25*D25)      + IF(N25="X",D25*W25*0.25,0)     ) * IF(M25="X",1.5,1) ) *      IF($AI$13=1,IF(F25="X",1,0.5),1))</f>
-        <v>1.575</v>
-      </c>
-      <c r="AA25" s="3">
-        <f>Z25/$Z$25</f>
-        <v>1</v>
-      </c>
-      <c r="AB25" s="20">
-        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
-        <v>2.5396825396825395</v>
-      </c>
-      <c r="AC25" s="19">
-        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
-        <v>1</v>
-      </c>
+      <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="6"/>
+      <c r="AA25" s="3"/>
+      <c r="AB25" s="20"/>
+      <c r="AC25" s="19"/>
     </row>
     <row r="26" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="1"/>
+      <c r="B26" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26" s="2">
+        <v>12</v>
+      </c>
+      <c r="D26" s="1">
+        <v>3</v>
+      </c>
       <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+      <c r="F26" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -13835,7 +13850,9 @@
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
+      <c r="N26" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="O26" s="1"/>
       <c r="P26" s="3">
         <f>IF(K26="X",1,($AF$3+H26)/20)</f>
@@ -13843,7 +13860,7 @@
       </c>
       <c r="Q26" s="3">
         <f>(C26/20)*IF($AI$6=1,0.5,1)</f>
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="R26" s="3">
         <f>(IF(( L26="X"),0,($AF$5+I26))/20)</f>
@@ -13851,50 +13868,50 @@
       </c>
       <c r="S26" s="6">
         <f>((1*Q26*(P26)*D26   +   (IF(J26="X",2,1)*R26*D26)      + IF(N26="X",D26*P26*0.25,0)     ) * IF(M26="X",1.5,1) ) *      IF($AI$6="1",0.5,1)</f>
-        <v>0</v>
+        <v>1.575</v>
       </c>
       <c r="T26" s="3">
-        <f>S26/$S$25</f>
-        <v>0</v>
-      </c>
-      <c r="U26" s="8" t="e">
-        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]</f>
-        <v>#DIV/0!</v>
+        <f>S26/$S$26</f>
+        <v>1</v>
+      </c>
+      <c r="U26" s="8">
+        <f>$AI$10/Table1453[[#This Row],[WoundsÆ]]</f>
+        <v>2.5396825396825395</v>
       </c>
       <c r="V26" s="4"/>
       <c r="W26" s="3">
-        <f>IF(K26="X",1,($AF$3+IF(F26="X",2,0)+H26)/20)</f>
+        <f>IF(K26="X",1,($AF$3+H26)/20)</f>
         <v>0.5</v>
       </c>
       <c r="X26" s="3">
-        <f>(C26/20)*IF($AI$13=1,IF(F26="X",1,0.5),1)</f>
-        <v>0</v>
+        <f>(C26/20)*IF($AI$14=1,IF(F26="X",1,0.5),1)</f>
+        <v>0.6</v>
       </c>
       <c r="Y26" s="3">
         <f>(IF((OR(K26="X", L26="X")),0,($AF$5+I26))/20)</f>
         <v>0.1</v>
       </c>
       <c r="Z26" s="6">
-        <f>IF(G26="X",0,((1*Q26*(P26)*D26   +   (IF(J26="X",2,1)*R26*D26)      + IF(N26="X",D26*P26*0.5,0)     ) * IF(M26="X",1.5,1) ) *      IF($AI$13=1,IF(F26="X",1,0.5),1))</f>
-        <v>0</v>
+        <f>IF(G26="X",0,((1*X26*(W26)*D26   +   (IF(J26="X",2,1)*Y26*D26)      + IF(N26="X",D26*W26*0.25,0)     ) * IF(M26="X",1.5,1) ) *      IF($AI$14=1,IF(F26="X",1,0.5),1))</f>
+        <v>1.575</v>
       </c>
       <c r="AA26" s="3">
-        <f>Z26/$Z$25</f>
-        <v>0</v>
-      </c>
-      <c r="AB26" s="20" t="e">
-        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
-        <v>#DIV/0!</v>
+        <f>Z26/$Z$26</f>
+        <v>1</v>
+      </c>
+      <c r="AB26" s="20">
+        <f>$AI$10/Table1453[[#This Row],[WoundÆ]]</f>
+        <v>2.5396825396825395</v>
       </c>
       <c r="AC26" s="19">
         <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="22"/>
-      <c r="C27" s="1"/>
+      <c r="C27" s="2"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -13924,11 +13941,11 @@
         <v>0</v>
       </c>
       <c r="T27" s="3">
-        <f>S27/$S$25</f>
+        <f>S27/$S$26</f>
         <v>0</v>
       </c>
       <c r="U27" s="8" t="e">
-        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]</f>
+        <f>$AI$10/Table1453[[#This Row],[WoundsÆ]]</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V27" s="4"/>
@@ -13937,7 +13954,7 @@
         <v>0.5</v>
       </c>
       <c r="X27" s="3">
-        <f>(C27/20)*IF($AI$13=1,IF(F27="X",1,0.5),1)</f>
+        <f>(C27/20)*IF($AI$14=1,IF(F27="X",1,0.5),1)</f>
         <v>0</v>
       </c>
       <c r="Y27" s="3">
@@ -13945,15 +13962,15 @@
         <v>0.1</v>
       </c>
       <c r="Z27" s="6">
-        <f>IF(G27="X",0,((1*Q27*(P27)*D27   +   (IF(J27="X",2,1)*R27*D27)      + IF(N27="X",D27*P27*0.5,0)     ) * IF(M27="X",1.5,1) ) *      IF($AI$13=1,IF(F27="X",1,0.5),1))</f>
+        <f>IF(G27="X",0,((1*Q27*(P27)*D27   +   (IF(J27="X",2,1)*R27*D27)      + IF(N27="X",D27*P27*0.5,0)     ) * IF(M27="X",1.5,1) ) *      IF($AI$14=1,IF(F27="X",1,0.5),1))</f>
         <v>0</v>
       </c>
       <c r="AA27" s="3">
-        <f>Z27/$Z$25</f>
+        <f>Z27/$Z$26</f>
         <v>0</v>
       </c>
       <c r="AB27" s="20" t="e">
-        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
+        <f>$AI$10/Table1453[[#This Row],[WoundÆ]]</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AC27" s="19">
@@ -13961,10 +13978,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="2"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -13977,20 +13994,59 @@
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="3"/>
-      <c r="R28" s="3"/>
-      <c r="S28" s="6"/>
-      <c r="T28" s="3"/>
-      <c r="U28" s="8"/>
+      <c r="P28" s="3">
+        <f>IF(K28="X",1,($AF$3+H28)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q28" s="3">
+        <f>(C28/20)*IF($AI$6=1,0.5,1)</f>
+        <v>0</v>
+      </c>
+      <c r="R28" s="3">
+        <f>(IF(( L28="X"),0,($AF$5+I28))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S28" s="6">
+        <f>((1*Q28*(P28)*D28   +   (IF(J28="X",2,1)*R28*D28)      + IF(N28="X",D28*P28*0.25,0)     ) * IF(M28="X",1.5,1) ) *      IF($AI$6="1",0.5,1)</f>
+        <v>0</v>
+      </c>
+      <c r="T28" s="3">
+        <f>S28/$S$26</f>
+        <v>0</v>
+      </c>
+      <c r="U28" s="8" t="e">
+        <f>$AI$10/Table1453[[#This Row],[WoundsÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="V28" s="4"/>
-      <c r="W28" s="4"/>
-      <c r="X28" s="3"/>
-      <c r="Y28" s="3"/>
-      <c r="Z28" s="6"/>
-      <c r="AA28" s="3"/>
-      <c r="AB28" s="8"/>
-      <c r="AC28" s="3"/>
+      <c r="W28" s="3">
+        <f>IF(K28="X",1,($AF$3+IF(F28="X",2,0)+H28)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="X28" s="3">
+        <f>(C28/20)*IF($AI$14=1,IF(F28="X",1,0.5),1)</f>
+        <v>0</v>
+      </c>
+      <c r="Y28" s="3">
+        <f>(IF((OR(K28="X", L28="X")),0,($AF$5+I28))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z28" s="6">
+        <f>IF(G28="X",0,((1*Q28*(P28)*D28   +   (IF(J28="X",2,1)*R28*D28)      + IF(N28="X",D28*P28*0.5,0)     ) * IF(M28="X",1.5,1) ) *      IF($AI$14=1,IF(F28="X",1,0.5),1))</f>
+        <v>0</v>
+      </c>
+      <c r="AA28" s="3">
+        <f>Z28/$Z$26</f>
+        <v>0</v>
+      </c>
+      <c r="AB28" s="20" t="e">
+        <f>$AI$10/Table1453[[#This Row],[WoundÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC28" s="19">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
@@ -14008,25 +14064,25 @@
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
-      <c r="P29" s="3"/>
+      <c r="P29" s="4"/>
       <c r="Q29" s="3"/>
       <c r="R29" s="3"/>
       <c r="S29" s="6"/>
       <c r="T29" s="3"/>
-      <c r="U29" s="19"/>
+      <c r="U29" s="8"/>
       <c r="V29" s="4"/>
-      <c r="W29" s="3"/>
+      <c r="W29" s="4"/>
       <c r="X29" s="3"/>
       <c r="Y29" s="3"/>
       <c r="Z29" s="6"/>
       <c r="AA29" s="3"/>
-      <c r="AB29" s="20"/>
-      <c r="AC29" s="19"/>
-    </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB29" s="8"/>
+      <c r="AC29" s="3"/>
+    </row>
+    <row r="30" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="2"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -14039,64 +14095,25 @@
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
-      <c r="P30" s="3">
-        <f>(10+$AF$4-$AI$5)/20</f>
-        <v>0.5</v>
-      </c>
-      <c r="Q30" s="3">
-        <f>(C30/20)*IF($AI$6=1,IF(F30="X",1,0.5),1)</f>
-        <v>0</v>
-      </c>
-      <c r="R30" s="3">
-        <f>(IF(( L30="X"),0,($AF$5+I30))/20)</f>
-        <v>0.1</v>
-      </c>
-      <c r="S30" s="6">
-        <f>1*Q30*P30*(1+R30)*D30 + IF(N30="X",D30*P30*0.25,0)</f>
-        <v>0</v>
-      </c>
-      <c r="T30" s="3">
-        <f>S30/$S$4</f>
-        <v>0</v>
-      </c>
-      <c r="U30" s="8" t="e">
-        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]/2</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="3"/>
+      <c r="U30" s="19"/>
       <c r="V30" s="4"/>
-      <c r="W30" s="3">
-        <f>(10+$AF$4-$AI$5)/20</f>
-        <v>0.5</v>
-      </c>
-      <c r="X30" s="3">
-        <f>(C30/20)</f>
-        <v>0</v>
-      </c>
-      <c r="Y30" s="3">
-        <f>(IF((OR(K30="X", L30="X")),0,($AF$5+I30))/20)</f>
-        <v>0.1</v>
-      </c>
-      <c r="Z30" s="6">
-        <f>IF(G30="X",0,1*X30*W30*(1+Y30)*D30) * IF($AI$13=1,IF(F30="X",1,0.5),1) + IF(N30="X",D30*P30*0.25,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AA30" s="3">
-        <f>Z30/$Z$4</f>
-        <v>0</v>
-      </c>
-      <c r="AB30" s="8" t="e">
-        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]/2</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC30" s="3">
-        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="W30" s="3"/>
+      <c r="X30" s="3"/>
+      <c r="Y30" s="3"/>
+      <c r="Z30" s="6"/>
+      <c r="AA30" s="3"/>
+      <c r="AB30" s="20"/>
+      <c r="AC30" s="19"/>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="2"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -14110,11 +14127,11 @@
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="3">
-        <f t="shared" ref="P31:P32" si="16">($AF$3 )/20</f>
+        <f>(10+$AF$4-$AI$5)/20</f>
         <v>0.5</v>
       </c>
       <c r="Q31" s="3">
-        <f>(C31/20)*IF($AI$6=1,0.5,1)</f>
+        <f>(C31/20)*IF($AI$6=1,IF(F31="X",1,0.5),1)</f>
         <v>0</v>
       </c>
       <c r="R31" s="3">
@@ -14122,43 +14139,43 @@
         <v>0.1</v>
       </c>
       <c r="S31" s="6">
-        <f>1*Q31*(P31)*(1+R31)*D31</f>
+        <f>1*Q31*P31*(1+R31)*D31 + IF(N31="X",D31*P31*0.25,0)</f>
         <v>0</v>
       </c>
       <c r="T31" s="3">
-        <f t="shared" ref="T31:T32" si="17">S31/$S$25</f>
+        <f>S31/$S$4</f>
         <v>0</v>
       </c>
-      <c r="U31" s="19" t="e">
-        <f>AI36/Table1453[[#This Row],[WoundsÆ]]</f>
+      <c r="U31" s="8" t="e">
+        <f>$AI$10/Table1453[[#This Row],[WoundsÆ]]/2</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V31" s="4"/>
       <c r="W31" s="3">
-        <f t="shared" ref="W31:W32" si="18">($AF$3)/20</f>
+        <f>(10+$AF$4-$AI$5)/20</f>
         <v>0.5</v>
       </c>
       <c r="X31" s="3">
-        <f>(C31/20)*IF($AI$6=1,IF(F31="X",1,0.5),1)</f>
+        <f>(C31/20)</f>
         <v>0</v>
       </c>
       <c r="Y31" s="3">
-        <f t="shared" ref="Y31:Y32" si="19">($AF$5/20)</f>
+        <f>(IF((OR(K31="X", L31="X")),0,($AF$5+I31))/20)</f>
         <v>0.1</v>
       </c>
       <c r="Z31" s="6">
-        <f>1*X31*(W31)*(1+Y31)*D31</f>
+        <f>IF(G31="X",0,1*X31*W31*(1+Y31)*D31) * IF($AI$14=1,IF(F31="X",1,0.5),1) + IF(N31="X",D31*P31*0.25,0)</f>
         <v>0</v>
       </c>
       <c r="AA31" s="3">
-        <f t="shared" ref="AA31:AA32" si="20">Z31/$Z$25</f>
+        <f>Z31/$Z$4</f>
         <v>0</v>
       </c>
-      <c r="AB31" s="20" t="e">
-        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
+      <c r="AB31" s="8" t="e">
+        <f>$AI$10/Table1453[[#This Row],[WoundÆ]]/2</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AC31" s="19">
+      <c r="AC31" s="3">
         <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
         <v>0</v>
       </c>
@@ -14180,7 +14197,7 @@
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
       <c r="P32" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="P32:P33" si="19">($AF$3 )/20</f>
         <v>0.5</v>
       </c>
       <c r="Q32" s="3">
@@ -14196,7 +14213,7 @@
         <v>0</v>
       </c>
       <c r="T32" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="T32:T33" si="20">S32/$S$26</f>
         <v>0</v>
       </c>
       <c r="U32" s="19" t="e">
@@ -14205,7 +14222,7 @@
       </c>
       <c r="V32" s="4"/>
       <c r="W32" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="W32:W33" si="21">($AF$3)/20</f>
         <v>0.5</v>
       </c>
       <c r="X32" s="3">
@@ -14213,7 +14230,7 @@
         <v>0</v>
       </c>
       <c r="Y32" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="Y32:Y33" si="22">($AF$5/20)</f>
         <v>0.1</v>
       </c>
       <c r="Z32" s="6">
@@ -14221,11 +14238,11 @@
         <v>0</v>
       </c>
       <c r="AA32" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="AA32:AA33" si="23">Z32/$Z$26</f>
         <v>0</v>
       </c>
       <c r="AB32" s="20" t="e">
-        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
+        <f>$AI$10/Table1453[[#This Row],[WoundÆ]]</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AC32" s="19">
@@ -14249,24 +14266,62 @@
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
-      <c r="P33" s="3"/>
-      <c r="Q33" s="3"/>
-      <c r="R33" s="3"/>
-      <c r="S33" s="6"/>
-      <c r="T33" s="3"/>
-      <c r="U33" s="19"/>
+      <c r="P33" s="3">
+        <f t="shared" si="19"/>
+        <v>0.5</v>
+      </c>
+      <c r="Q33" s="3">
+        <f>(C33/20)*IF($AI$6=1,0.5,1)</f>
+        <v>0</v>
+      </c>
+      <c r="R33" s="3">
+        <f>(IF(( L33="X"),0,($AF$5+I33))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S33" s="6">
+        <f>1*Q33*(P33)*(1+R33)*D33</f>
+        <v>0</v>
+      </c>
+      <c r="T33" s="3">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="U33" s="19" t="e">
+        <f>AI38/Table1453[[#This Row],[WoundsÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="V33" s="4"/>
-      <c r="W33" s="3"/>
-      <c r="X33" s="3"/>
-      <c r="Y33" s="3"/>
-      <c r="Z33" s="6"/>
-      <c r="AA33" s="3"/>
-      <c r="AB33" s="20"/>
-      <c r="AC33" s="19"/>
-      <c r="AD33" s="16"/>
+      <c r="W33" s="3">
+        <f t="shared" si="21"/>
+        <v>0.5</v>
+      </c>
+      <c r="X33" s="3">
+        <f>(C33/20)*IF($AI$6=1,IF(F33="X",1,0.5),1)</f>
+        <v>0</v>
+      </c>
+      <c r="Y33" s="3">
+        <f t="shared" si="22"/>
+        <v>0.1</v>
+      </c>
+      <c r="Z33" s="6">
+        <f>1*X33*(W33)*(1+Y33)*D33</f>
+        <v>0</v>
+      </c>
+      <c r="AA33" s="3">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="AB33" s="20" t="e">
+        <f>$AI$10/Table1453[[#This Row],[WoundÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC33" s="19">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
+      <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="2"/>
       <c r="D34" s="1"/>
@@ -14281,79 +14336,40 @@
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
-      <c r="P34" s="3">
-        <f>IF(K34="X",1,($AF$3+H34)/20)</f>
-        <v>0.5</v>
-      </c>
-      <c r="Q34" s="3">
-        <f>(C34/20)*IF($AI$6=1,0.5,1)</f>
-        <v>0</v>
-      </c>
-      <c r="R34" s="3">
-        <f>(IF(( L34="X"),0,($AF$5+I34))/20)</f>
-        <v>0.1</v>
-      </c>
-      <c r="S34" s="6">
-        <f>((1*Q34*(P34)*D34   +   (IF(J34="X",2,1)*R34*D34)      + IF(N34="X",D34*P34*0.25,0)     ) * IF(M34="X",1.5,1) ) *      IF($AI$6="1",0.5,1)</f>
-        <v>0</v>
-      </c>
-      <c r="T34" s="3">
-        <f>S34/$S$15</f>
-        <v>0</v>
-      </c>
-      <c r="U34" s="8" t="e">
-        <f>$AI$9/Table1453[[#This Row],[WoundsÆ]]</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="6"/>
+      <c r="T34" s="3"/>
+      <c r="U34" s="19"/>
       <c r="V34" s="4"/>
-      <c r="W34" s="3">
-        <f>IF(K34="X",1,($AF$3+IF(F34="X",2,0)+H34)/20)</f>
-        <v>0.5</v>
-      </c>
-      <c r="X34" s="3">
-        <f>(C34/20)*IF($AI$13=1,IF(F34="X",1,0.5),1)</f>
-        <v>0</v>
-      </c>
-      <c r="Y34" s="3">
-        <f>(IF((OR(K34="X", L34="X")),0,($AF$5+I34))/20)</f>
-        <v>0.1</v>
-      </c>
-      <c r="Z34" s="6">
-        <f>IF(G34="X",0,((1*Q34*(P34)*D34   +   (IF(J34="X",2,1)*R34*D34)      + IF(N34="X",D34*P34*0.5,0)     ) * IF(M34="X",1.5,1) ) *      IF($AI$13=1,IF(F34="X",1,0.5),1))</f>
-        <v>0</v>
-      </c>
-      <c r="AA34" s="3" t="e">
-        <f t="shared" ref="AA34" si="21">Z34/$Z$15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AB34" s="20" t="e">
-        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC34" s="19" t="e">
-        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="W34" s="3"/>
+      <c r="X34" s="3"/>
+      <c r="Y34" s="3"/>
+      <c r="Z34" s="6"/>
+      <c r="AA34" s="3"/>
+      <c r="AB34" s="20"/>
+      <c r="AC34" s="19"/>
       <c r="AD34" s="16"/>
     </row>
     <row r="35" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
-      <c r="O35" s="9"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
       <c r="P35" s="3">
-        <f t="shared" ref="P35" si="22">($AF$3 )/20</f>
+        <f>IF(K35="X",1,($AF$3+H35)/20)</f>
         <v>0.5</v>
       </c>
       <c r="Q35" s="3">
@@ -14365,45 +14381,45 @@
         <v>0.1</v>
       </c>
       <c r="S35" s="6">
-        <f>1*Q35*(P35)*(1+R35)*D35</f>
+        <f>((1*Q35*(P35)*D35   +   (IF(J35="X",2,1)*R35*D35)      + IF(N35="X",D35*P35*0.25,0)     ) * IF(M35="X",1.5,1) ) *      IF($AI$6="1",0.5,1)</f>
         <v>0</v>
       </c>
       <c r="T35" s="3">
-        <f t="shared" ref="T35" si="23">S35/$S$25</f>
+        <f>S35/$S$16</f>
         <v>0</v>
       </c>
-      <c r="U35" s="19" t="e">
-        <f>AI40/Table1453[[#This Row],[WoundsÆ]]</f>
+      <c r="U35" s="8" t="e">
+        <f>$AI$10/Table1453[[#This Row],[WoundsÆ]]</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V35" s="4"/>
       <c r="W35" s="3">
-        <f t="shared" ref="W35" si="24">($AF$3)/20</f>
+        <f>IF(K35="X",1,($AF$3+IF(F35="X",2,0)+H35)/20)</f>
         <v>0.5</v>
       </c>
       <c r="X35" s="3">
-        <f>(C35/20)*IF($AI$6=1,IF(F35="X",1,0.5),1)</f>
+        <f>(C35/20)*IF($AI$14=1,IF(F35="X",1,0.5),1)</f>
         <v>0</v>
       </c>
       <c r="Y35" s="3">
-        <f t="shared" ref="Y35" si="25">($AF$5/20)</f>
+        <f>(IF((OR(K35="X", L35="X")),0,($AF$5+I35))/20)</f>
         <v>0.1</v>
       </c>
       <c r="Z35" s="6">
-        <f>1*X35*(W35)*(1+Y35)*D35</f>
+        <f>IF(G35="X",0,((1*Q35*(P35)*D35   +   (IF(J35="X",2,1)*R35*D35)      + IF(N35="X",D35*P35*0.5,0)     ) * IF(M35="X",1.5,1) ) *      IF($AI$14=1,IF(F35="X",1,0.5),1))</f>
         <v>0</v>
       </c>
-      <c r="AA35" s="3">
-        <f t="shared" ref="AA35" si="26">Z35/$Z$25</f>
-        <v>0</v>
+      <c r="AA35" s="3" t="e">
+        <f t="shared" ref="AA35" si="24">Z35/$Z$16</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="AB35" s="20" t="e">
-        <f>$AI$9/Table1453[[#This Row],[WoundÆ]]</f>
+        <f>$AI$10/Table1453[[#This Row],[WoundÆ]]</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AC35" s="19">
+      <c r="AC35" s="19" t="e">
         <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="AD35" s="16"/>
     </row>
@@ -14423,20 +14439,59 @@
       <c r="M36" s="9"/>
       <c r="N36" s="9"/>
       <c r="O36" s="9"/>
-      <c r="P36" s="3"/>
-      <c r="Q36" s="3"/>
-      <c r="R36" s="3"/>
-      <c r="S36" s="6"/>
-      <c r="T36" s="3"/>
-      <c r="U36" s="8"/>
+      <c r="P36" s="3">
+        <f t="shared" ref="P36" si="25">($AF$3 )/20</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q36" s="3">
+        <f>(C36/20)*IF($AI$6=1,0.5,1)</f>
+        <v>0</v>
+      </c>
+      <c r="R36" s="3">
+        <f>(IF(( L36="X"),0,($AF$5+I36))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S36" s="6">
+        <f>1*Q36*(P36)*(1+R36)*D36</f>
+        <v>0</v>
+      </c>
+      <c r="T36" s="3">
+        <f t="shared" ref="T36" si="26">S36/$S$26</f>
+        <v>0</v>
+      </c>
+      <c r="U36" s="19" t="e">
+        <f>AI41/Table1453[[#This Row],[WoundsÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="V36" s="4"/>
-      <c r="W36" s="3"/>
-      <c r="X36" s="3"/>
-      <c r="Y36" s="3"/>
-      <c r="Z36" s="6"/>
-      <c r="AA36" s="3"/>
-      <c r="AB36" s="20"/>
-      <c r="AC36" s="19"/>
+      <c r="W36" s="3">
+        <f t="shared" ref="W36" si="27">($AF$3)/20</f>
+        <v>0.5</v>
+      </c>
+      <c r="X36" s="3">
+        <f>(C36/20)*IF($AI$6=1,IF(F36="X",1,0.5),1)</f>
+        <v>0</v>
+      </c>
+      <c r="Y36" s="3">
+        <f t="shared" ref="Y36" si="28">($AF$5/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z36" s="6">
+        <f>1*X36*(W36)*(1+Y36)*D36</f>
+        <v>0</v>
+      </c>
+      <c r="AA36" s="3">
+        <f t="shared" ref="AA36" si="29">Z36/$Z$26</f>
+        <v>0</v>
+      </c>
+      <c r="AB36" s="20" t="e">
+        <f>$AI$10/Table1453[[#This Row],[WoundÆ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC36" s="19">
+        <f>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</f>
+        <v>0</v>
+      </c>
       <c r="AD36" s="16"/>
     </row>
     <row r="37" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
@@ -14533,29 +14588,30 @@
       <c r="AA39" s="3"/>
       <c r="AB39" s="20"/>
       <c r="AC39" s="19"/>
+      <c r="AD39" s="16"/>
     </row>
     <row r="40" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-      <c r="N40" s="1"/>
-      <c r="O40" s="1"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
+      <c r="O40" s="9"/>
       <c r="P40" s="3"/>
       <c r="Q40" s="3"/>
       <c r="R40" s="3"/>
       <c r="S40" s="6"/>
       <c r="T40" s="3"/>
-      <c r="U40" s="19"/>
+      <c r="U40" s="8"/>
       <c r="V40" s="4"/>
       <c r="W40" s="3"/>
       <c r="X40" s="3"/>
@@ -14567,36 +14623,37 @@
     </row>
     <row r="41" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="9"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
-      <c r="J41" s="9"/>
-      <c r="K41" s="9"/>
-      <c r="L41" s="9"/>
-      <c r="M41" s="9"/>
-      <c r="N41" s="9"/>
-      <c r="O41" s="11"/>
-      <c r="P41" s="11"/>
-      <c r="Q41" s="11"/>
-      <c r="R41" s="11"/>
-      <c r="S41" s="11"/>
-      <c r="T41" s="13"/>
-      <c r="U41" s="14"/>
-      <c r="V41" s="11"/>
-      <c r="W41" s="11"/>
-      <c r="X41" s="11"/>
-      <c r="Y41" s="11"/>
-      <c r="Z41" s="11"/>
-      <c r="AA41" s="13"/>
-      <c r="AB41" s="11"/>
-      <c r="AC41" s="16"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="3"/>
+      <c r="S41" s="6"/>
+      <c r="T41" s="3"/>
+      <c r="U41" s="19"/>
+      <c r="V41" s="4"/>
+      <c r="W41" s="3"/>
+      <c r="X41" s="3"/>
+      <c r="Y41" s="3"/>
+      <c r="Z41" s="6"/>
+      <c r="AA41" s="3"/>
+      <c r="AB41" s="20"/>
+      <c r="AC41" s="19"/>
     </row>
     <row r="42" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="9"/>
       <c r="B42" s="10"/>
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
@@ -14656,13 +14713,43 @@
       <c r="AB43" s="11"/>
       <c r="AC43" s="16"/>
     </row>
+    <row r="44" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B44" s="10"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="9"/>
+      <c r="L44" s="9"/>
+      <c r="M44" s="9"/>
+      <c r="N44" s="9"/>
+      <c r="O44" s="11"/>
+      <c r="P44" s="11"/>
+      <c r="Q44" s="11"/>
+      <c r="R44" s="11"/>
+      <c r="S44" s="11"/>
+      <c r="T44" s="13"/>
+      <c r="U44" s="14"/>
+      <c r="V44" s="11"/>
+      <c r="W44" s="11"/>
+      <c r="X44" s="11"/>
+      <c r="Y44" s="11"/>
+      <c r="Z44" s="11"/>
+      <c r="AA44" s="13"/>
+      <c r="AB44" s="11"/>
+      <c r="AC44" s="16"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="P2:S2"/>
     <mergeCell ref="W2:Z2"/>
   </mergeCells>
-  <conditionalFormatting sqref="AA41:AA43 T41:T43 U31:U33 AB31:AB33 AB35:AB39 U35:U39 AB4:AB28 U4:U28">
+  <conditionalFormatting sqref="AA42:AA44 T42:T44 U32:U34 AB32:AB34 AB36:AB40 U36:U40 AB4:AB29 U4:U29">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -14674,7 +14761,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z41:Z43 S41:S43 T31:T33 AA31:AA33 AA35:AA39 T35:T39 AA4:AA28 T4:T28">
+  <conditionalFormatting sqref="Z42:Z44 S42:S44 T32:T34 AA32:AA34 AA36:AA40 T36:T40 AA4:AA29 T4:T29">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -14686,7 +14773,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB41:AB43 AC31:AC33 AC35:AC39 AC4:AC28">
+  <conditionalFormatting sqref="AB42:AB44 AC32:AC34 AC36:AC40 AC4:AC29">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -14698,7 +14785,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB30 U30">
+  <conditionalFormatting sqref="U31 AB31">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -14710,7 +14797,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA30 T30">
+  <conditionalFormatting sqref="T31 AA31">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -14722,7 +14809,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC30">
+  <conditionalFormatting sqref="AC31">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -14734,7 +14821,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB34 U34">
+  <conditionalFormatting sqref="U35 AB35">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -14746,7 +14833,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA34 T34">
+  <conditionalFormatting sqref="T35 AA35">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -14758,7 +14845,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC34">
+  <conditionalFormatting sqref="AC35">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0.5"/>

</xml_diff>

<commit_message>
Added "Hydra Dominatus", small fix in the balancing sheet
</commit_message>
<xml_diff>
--- a/Balancing Sheet.xlsx
+++ b/Balancing Sheet.xlsx
@@ -609,14 +609,6 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="123">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2081,6 +2073,14 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2724,85 +2724,85 @@
     <tableColumn id="29" name="No Crits     ." dataDxfId="80"/>
     <tableColumn id="32" name="Lethal Wounds    ." dataDxfId="79"/>
     <tableColumn id="27" name="Lethal Weapon    ." dataDxfId="78"/>
-    <tableColumn id="17" name="Rend       ." dataDxfId="0"/>
-    <tableColumn id="7" name="Column2" dataDxfId="77" dataCellStyle="Percent"/>
-    <tableColumn id="8" name="Hit%" dataDxfId="76" dataCellStyle="Percent"/>
-    <tableColumn id="9" name="Wound%" dataDxfId="75" dataCellStyle="Percent"/>
-    <tableColumn id="11" name="Crit%" dataDxfId="74" dataCellStyle="Percent"/>
-    <tableColumn id="12" name="WoundsÆ" dataDxfId="73" dataCellStyle="Percent"/>
-    <tableColumn id="20" name="% Base" dataDxfId="72" dataCellStyle="Percent"/>
-    <tableColumn id="13" name="To Kill" dataDxfId="71" dataCellStyle="Comma"/>
-    <tableColumn id="14" name="Column3" dataDxfId="70" dataCellStyle="Percent"/>
-    <tableColumn id="15" name="Hit %" dataDxfId="69" dataCellStyle="Percent"/>
-    <tableColumn id="16" name="Wound %" dataDxfId="68" dataCellStyle="Percent"/>
-    <tableColumn id="18" name="Crit %" dataDxfId="67" dataCellStyle="Percent"/>
-    <tableColumn id="19" name="WoundÆ" dataDxfId="66" dataCellStyle="Percent"/>
-    <tableColumn id="21" name="% Base2" dataDxfId="65" dataCellStyle="Percent"/>
-    <tableColumn id="22" name="To Kill2" dataDxfId="64" dataCellStyle="Percent"/>
-    <tableColumn id="10" name="Combo" dataDxfId="63" dataCellStyle="Percent"/>
+    <tableColumn id="17" name="Rend       ." dataDxfId="77"/>
+    <tableColumn id="7" name="Column2" dataDxfId="76" dataCellStyle="Percent"/>
+    <tableColumn id="8" name="Hit%" dataDxfId="75" dataCellStyle="Percent"/>
+    <tableColumn id="9" name="Wound%" dataDxfId="74" dataCellStyle="Percent"/>
+    <tableColumn id="11" name="Crit%" dataDxfId="73" dataCellStyle="Percent"/>
+    <tableColumn id="12" name="WoundsÆ" dataDxfId="72" dataCellStyle="Percent"/>
+    <tableColumn id="20" name="% Base" dataDxfId="71" dataCellStyle="Percent"/>
+    <tableColumn id="13" name="To Kill" dataDxfId="70" dataCellStyle="Comma"/>
+    <tableColumn id="14" name="Column3" dataDxfId="69" dataCellStyle="Percent"/>
+    <tableColumn id="15" name="Hit %" dataDxfId="68" dataCellStyle="Percent"/>
+    <tableColumn id="16" name="Wound %" dataDxfId="67" dataCellStyle="Percent"/>
+    <tableColumn id="18" name="Crit %" dataDxfId="66" dataCellStyle="Percent"/>
+    <tableColumn id="19" name="WoundÆ" dataDxfId="65" dataCellStyle="Percent"/>
+    <tableColumn id="21" name="% Base2" dataDxfId="64" dataCellStyle="Percent"/>
+    <tableColumn id="22" name="To Kill2" dataDxfId="63" dataCellStyle="Percent"/>
+    <tableColumn id="10" name="Combo" dataDxfId="62" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="B3:AE35" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61" dataCellStyle="Percent">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="B3:AE35" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60" dataCellStyle="Percent">
   <autoFilter ref="B3:AE35"/>
   <tableColumns count="30">
-    <tableColumn id="1" name="Name" dataDxfId="60"/>
-    <tableColumn id="2" name="Damage" dataDxfId="59"/>
-    <tableColumn id="3" name="Attacks" dataDxfId="58"/>
-    <tableColumn id="5" name="Note" dataDxfId="57"/>
-    <tableColumn id="6" name="Penetration" dataDxfId="56"/>
-    <tableColumn id="30" name="Light Weapon    ." dataDxfId="55"/>
-    <tableColumn id="23" name="MM      ." dataDxfId="54"/>
-    <tableColumn id="24" name="Crit       ." dataDxfId="53"/>
-    <tableColumn id="26" name="Weak Spots" dataDxfId="52"/>
-    <tableColumn id="25" name="Cone      ." dataDxfId="51"/>
-    <tableColumn id="29" name="No Crits     ." dataDxfId="50"/>
-    <tableColumn id="32" name="2H        ." dataDxfId="49"/>
-    <tableColumn id="33" name="Heavy Strikes      ." dataDxfId="48"/>
-    <tableColumn id="4" name="Lethal Wounds    ." dataDxfId="47"/>
-    <tableColumn id="28" name="Lethal Weapon    ." dataDxfId="46"/>
-    <tableColumn id="27" name="Column2" dataDxfId="45"/>
-    <tableColumn id="7" name="Hit%" dataDxfId="44" dataCellStyle="Percent">
+    <tableColumn id="1" name="Name" dataDxfId="59"/>
+    <tableColumn id="2" name="Damage" dataDxfId="58"/>
+    <tableColumn id="3" name="Attacks" dataDxfId="57"/>
+    <tableColumn id="5" name="Note" dataDxfId="56"/>
+    <tableColumn id="6" name="Penetration" dataDxfId="55"/>
+    <tableColumn id="30" name="Light Weapon    ." dataDxfId="54"/>
+    <tableColumn id="23" name="MM      ." dataDxfId="53"/>
+    <tableColumn id="24" name="Crit       ." dataDxfId="52"/>
+    <tableColumn id="26" name="Weak Spots" dataDxfId="51"/>
+    <tableColumn id="25" name="Cone      ." dataDxfId="50"/>
+    <tableColumn id="29" name="No Crits     ." dataDxfId="49"/>
+    <tableColumn id="32" name="2H        ." dataDxfId="48"/>
+    <tableColumn id="33" name="Heavy Strikes      ." dataDxfId="47"/>
+    <tableColumn id="4" name="Lethal Wounds    ." dataDxfId="46"/>
+    <tableColumn id="28" name="Lethal Weapon    ." dataDxfId="45"/>
+    <tableColumn id="27" name="Column2" dataDxfId="44"/>
+    <tableColumn id="7" name="Hit%" dataDxfId="43" dataCellStyle="Percent">
       <calculatedColumnFormula>($AH$3 )/20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Wound%" dataDxfId="43" dataCellStyle="Percent">
+    <tableColumn id="8" name="Wound%" dataDxfId="42" dataCellStyle="Percent">
       <calculatedColumnFormula>(C4/20)*IF($AK$6=1,0.5,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Crit%" dataDxfId="42" dataCellStyle="Percent">
+    <tableColumn id="9" name="Crit%" dataDxfId="41" dataCellStyle="Percent">
       <calculatedColumnFormula>(IF(( L4="X"),0,($AH$5+I4))/20)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="WoundsÆ" dataDxfId="41">
+    <tableColumn id="11" name="WoundsÆ" dataDxfId="40">
       <calculatedColumnFormula>1*S4*(R4)*(1+T4)*D4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="% Base" dataDxfId="40" dataCellStyle="Percent">
+    <tableColumn id="12" name="% Base" dataDxfId="39" dataCellStyle="Percent">
       <calculatedColumnFormula>U4/$U$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="To Kill" dataDxfId="39" dataCellStyle="Percent">
+    <tableColumn id="20" name="To Kill" dataDxfId="38" dataCellStyle="Percent">
       <calculatedColumnFormula>AK9/Table145[[#This Row],[WoundsÆ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Column3" dataDxfId="38"/>
-    <tableColumn id="14" name="Hit %" dataDxfId="37" dataCellStyle="Percent">
+    <tableColumn id="13" name="Column3" dataDxfId="37"/>
+    <tableColumn id="14" name="Hit %" dataDxfId="36" dataCellStyle="Percent">
       <calculatedColumnFormula>($AH$3)/20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Wound %" dataDxfId="36" dataCellStyle="Percent">
+    <tableColumn id="15" name="Wound %" dataDxfId="35" dataCellStyle="Percent">
       <calculatedColumnFormula>(C4/20)*IF($AK$6=1,IF(F4="X",1,0.5),1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Crit %" dataDxfId="35" dataCellStyle="Percent">
+    <tableColumn id="16" name="Crit %" dataDxfId="34" dataCellStyle="Percent">
       <calculatedColumnFormula>($AH$5/20)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="WoundÆ" dataDxfId="34">
+    <tableColumn id="18" name="WoundÆ" dataDxfId="33">
       <calculatedColumnFormula>1*Z4*(Y4)*(1+AA4)*D4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="% Base2" dataDxfId="33" dataCellStyle="Percent">
+    <tableColumn id="19" name="% Base2" dataDxfId="32" dataCellStyle="Percent">
       <calculatedColumnFormula>AB4/$AB$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="To Kill2" dataDxfId="32" dataCellStyle="Percent">
+    <tableColumn id="21" name="To Kill2" dataDxfId="31" dataCellStyle="Percent">
       <calculatedColumnFormula>$AK$9/Table145[[#This Row],[WoundÆ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="Combo" dataDxfId="31" dataCellStyle="Percent">
+    <tableColumn id="22" name="Combo" dataDxfId="30" dataCellStyle="Percent">
       <calculatedColumnFormula>(Table145[[#This Row],[% Base]]+Table145[[#This Row],[% Base2]])/2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2811,61 +2811,61 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table1453" displayName="Table1453" ref="B3:AC36" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" dataCellStyle="Percent">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table1453" displayName="Table1453" ref="B3:AC36" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" dataCellStyle="Percent">
   <autoFilter ref="B3:AC36"/>
   <tableColumns count="28">
-    <tableColumn id="1" name="Name" dataDxfId="28"/>
-    <tableColumn id="2" name="Damage" dataDxfId="27"/>
-    <tableColumn id="3" name="Attacks" dataDxfId="26"/>
-    <tableColumn id="5" name="Note" dataDxfId="25"/>
-    <tableColumn id="6" name="Penetration" dataDxfId="24"/>
-    <tableColumn id="30" name="Light Weapon    ." dataDxfId="23"/>
-    <tableColumn id="23" name="MM      ." dataDxfId="22"/>
-    <tableColumn id="24" name="Crit       ." dataDxfId="21"/>
-    <tableColumn id="26" name="Weak Spots" dataDxfId="20"/>
-    <tableColumn id="25" name="Cone      ." dataDxfId="19"/>
-    <tableColumn id="29" name="No Crits     ." dataDxfId="18"/>
-    <tableColumn id="4" name="Lethal Wounds    ." dataDxfId="17"/>
-    <tableColumn id="28" name="Lethal Weapon    ." dataDxfId="16"/>
-    <tableColumn id="27" name="Column2" dataDxfId="15"/>
-    <tableColumn id="7" name="Hit%" dataDxfId="14" dataCellStyle="Percent">
+    <tableColumn id="1" name="Name" dataDxfId="27"/>
+    <tableColumn id="2" name="Damage" dataDxfId="26"/>
+    <tableColumn id="3" name="Attacks" dataDxfId="25"/>
+    <tableColumn id="5" name="Note" dataDxfId="24"/>
+    <tableColumn id="6" name="Penetration" dataDxfId="23"/>
+    <tableColumn id="30" name="Light Weapon    ." dataDxfId="22"/>
+    <tableColumn id="23" name="MM      ." dataDxfId="21"/>
+    <tableColumn id="24" name="Crit       ." dataDxfId="20"/>
+    <tableColumn id="26" name="Weak Spots" dataDxfId="19"/>
+    <tableColumn id="25" name="Cone      ." dataDxfId="18"/>
+    <tableColumn id="29" name="No Crits     ." dataDxfId="17"/>
+    <tableColumn id="4" name="Lethal Wounds    ." dataDxfId="16"/>
+    <tableColumn id="28" name="Lethal Weapon    ." dataDxfId="15"/>
+    <tableColumn id="27" name="Column2" dataDxfId="14"/>
+    <tableColumn id="7" name="Hit%" dataDxfId="13" dataCellStyle="Percent">
       <calculatedColumnFormula>($AF$3 )/20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Wound%" dataDxfId="13" dataCellStyle="Percent">
+    <tableColumn id="8" name="Wound%" dataDxfId="12" dataCellStyle="Percent">
       <calculatedColumnFormula>(C4/20)*IF($AI$6=1,0.5,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Crit%" dataDxfId="12" dataCellStyle="Percent">
+    <tableColumn id="9" name="Crit%" dataDxfId="11" dataCellStyle="Percent">
       <calculatedColumnFormula>(IF(( L4="X"),0,($AF$5+I4))/20)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="WoundsÆ" dataDxfId="11">
+    <tableColumn id="11" name="WoundsÆ" dataDxfId="10">
       <calculatedColumnFormula>1*Q4*(P4)*(1+R4)*D4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="% Base" dataDxfId="10" dataCellStyle="Percent">
+    <tableColumn id="12" name="% Base" dataDxfId="9" dataCellStyle="Percent">
       <calculatedColumnFormula>S4/$S$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="To Kill" dataDxfId="9" dataCellStyle="Percent">
+    <tableColumn id="20" name="To Kill" dataDxfId="8" dataCellStyle="Percent">
       <calculatedColumnFormula>AI10/Table1453[[#This Row],[WoundsÆ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Column3" dataDxfId="8"/>
-    <tableColumn id="14" name="Hit %" dataDxfId="7" dataCellStyle="Percent">
+    <tableColumn id="13" name="Column3" dataDxfId="7"/>
+    <tableColumn id="14" name="Hit %" dataDxfId="6" dataCellStyle="Percent">
       <calculatedColumnFormula>($AF$3)/20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Wound %" dataDxfId="6" dataCellStyle="Percent">
+    <tableColumn id="15" name="Wound %" dataDxfId="5" dataCellStyle="Percent">
       <calculatedColumnFormula>(C4/20)*IF($AI$6=1,IF(F4="X",1,0.5),1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Crit %" dataDxfId="5" dataCellStyle="Percent">
+    <tableColumn id="16" name="Crit %" dataDxfId="4" dataCellStyle="Percent">
       <calculatedColumnFormula>($AF$5/20)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="WoundÆ" dataDxfId="4">
+    <tableColumn id="18" name="WoundÆ" dataDxfId="3">
       <calculatedColumnFormula>1*X4*(W4)*(1+Y4)*D4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="% Base2" dataDxfId="3" dataCellStyle="Percent">
+    <tableColumn id="19" name="% Base2" dataDxfId="2" dataCellStyle="Percent">
       <calculatedColumnFormula>Z4/$Z$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="To Kill2" dataDxfId="2" dataCellStyle="Percent">
+    <tableColumn id="21" name="To Kill2" dataDxfId="1" dataCellStyle="Percent">
       <calculatedColumnFormula>$AI$10/Table1453[[#This Row],[WoundÆ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="Combo" dataDxfId="1" dataCellStyle="Percent">
+    <tableColumn id="22" name="Combo" dataDxfId="0" dataCellStyle="Percent">
       <calculatedColumnFormula>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6255,8 +6255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AJ67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AG5" sqref="AG5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6422,7 +6422,7 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="3">
         <f>(10+$AG$4-$AJ$5)/20</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="R4" s="3">
         <f>(C4/20)*IF($AJ$6=1,IF(F4="X",1,0.5),1)</f>
@@ -6433,8 +6433,8 @@
         <v>0.1</v>
       </c>
       <c r="T4" s="5">
-        <f>1*R4*Q4*(1+S4)*D4 + IF(N4="X",D4*Q4*0.25,0) + IF(M4="X",D4*Q4*R4*0.5,0) + 2*(O4/20)</f>
-        <v>0.88000000000000012</v>
+        <f>1*R4*Q4*(1+S4)*D4 + IF(N4="X",D4*Q4*0.25,0) + IF(M4="X",D4*Q4*R4*0.5,0) +  2*(O4/20)*Q4*R4</f>
+        <v>0.44000000000000006</v>
       </c>
       <c r="U4" s="3">
         <f>T4/$T$4</f>
@@ -6442,12 +6442,12 @@
       </c>
       <c r="V4" s="7">
         <f>$AJ$3/T4/2</f>
-        <v>2.2727272727272725</v>
+        <v>4.545454545454545</v>
       </c>
       <c r="W4" s="4"/>
       <c r="X4" s="3">
         <f>(10+$AG$4-$AJ$5)/20</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Y4" s="3">
         <f>(C4/20)</f>
@@ -6458,8 +6458,8 @@
         <v>0.1</v>
       </c>
       <c r="AA4" s="5">
-        <f>IF(G4="X",0,1*Y4*X4*(1+Z4)*D4) * IF($AJ$13=1,IF(F4="X",1,0.5),1) + IF(N4="X",D4*Q4*0.25,0) + 2*(O4/20)</f>
-        <v>0.44000000000000006</v>
+        <f>IF(G4="X",0,1*Y4*X4*(1+Z4)*D4) * IF($AJ$13=1,IF(F4="X",1,0.5),1) + IF(N4="X",D4*Q4*0.25,0) +  2*(O4/20)*Q4*R4</f>
+        <v>0.22000000000000003</v>
       </c>
       <c r="AB4" s="3">
         <f>AA4/$AA$4</f>
@@ -6467,7 +6467,7 @@
       </c>
       <c r="AC4" s="7">
         <f t="shared" ref="AC4:AC12" si="0">$AJ$9/AA4/2</f>
-        <v>4.545454545454545</v>
+        <v>9.0909090909090899</v>
       </c>
       <c r="AD4" s="3">
         <f>(U4+AB4)/2</f>
@@ -6478,7 +6478,7 @@
         <v>85</v>
       </c>
       <c r="AG4">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AI4" t="s">
         <v>85</v>
@@ -6511,7 +6511,7 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="3">
         <f t="shared" ref="Q5:Q12" si="1">(10+$AG$4-$AJ$5)/20</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="R5" s="3">
         <f t="shared" ref="R5:R11" si="2">(C5/20)*IF($AJ$6=1,IF(F5="X",1,0.5),1)</f>
@@ -6522,8 +6522,8 @@
         <v>0.1</v>
       </c>
       <c r="T5" s="5">
-        <f t="shared" ref="T5:T12" si="4">1*R5*Q5*(1+S5)*D5 + IF(N5="X",D5*Q5*0.25,0) + IF(M5="X",D5*Q5*R5*0.5,0) + 2*(O5/20)</f>
-        <v>1.1000000000000001</v>
+        <f t="shared" ref="T5:T12" si="4">1*R5*Q5*(1+S5)*D5 + IF(N5="X",D5*Q5*0.25,0) + IF(M5="X",D5*Q5*R5*0.5,0) +  2*(O5/20)*Q5*R5</f>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U5" s="3">
         <f>T5/$T$4</f>
@@ -6531,12 +6531,12 @@
       </c>
       <c r="V5" s="7">
         <f t="shared" ref="V5:V11" si="5">$AJ$3/T5/2</f>
-        <v>1.8181818181818181</v>
+        <v>3.6363636363636362</v>
       </c>
       <c r="W5" s="4"/>
       <c r="X5" s="3">
         <f t="shared" ref="X5:X12" si="6">(10+$AG$4-$AJ$5)/20</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Y5" s="3">
         <f>(C5/20)*IF($AK$14=1,IF(F5="X",1,0.5),1)</f>
@@ -6547,8 +6547,8 @@
         <v>0.1</v>
       </c>
       <c r="AA5" s="5">
-        <f t="shared" ref="AA5:AA12" si="8">IF(G5="X",0,1*Y5*X5*(1+Z5)*D5) * IF($AJ$13=1,IF(F5="X",1,0.5),1) + IF(N5="X",D5*Q5*0.25,0) + 2*(O5/20)</f>
-        <v>0.55000000000000004</v>
+        <f t="shared" ref="AA5:AA12" si="8">IF(G5="X",0,1*Y5*X5*(1+Z5)*D5) * IF($AJ$13=1,IF(F5="X",1,0.5),1) + IF(N5="X",D5*Q5*0.25,0) +  2*(O5/20)*Q5*R5</f>
+        <v>0.27500000000000002</v>
       </c>
       <c r="AB5" s="3">
         <f>AA5/$AA$4</f>
@@ -6556,7 +6556,7 @@
       </c>
       <c r="AC5" s="7">
         <f t="shared" si="0"/>
-        <v>3.6363636363636362</v>
+        <v>7.2727272727272725</v>
       </c>
       <c r="AD5" s="3">
         <f t="shared" ref="AD5:AD11" si="9">(U5+AB5)/2</f>
@@ -6602,7 +6602,7 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="R6" s="3">
         <f t="shared" si="2"/>
@@ -6614,7 +6614,7 @@
       </c>
       <c r="T6" s="5">
         <f t="shared" si="4"/>
-        <v>0.88000000000000012</v>
+        <v>0.44000000000000006</v>
       </c>
       <c r="U6" s="3">
         <f t="shared" ref="U6:U11" si="10">T6/$T$4</f>
@@ -6622,12 +6622,12 @@
       </c>
       <c r="V6" s="7">
         <f t="shared" si="5"/>
-        <v>2.2727272727272725</v>
+        <v>4.545454545454545</v>
       </c>
       <c r="W6" s="4"/>
       <c r="X6" s="3">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Y6" s="3">
         <f>(C6/20)*IF($AK$14=1,IF(F6="X",1,0.5),1)</f>
@@ -6639,7 +6639,7 @@
       </c>
       <c r="AA6" s="5">
         <f t="shared" si="8"/>
-        <v>0.44000000000000006</v>
+        <v>0.22000000000000003</v>
       </c>
       <c r="AB6" s="3">
         <f t="shared" ref="AB6:AB11" si="11">AA6/$AA$4</f>
@@ -6647,7 +6647,7 @@
       </c>
       <c r="AC6" s="7">
         <f t="shared" si="0"/>
-        <v>4.545454545454545</v>
+        <v>9.0909090909090899</v>
       </c>
       <c r="AD6" s="3">
         <f t="shared" si="9"/>
@@ -6685,7 +6685,7 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="R7" s="3">
         <f t="shared" si="2"/>
@@ -6697,7 +6697,7 @@
       </c>
       <c r="T7" s="5">
         <f t="shared" si="4"/>
-        <v>1.2375</v>
+        <v>0.61875000000000002</v>
       </c>
       <c r="U7" s="3">
         <f t="shared" si="10"/>
@@ -6705,12 +6705,12 @@
       </c>
       <c r="V7" s="7">
         <f t="shared" si="5"/>
-        <v>1.6161616161616161</v>
+        <v>3.2323232323232323</v>
       </c>
       <c r="W7" s="4"/>
       <c r="X7" s="3">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Y7" s="3">
         <f>(C7/20)*IF($AK$14=1,IF(F7="X",1,0.5),1)</f>
@@ -6722,7 +6722,7 @@
       </c>
       <c r="AA7" s="5">
         <f t="shared" si="8"/>
-        <v>0.61875000000000002</v>
+        <v>0.30937500000000001</v>
       </c>
       <c r="AB7" s="3">
         <f t="shared" si="11"/>
@@ -6730,7 +6730,7 @@
       </c>
       <c r="AC7" s="7">
         <f t="shared" si="0"/>
-        <v>3.2323232323232323</v>
+        <v>6.4646464646464645</v>
       </c>
       <c r="AD7" s="3">
         <f t="shared" si="9"/>
@@ -6764,7 +6764,7 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="R8" s="3">
         <f t="shared" si="2"/>
@@ -6776,7 +6776,7 @@
       </c>
       <c r="T8" s="5">
         <f t="shared" si="4"/>
-        <v>0.88000000000000012</v>
+        <v>0.44000000000000006</v>
       </c>
       <c r="U8" s="3">
         <f t="shared" si="10"/>
@@ -6784,12 +6784,12 @@
       </c>
       <c r="V8" s="7">
         <f t="shared" si="5"/>
-        <v>2.2727272727272725</v>
+        <v>4.545454545454545</v>
       </c>
       <c r="W8" s="4"/>
       <c r="X8" s="3">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Y8" s="3">
         <f>(C8/20)*IF($AK$14=1,IF(F8="X",1,0.5),1)</f>
@@ -6801,7 +6801,7 @@
       </c>
       <c r="AA8" s="5">
         <f t="shared" si="8"/>
-        <v>0.88000000000000012</v>
+        <v>0.44000000000000006</v>
       </c>
       <c r="AB8" s="3">
         <f t="shared" si="11"/>
@@ -6809,7 +6809,7 @@
       </c>
       <c r="AC8" s="7">
         <f t="shared" si="0"/>
-        <v>2.2727272727272725</v>
+        <v>4.545454545454545</v>
       </c>
       <c r="AD8" s="3">
         <f t="shared" si="9"/>
@@ -6848,7 +6848,7 @@
       <c r="P9" s="3"/>
       <c r="Q9" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="R9" s="3">
         <f t="shared" ref="R9" si="12">(C9/20)*IF($AJ$6=1,IF(F9="X",1,0.5),1)</f>
@@ -6860,7 +6860,7 @@
       </c>
       <c r="T9" s="5">
         <f t="shared" si="4"/>
-        <v>1.1000000000000001</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U9" s="3">
         <f t="shared" ref="U9" si="14">T9/$T$4</f>
@@ -6868,12 +6868,12 @@
       </c>
       <c r="V9" s="7">
         <f t="shared" ref="V9" si="15">$AJ$3/T9/2</f>
-        <v>1.8181818181818181</v>
+        <v>3.6363636363636362</v>
       </c>
       <c r="W9" s="4"/>
       <c r="X9" s="3">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Y9" s="3">
         <f>(C9/20)*IF($AK$14=1,IF(F9="X",1,0.5),1)</f>
@@ -6885,7 +6885,7 @@
       </c>
       <c r="AA9" s="5">
         <f t="shared" si="8"/>
-        <v>1.1000000000000001</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AB9" s="3">
         <f t="shared" ref="AB9" si="17">AA9/$AA$4</f>
@@ -6893,7 +6893,7 @@
       </c>
       <c r="AC9" s="7">
         <f t="shared" si="0"/>
-        <v>1.8181818181818181</v>
+        <v>3.6363636363636362</v>
       </c>
       <c r="AD9" s="3">
         <f t="shared" ref="AD9" si="18">(U9+AB9)/2</f>
@@ -6933,7 +6933,7 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="R10" s="3">
         <f t="shared" si="2"/>
@@ -6945,7 +6945,7 @@
       </c>
       <c r="T10" s="5">
         <f t="shared" si="4"/>
-        <v>1.3200000000000003</v>
+        <v>0.66000000000000014</v>
       </c>
       <c r="U10" s="3">
         <f t="shared" si="10"/>
@@ -6953,12 +6953,12 @@
       </c>
       <c r="V10" s="7">
         <f t="shared" si="5"/>
-        <v>1.5151515151515149</v>
+        <v>3.0303030303030298</v>
       </c>
       <c r="W10" s="4"/>
       <c r="X10" s="3">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Y10" s="3">
         <f t="shared" ref="Y10:Y11" si="19">(C10/20)*IF($AK$14=1,IF(F10="X",1,0.5),1)</f>
@@ -7018,7 +7018,7 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="R11" s="3">
         <f t="shared" si="2"/>
@@ -7030,7 +7030,7 @@
       </c>
       <c r="T11" s="5">
         <f t="shared" si="4"/>
-        <v>1.6500000000000001</v>
+        <v>0.82500000000000007</v>
       </c>
       <c r="U11" s="3">
         <f t="shared" si="10"/>
@@ -7038,12 +7038,12 @@
       </c>
       <c r="V11" s="7">
         <f t="shared" si="5"/>
-        <v>1.2121212121212119</v>
+        <v>2.4242424242424239</v>
       </c>
       <c r="W11" s="4"/>
       <c r="X11" s="3">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Y11" s="3">
         <f t="shared" si="19"/>
@@ -7103,7 +7103,7 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="R12" s="3">
         <f t="shared" ref="R12" si="20">(C12/20)*IF($AJ$6=1,IF(F12="X",1,0.5),1)</f>
@@ -7115,7 +7115,7 @@
       </c>
       <c r="T12" s="5">
         <f t="shared" si="4"/>
-        <v>1.92</v>
+        <v>0.96</v>
       </c>
       <c r="U12" s="3">
         <f t="shared" ref="U12" si="22">T12/$T$4</f>
@@ -7123,12 +7123,12 @@
       </c>
       <c r="V12" s="7">
         <f t="shared" ref="V12" si="23">$AJ$3/T12/2</f>
-        <v>1.0416666666666667</v>
+        <v>2.0833333333333335</v>
       </c>
       <c r="W12" s="4"/>
       <c r="X12" s="3">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Y12" s="3">
         <f t="shared" ref="Y12" si="24">(C12/20)*IF($AK$14=1,IF(F12="X",1,0.5),1)</f>
@@ -7140,7 +7140,7 @@
       </c>
       <c r="AA12" s="5">
         <f t="shared" si="8"/>
-        <v>0.66</v>
+        <v>0.33</v>
       </c>
       <c r="AB12" s="3">
         <f t="shared" ref="AB12" si="26">AA12/$AA$4</f>
@@ -7148,7 +7148,7 @@
       </c>
       <c r="AC12" s="7">
         <f t="shared" si="0"/>
-        <v>3.0303030303030303</v>
+        <v>6.0606060606060606</v>
       </c>
       <c r="AD12" s="3">
         <f t="shared" ref="AD12" si="27">(U12+AB12)/2</f>
@@ -7235,7 +7235,7 @@
         <v>0.1</v>
       </c>
       <c r="T14" s="28">
-        <f>((1*R14*(Q14)*D14   +   (IF(J14="X",2,1)*S14*D14)      + IF(N14="X",D14*Q14*0.25,0)     ) * IF(M14="X",1.5,1) ) *      IF($AK$6="1",0.5,1)  + 2*(O14/20)</f>
+        <f>((1*R14*(Q14)*D14   +   (IF(J14="X",2,1)*S14*D14)      + IF(N14="X",D14*Q14*0.25,0)     ) * IF(M14="X",1.5,1) ) *      IF($AK$6="1",0.5,1)  + 2*(O14/20)*Q14*R14</f>
         <v>0.60000000000000009</v>
       </c>
       <c r="U14" s="17">
@@ -7260,7 +7260,7 @@
         <v>0.1</v>
       </c>
       <c r="AA14" s="28">
-        <f>IF(G14="X",0,((1*Y14*(X14)*D14   +   (IF(J14="X",2,1)*Z14*D14)      + IF(N14="X",D14*X14*0.25,0)     ) * IF(M14="X",1.5,1) ) *      IF($AJ$13=1,IF(F14="X",1,0.5),1)) + 2*(O14/20)</f>
+        <f>IF(G14="X",0,((1*Y14*(X14)*D14   +   (IF(J14="X",2,1)*Z14*D14)      + IF(N14="X",D14*X14*0.25,0)     ) * IF(M14="X",1.5,1) ) *      IF($AJ$13=1,IF(F14="X",1,0.5),1)) +2*(O14/20)*Q14*R14</f>
         <v>0.30000000000000004</v>
       </c>
       <c r="AB14" s="3">
@@ -7314,7 +7314,7 @@
         <v>0.1</v>
       </c>
       <c r="T15" s="28">
-        <f t="shared" ref="T15:T36" si="35">((1*R15*(Q15)*D15   +   (IF(J15="X",2,1)*S15*D15)      + IF(N15="X",D15*Q15*0.25,0)     ) * IF(M15="X",1.5,1) ) *      IF($AK$6="1",0.5,1)  + 2*(O15/20)</f>
+        <f t="shared" ref="T15:T36" si="35">((1*R15*(Q15)*D15   +   (IF(J15="X",2,1)*S15*D15)      + IF(N15="X",D15*Q15*0.25,0)     ) * IF(M15="X",1.5,1) ) *      IF($AK$6="1",0.5,1)  + 2*(O15/20)*Q15*R15</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="U15" s="17">
@@ -7339,7 +7339,7 @@
         <v>0.1</v>
       </c>
       <c r="AA15" s="28">
-        <f t="shared" ref="AA15:AA36" si="39">IF(G15="X",0,((1*Y15*(X15)*D15   +   (IF(J15="X",2,1)*Z15*D15)      + IF(N15="X",D15*X15*0.25,0)     ) * IF(M15="X",1.5,1) ) *      IF($AJ$13=1,IF(F15="X",1,0.5),1)) + 2*(O15/20)</f>
+        <f t="shared" ref="AA15:AA36" si="39">IF(G15="X",0,((1*Y15*(X15)*D15   +   (IF(J15="X",2,1)*Z15*D15)      + IF(N15="X",D15*X15*0.25,0)     ) * IF(M15="X",1.5,1) ) *      IF($AJ$13=1,IF(F15="X",1,0.5),1)) +2*(O15/20)*Q15*R15</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="AB15" s="3">
@@ -7617,7 +7617,9 @@
       <c r="N19" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="O19" s="1"/>
+      <c r="O19" s="1">
+        <v>10</v>
+      </c>
       <c r="P19" s="1"/>
       <c r="Q19" s="3">
         <f t="shared" si="32"/>
@@ -7633,15 +7635,15 @@
       </c>
       <c r="T19" s="28">
         <f t="shared" si="35"/>
-        <v>0.85000000000000009</v>
+        <v>1.05</v>
       </c>
       <c r="U19" s="17">
         <f t="shared" si="28"/>
-        <v>1.4166666666666665</v>
+        <v>1.7499999999999998</v>
       </c>
       <c r="V19" s="7">
         <f t="shared" si="36"/>
-        <v>2.3529411764705879</v>
+        <v>1.9047619047619047</v>
       </c>
       <c r="W19" s="3"/>
       <c r="X19" s="3">
@@ -7658,19 +7660,19 @@
       </c>
       <c r="AA19" s="28">
         <f t="shared" si="39"/>
-        <v>0.42500000000000004</v>
+        <v>0.625</v>
       </c>
       <c r="AB19" s="3">
         <f t="shared" si="30"/>
-        <v>1.4166666666666665</v>
+        <v>2.083333333333333</v>
       </c>
       <c r="AC19" s="18">
         <f t="shared" si="31"/>
-        <v>4.7058823529411757</v>
+        <v>3.2</v>
       </c>
       <c r="AD19" s="3">
         <f t="shared" si="40"/>
-        <v>1.4166666666666665</v>
+        <v>1.9166666666666665</v>
       </c>
       <c r="AE19" s="17"/>
     </row>
@@ -9023,7 +9025,7 @@
       <c r="P39" s="1"/>
       <c r="Q39" s="3">
         <f>(10+$AG$4-$AJ$5)/20</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="R39" s="3">
         <f>(C39/20)*IF($AJ$6=1,IF(F39="X",1,0.5),1)</f>
@@ -9034,21 +9036,21 @@
         <v>0.1</v>
       </c>
       <c r="T39" s="5">
-        <f>1*R39*Q39*(1+S39)*D39 + IF(N39="X",D39*Q39*0.25,0) + IF(M39="X",D39*Q39*R39*0.5,0) + 2*(O39/20)</f>
-        <v>2.98</v>
+        <f>1*R39*Q39*(1+S39)*D39 + IF(N39="X",D39*Q39*0.25,0) + IF(M39="X",D39*Q39*R39*0.5,0) + 2*(O39/20)*Q39*R39</f>
+        <v>1.29</v>
       </c>
       <c r="U39" s="3">
         <f>T39/$T$4</f>
-        <v>3.3863636363636358</v>
+        <v>2.9318181818181817</v>
       </c>
       <c r="V39" s="7">
         <f>$AJ$3/T39/2</f>
-        <v>0.67114093959731547</v>
+        <v>1.5503875968992247</v>
       </c>
       <c r="W39" s="4"/>
       <c r="X39" s="3">
         <f>(10+$AG$4-$AJ$5)/20</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Y39" s="3">
         <f>(C39/20)</f>
@@ -9059,20 +9061,20 @@
         <v>0.1</v>
       </c>
       <c r="AA39" s="5">
-        <f>IF(G39="X",0,1*Y39*X39*(1+Z39)*D39) * IF($AJ$13=1,IF(F39="X",1,0.5),1) + IF(N39="X",D39*Q39*0.25,0) + 2*(O39/20)</f>
-        <v>1.99</v>
+        <f>IF(G39="X",0,1*Y39*X39*(1+Z39)*D39) * IF($AJ$13=1,IF(F39="X",1,0.5),1) + IF(N39="X",D39*Q39*0.25,0) +  2*(O39/20)*Q39*R39</f>
+        <v>0.79499999999999993</v>
       </c>
       <c r="AB39" s="3">
         <f>AA39/$AA$4</f>
-        <v>4.5227272727272725</v>
+        <v>3.6136363636363629</v>
       </c>
       <c r="AC39" s="7">
         <f t="shared" ref="AC39" si="49">$AJ$9/AA39/2</f>
-        <v>1.0050251256281406</v>
+        <v>2.5157232704402519</v>
       </c>
       <c r="AD39" s="3">
         <f>(U39+AB39)/2</f>
-        <v>3.9545454545454541</v>
+        <v>3.2727272727272725</v>
       </c>
       <c r="AE39" s="17"/>
     </row>
@@ -9467,7 +9469,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V39 AC39">
+  <conditionalFormatting sqref="AC39 V39">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -9479,7 +9481,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB39 U39">
+  <conditionalFormatting sqref="U39 AB39">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -12107,7 +12109,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W30 AD30">
+  <conditionalFormatting sqref="AD30 W30">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -12119,7 +12121,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V30 AC30">
+  <conditionalFormatting sqref="AC30 V30">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -12143,7 +12145,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W34 AD34">
+  <conditionalFormatting sqref="AD34 W34">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -12155,7 +12157,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V34 AC34">
+  <conditionalFormatting sqref="AC34 V34">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -14840,7 +14842,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U31 AB31">
+  <conditionalFormatting sqref="AB31 U31">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -14852,7 +14854,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T31 AA31">
+  <conditionalFormatting sqref="AA31 T31">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -14876,7 +14878,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U35 AB35">
+  <conditionalFormatting sqref="AB35 U35">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -14888,7 +14890,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T35 AA35">
+  <conditionalFormatting sqref="AA35 T35">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0.5"/>

</xml_diff>

<commit_message>
Added "Furious Fists", Balancing
</commit_message>
<xml_diff>
--- a/Balancing Sheet.xlsx
+++ b/Balancing Sheet.xlsx
@@ -3176,7 +3176,7 @@
   <dimension ref="A2:AI66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF6" sqref="AF6"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4394,9 +4394,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="1">
-        <v>0</v>
-      </c>
+      <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -9474,7 +9472,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V39 AC39">
+  <conditionalFormatting sqref="AC39 V39">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -9486,7 +9484,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB39 U39">
+  <conditionalFormatting sqref="U39 AB39">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -12114,7 +12112,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W30 AD30">
+  <conditionalFormatting sqref="AD30 W30">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -12126,7 +12124,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V30 AC30">
+  <conditionalFormatting sqref="AC30 V30">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -12150,7 +12148,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W34 AD34">
+  <conditionalFormatting sqref="AD34 W34">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -12162,7 +12160,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V34 AC34">
+  <conditionalFormatting sqref="AC34 V34">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -14847,7 +14845,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U31 AB31">
+  <conditionalFormatting sqref="AB31 U31">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -14859,7 +14857,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T31 AA31">
+  <conditionalFormatting sqref="AA31 T31">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -14883,7 +14881,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U35 AB35">
+  <conditionalFormatting sqref="AB35 U35">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -14895,7 +14893,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T35 AA35">
+  <conditionalFormatting sqref="AA35 T35">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0.5"/>

</xml_diff>

<commit_message>
New SM Equipment, new Hero, Balancing
New: "Grand Librarian Balthasar", two new equipments and an armor
upgrade
</commit_message>
<xml_diff>
--- a/Balancing Sheet.xlsx
+++ b/Balancing Sheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Space Marines" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="141">
   <si>
     <t>Name</t>
   </si>
@@ -460,6 +460,9 @@
   <si>
     <t>Helbrute</t>
   </si>
+  <si>
+    <t>Heavy Strikes        .</t>
+  </si>
 </sst>
 </file>
 
@@ -619,17 +622,25 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="123">
+  <dxfs count="124">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2692,138 +2703,139 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:AC38" totalsRowShown="0" headerRowDxfId="122" dataDxfId="121" dataCellStyle="Percent">
-  <autoFilter ref="B3:AC38"/>
-  <tableColumns count="28">
-    <tableColumn id="1" name="Name" dataDxfId="120"/>
-    <tableColumn id="2" name="Damage" dataDxfId="119"/>
-    <tableColumn id="3" name="Attacks" dataDxfId="118"/>
-    <tableColumn id="5" name="Note" dataDxfId="117"/>
-    <tableColumn id="6" name="Penetration" dataDxfId="116"/>
-    <tableColumn id="23" name="Light Weapon    ." dataDxfId="115"/>
-    <tableColumn id="24" name="MM      ." dataDxfId="114"/>
-    <tableColumn id="4" name="Crit       ." dataDxfId="113"/>
-    <tableColumn id="26" name="Weak Spots" dataDxfId="112"/>
-    <tableColumn id="25" name="Cone      ." dataDxfId="111"/>
-    <tableColumn id="29" name="No Crits     ." dataDxfId="110"/>
-    <tableColumn id="32" name="Lethal Wounds    ." dataDxfId="109"/>
-    <tableColumn id="27" name="Lethal Weapon    ." dataDxfId="108"/>
-    <tableColumn id="7" name="Column2" dataDxfId="107" dataCellStyle="Percent"/>
-    <tableColumn id="8" name="Hit%" dataDxfId="106" dataCellStyle="Percent"/>
-    <tableColumn id="9" name="Wound%" dataDxfId="105" dataCellStyle="Percent"/>
-    <tableColumn id="11" name="Crit%" dataDxfId="104" dataCellStyle="Percent"/>
-    <tableColumn id="12" name="WoundsÆ" dataDxfId="103" dataCellStyle="Percent"/>
-    <tableColumn id="20" name="% Base" dataDxfId="102" dataCellStyle="Percent"/>
-    <tableColumn id="13" name="To Kill" dataDxfId="101" dataCellStyle="Comma"/>
-    <tableColumn id="14" name="Column3" dataDxfId="100" dataCellStyle="Percent"/>
-    <tableColumn id="15" name="Hit %" dataDxfId="99" dataCellStyle="Percent"/>
-    <tableColumn id="16" name="Wound %" dataDxfId="98" dataCellStyle="Percent"/>
-    <tableColumn id="18" name="Crit %" dataDxfId="97" dataCellStyle="Percent"/>
-    <tableColumn id="19" name="WoundÆ" dataDxfId="96" dataCellStyle="Percent"/>
-    <tableColumn id="21" name="% Base2" dataDxfId="95" dataCellStyle="Percent"/>
-    <tableColumn id="22" name="To Kill2" dataDxfId="94" dataCellStyle="Percent"/>
-    <tableColumn id="10" name="Combo" dataDxfId="93" dataCellStyle="Percent"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:AD38" totalsRowShown="0" headerRowDxfId="123" dataDxfId="122" dataCellStyle="Percent">
+  <autoFilter ref="B3:AD38"/>
+  <tableColumns count="29">
+    <tableColumn id="1" name="Name" dataDxfId="121"/>
+    <tableColumn id="2" name="Damage" dataDxfId="120"/>
+    <tableColumn id="3" name="Attacks" dataDxfId="119"/>
+    <tableColumn id="5" name="Note" dataDxfId="118"/>
+    <tableColumn id="6" name="Penetration" dataDxfId="117"/>
+    <tableColumn id="23" name="Light Weapon    ." dataDxfId="116"/>
+    <tableColumn id="17" name="Heavy Strikes        ." dataDxfId="0"/>
+    <tableColumn id="24" name="MM      ." dataDxfId="115"/>
+    <tableColumn id="4" name="Crit       ." dataDxfId="114"/>
+    <tableColumn id="26" name="Weak Spots" dataDxfId="113"/>
+    <tableColumn id="25" name="Cone      ." dataDxfId="112"/>
+    <tableColumn id="29" name="No Crits     ." dataDxfId="111"/>
+    <tableColumn id="32" name="Lethal Wounds    ." dataDxfId="110"/>
+    <tableColumn id="27" name="Lethal Weapon    ." dataDxfId="109"/>
+    <tableColumn id="7" name="Column2" dataDxfId="108" dataCellStyle="Percent"/>
+    <tableColumn id="8" name="Hit%" dataDxfId="107" dataCellStyle="Percent"/>
+    <tableColumn id="9" name="Wound%" dataDxfId="106" dataCellStyle="Percent"/>
+    <tableColumn id="11" name="Crit%" dataDxfId="105" dataCellStyle="Percent"/>
+    <tableColumn id="12" name="WoundsÆ" dataDxfId="104" dataCellStyle="Percent"/>
+    <tableColumn id="20" name="% Base" dataDxfId="103" dataCellStyle="Percent"/>
+    <tableColumn id="13" name="To Kill" dataDxfId="102" dataCellStyle="Comma"/>
+    <tableColumn id="14" name="Column3" dataDxfId="101" dataCellStyle="Percent"/>
+    <tableColumn id="15" name="Hit %" dataDxfId="100" dataCellStyle="Percent"/>
+    <tableColumn id="16" name="Wound %" dataDxfId="99" dataCellStyle="Percent"/>
+    <tableColumn id="18" name="Crit %" dataDxfId="98" dataCellStyle="Percent"/>
+    <tableColumn id="19" name="WoundÆ" dataDxfId="97" dataCellStyle="Percent"/>
+    <tableColumn id="21" name="% Base2" dataDxfId="96" dataCellStyle="Percent"/>
+    <tableColumn id="22" name="To Kill2" dataDxfId="95" dataCellStyle="Percent"/>
+    <tableColumn id="10" name="Combo" dataDxfId="94" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table16" displayName="Table16" ref="B3:AD40" totalsRowShown="0" headerRowDxfId="92" dataDxfId="91" dataCellStyle="Percent">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table16" displayName="Table16" ref="B3:AD40" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92" dataCellStyle="Percent">
   <autoFilter ref="B3:AD40"/>
   <tableColumns count="29">
-    <tableColumn id="1" name="Name" dataDxfId="90"/>
-    <tableColumn id="2" name="Damage" dataDxfId="89"/>
-    <tableColumn id="3" name="Attacks" dataDxfId="88"/>
-    <tableColumn id="5" name="Note" dataDxfId="87"/>
-    <tableColumn id="6" name="Penetration" dataDxfId="86"/>
-    <tableColumn id="23" name="Light Weapon    ." dataDxfId="85"/>
-    <tableColumn id="24" name="MM      ." dataDxfId="84"/>
-    <tableColumn id="4" name="Crit       ." dataDxfId="83"/>
-    <tableColumn id="26" name="Weak Spots" dataDxfId="82"/>
-    <tableColumn id="25" name="Cone      ." dataDxfId="81"/>
-    <tableColumn id="29" name="No Crits     ." dataDxfId="80"/>
-    <tableColumn id="32" name="Lethal Wounds    ." dataDxfId="79"/>
-    <tableColumn id="27" name="Lethal Weapon    ." dataDxfId="78"/>
-    <tableColumn id="17" name="Rend       ." dataDxfId="77"/>
-    <tableColumn id="7" name="Column2" dataDxfId="76" dataCellStyle="Percent"/>
-    <tableColumn id="8" name="Hit%" dataDxfId="75" dataCellStyle="Percent"/>
-    <tableColumn id="9" name="Wound%" dataDxfId="74" dataCellStyle="Percent"/>
-    <tableColumn id="11" name="Crit%" dataDxfId="73" dataCellStyle="Percent"/>
-    <tableColumn id="12" name="WoundsÆ" dataDxfId="72" dataCellStyle="Percent"/>
-    <tableColumn id="20" name="% Base" dataDxfId="71" dataCellStyle="Percent"/>
-    <tableColumn id="13" name="To Kill" dataDxfId="70" dataCellStyle="Comma"/>
-    <tableColumn id="14" name="Column3" dataDxfId="69" dataCellStyle="Percent"/>
-    <tableColumn id="15" name="Hit %" dataDxfId="68" dataCellStyle="Percent"/>
-    <tableColumn id="16" name="Wound %" dataDxfId="67" dataCellStyle="Percent"/>
-    <tableColumn id="18" name="Crit %" dataDxfId="66" dataCellStyle="Percent"/>
-    <tableColumn id="19" name="WoundÆ" dataDxfId="65" dataCellStyle="Percent"/>
-    <tableColumn id="21" name="% Base2" dataDxfId="64" dataCellStyle="Percent"/>
-    <tableColumn id="22" name="To Kill2" dataDxfId="63" dataCellStyle="Percent"/>
-    <tableColumn id="10" name="Combo" dataDxfId="62" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="Name" dataDxfId="91"/>
+    <tableColumn id="2" name="Damage" dataDxfId="90"/>
+    <tableColumn id="3" name="Attacks" dataDxfId="89"/>
+    <tableColumn id="5" name="Note" dataDxfId="88"/>
+    <tableColumn id="6" name="Penetration" dataDxfId="87"/>
+    <tableColumn id="23" name="Light Weapon    ." dataDxfId="86"/>
+    <tableColumn id="24" name="MM      ." dataDxfId="85"/>
+    <tableColumn id="4" name="Crit       ." dataDxfId="84"/>
+    <tableColumn id="26" name="Weak Spots" dataDxfId="83"/>
+    <tableColumn id="25" name="Cone      ." dataDxfId="82"/>
+    <tableColumn id="29" name="No Crits     ." dataDxfId="81"/>
+    <tableColumn id="32" name="Lethal Wounds    ." dataDxfId="80"/>
+    <tableColumn id="27" name="Lethal Weapon    ." dataDxfId="79"/>
+    <tableColumn id="17" name="Rend       ." dataDxfId="78"/>
+    <tableColumn id="7" name="Column2" dataDxfId="77" dataCellStyle="Percent"/>
+    <tableColumn id="8" name="Hit%" dataDxfId="76" dataCellStyle="Percent"/>
+    <tableColumn id="9" name="Wound%" dataDxfId="75" dataCellStyle="Percent"/>
+    <tableColumn id="11" name="Crit%" dataDxfId="74" dataCellStyle="Percent"/>
+    <tableColumn id="12" name="WoundsÆ" dataDxfId="73" dataCellStyle="Percent"/>
+    <tableColumn id="20" name="% Base" dataDxfId="72" dataCellStyle="Percent"/>
+    <tableColumn id="13" name="To Kill" dataDxfId="71" dataCellStyle="Comma"/>
+    <tableColumn id="14" name="Column3" dataDxfId="70" dataCellStyle="Percent"/>
+    <tableColumn id="15" name="Hit %" dataDxfId="69" dataCellStyle="Percent"/>
+    <tableColumn id="16" name="Wound %" dataDxfId="68" dataCellStyle="Percent"/>
+    <tableColumn id="18" name="Crit %" dataDxfId="67" dataCellStyle="Percent"/>
+    <tableColumn id="19" name="WoundÆ" dataDxfId="66" dataCellStyle="Percent"/>
+    <tableColumn id="21" name="% Base2" dataDxfId="65" dataCellStyle="Percent"/>
+    <tableColumn id="22" name="To Kill2" dataDxfId="64" dataCellStyle="Percent"/>
+    <tableColumn id="10" name="Combo" dataDxfId="63" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="B3:AE35" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60" dataCellStyle="Percent">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="B3:AE35" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61" dataCellStyle="Percent">
   <autoFilter ref="B3:AE35"/>
   <tableColumns count="30">
-    <tableColumn id="1" name="Name" dataDxfId="59"/>
-    <tableColumn id="2" name="Damage" dataDxfId="58"/>
-    <tableColumn id="3" name="Attacks" dataDxfId="57"/>
-    <tableColumn id="5" name="Note" dataDxfId="56"/>
-    <tableColumn id="6" name="Penetration" dataDxfId="55"/>
-    <tableColumn id="30" name="Light Weapon    ." dataDxfId="54"/>
-    <tableColumn id="23" name="MM      ." dataDxfId="53"/>
-    <tableColumn id="24" name="Crit       ." dataDxfId="52"/>
-    <tableColumn id="26" name="Weak Spots" dataDxfId="51"/>
-    <tableColumn id="25" name="Cone      ." dataDxfId="50"/>
-    <tableColumn id="29" name="No Crits     ." dataDxfId="49"/>
-    <tableColumn id="32" name="2H        ." dataDxfId="48"/>
-    <tableColumn id="33" name="Heavy Strikes      ." dataDxfId="47"/>
-    <tableColumn id="4" name="Lethal Wounds    ." dataDxfId="46"/>
-    <tableColumn id="28" name="Lethal Weapon    ." dataDxfId="45"/>
-    <tableColumn id="27" name="Column2" dataDxfId="44"/>
-    <tableColumn id="7" name="Hit%" dataDxfId="43" dataCellStyle="Percent">
+    <tableColumn id="1" name="Name" dataDxfId="60"/>
+    <tableColumn id="2" name="Damage" dataDxfId="59"/>
+    <tableColumn id="3" name="Attacks" dataDxfId="58"/>
+    <tableColumn id="5" name="Note" dataDxfId="57"/>
+    <tableColumn id="6" name="Penetration" dataDxfId="56"/>
+    <tableColumn id="30" name="Light Weapon    ." dataDxfId="55"/>
+    <tableColumn id="23" name="MM      ." dataDxfId="54"/>
+    <tableColumn id="24" name="Crit       ." dataDxfId="53"/>
+    <tableColumn id="26" name="Weak Spots" dataDxfId="52"/>
+    <tableColumn id="25" name="Cone      ." dataDxfId="51"/>
+    <tableColumn id="29" name="No Crits     ." dataDxfId="50"/>
+    <tableColumn id="32" name="2H        ." dataDxfId="49"/>
+    <tableColumn id="33" name="Heavy Strikes      ." dataDxfId="48"/>
+    <tableColumn id="4" name="Lethal Wounds    ." dataDxfId="47"/>
+    <tableColumn id="28" name="Lethal Weapon    ." dataDxfId="46"/>
+    <tableColumn id="27" name="Column2" dataDxfId="45"/>
+    <tableColumn id="7" name="Hit%" dataDxfId="44" dataCellStyle="Percent">
       <calculatedColumnFormula>($AH$3 )/20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Wound%" dataDxfId="42" dataCellStyle="Percent">
+    <tableColumn id="8" name="Wound%" dataDxfId="43" dataCellStyle="Percent">
       <calculatedColumnFormula>(C4/20)*IF($AK$6=1,0.5,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Crit%" dataDxfId="41" dataCellStyle="Percent">
+    <tableColumn id="9" name="Crit%" dataDxfId="42" dataCellStyle="Percent">
       <calculatedColumnFormula>(IF(( L4="X"),0,($AH$5+I4))/20)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="WoundsÆ" dataDxfId="40">
+    <tableColumn id="11" name="WoundsÆ" dataDxfId="41">
       <calculatedColumnFormula>1*S4*(R4)*(1+T4)*D4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="% Base" dataDxfId="39" dataCellStyle="Percent">
+    <tableColumn id="12" name="% Base" dataDxfId="40" dataCellStyle="Percent">
       <calculatedColumnFormula>U4/$U$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="To Kill" dataDxfId="38" dataCellStyle="Percent">
+    <tableColumn id="20" name="To Kill" dataDxfId="39" dataCellStyle="Percent">
       <calculatedColumnFormula>AK9/Table145[[#This Row],[WoundsÆ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Column3" dataDxfId="37"/>
-    <tableColumn id="14" name="Hit %" dataDxfId="36" dataCellStyle="Percent">
+    <tableColumn id="13" name="Column3" dataDxfId="38"/>
+    <tableColumn id="14" name="Hit %" dataDxfId="37" dataCellStyle="Percent">
       <calculatedColumnFormula>($AH$3)/20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Wound %" dataDxfId="35" dataCellStyle="Percent">
+    <tableColumn id="15" name="Wound %" dataDxfId="36" dataCellStyle="Percent">
       <calculatedColumnFormula>(C4/20)*IF($AK$6=1,IF(F4="X",1,0.5),1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Crit %" dataDxfId="34" dataCellStyle="Percent">
+    <tableColumn id="16" name="Crit %" dataDxfId="35" dataCellStyle="Percent">
       <calculatedColumnFormula>($AH$5/20)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="WoundÆ" dataDxfId="33">
+    <tableColumn id="18" name="WoundÆ" dataDxfId="34">
       <calculatedColumnFormula>1*Z4*(Y4)*(1+AA4)*D4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="% Base2" dataDxfId="32" dataCellStyle="Percent">
+    <tableColumn id="19" name="% Base2" dataDxfId="33" dataCellStyle="Percent">
       <calculatedColumnFormula>AB4/$AB$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="To Kill2" dataDxfId="31" dataCellStyle="Percent">
+    <tableColumn id="21" name="To Kill2" dataDxfId="32" dataCellStyle="Percent">
       <calculatedColumnFormula>$AK$9/Table145[[#This Row],[WoundÆ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="Combo" dataDxfId="30" dataCellStyle="Percent">
+    <tableColumn id="22" name="Combo" dataDxfId="31" dataCellStyle="Percent">
       <calculatedColumnFormula>(Table145[[#This Row],[% Base]]+Table145[[#This Row],[% Base2]])/2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2832,61 +2844,61 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table1453" displayName="Table1453" ref="B3:AC36" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" dataCellStyle="Percent">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table1453" displayName="Table1453" ref="B3:AC36" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" dataCellStyle="Percent">
   <autoFilter ref="B3:AC36"/>
   <tableColumns count="28">
-    <tableColumn id="1" name="Name" dataDxfId="27"/>
-    <tableColumn id="2" name="Damage" dataDxfId="26"/>
-    <tableColumn id="3" name="Attacks" dataDxfId="25"/>
-    <tableColumn id="5" name="Note" dataDxfId="24"/>
-    <tableColumn id="6" name="Penetration" dataDxfId="23"/>
-    <tableColumn id="30" name="Light Weapon    ." dataDxfId="22"/>
-    <tableColumn id="23" name="MM      ." dataDxfId="21"/>
-    <tableColumn id="24" name="Crit       ." dataDxfId="20"/>
-    <tableColumn id="26" name="Weak Spots" dataDxfId="19"/>
-    <tableColumn id="25" name="Cone      ." dataDxfId="18"/>
-    <tableColumn id="29" name="No Crits     ." dataDxfId="17"/>
-    <tableColumn id="4" name="Lethal Wounds    ." dataDxfId="16"/>
-    <tableColumn id="28" name="Lethal Weapon    ." dataDxfId="15"/>
-    <tableColumn id="27" name="Column2" dataDxfId="14"/>
-    <tableColumn id="7" name="Hit%" dataDxfId="13" dataCellStyle="Percent">
+    <tableColumn id="1" name="Name" dataDxfId="28"/>
+    <tableColumn id="2" name="Damage" dataDxfId="27"/>
+    <tableColumn id="3" name="Attacks" dataDxfId="26"/>
+    <tableColumn id="5" name="Note" dataDxfId="25"/>
+    <tableColumn id="6" name="Penetration" dataDxfId="24"/>
+    <tableColumn id="30" name="Light Weapon    ." dataDxfId="23"/>
+    <tableColumn id="23" name="MM      ." dataDxfId="22"/>
+    <tableColumn id="24" name="Crit       ." dataDxfId="21"/>
+    <tableColumn id="26" name="Weak Spots" dataDxfId="20"/>
+    <tableColumn id="25" name="Cone      ." dataDxfId="19"/>
+    <tableColumn id="29" name="No Crits     ." dataDxfId="18"/>
+    <tableColumn id="4" name="Lethal Wounds    ." dataDxfId="17"/>
+    <tableColumn id="28" name="Lethal Weapon    ." dataDxfId="16"/>
+    <tableColumn id="27" name="Column2" dataDxfId="15"/>
+    <tableColumn id="7" name="Hit%" dataDxfId="14" dataCellStyle="Percent">
       <calculatedColumnFormula>($AF$3 )/20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Wound%" dataDxfId="12" dataCellStyle="Percent">
+    <tableColumn id="8" name="Wound%" dataDxfId="13" dataCellStyle="Percent">
       <calculatedColumnFormula>(C4/20)*IF($AI$6=1,0.5,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Crit%" dataDxfId="11" dataCellStyle="Percent">
+    <tableColumn id="9" name="Crit%" dataDxfId="12" dataCellStyle="Percent">
       <calculatedColumnFormula>(IF(( L4="X"),0,($AF$5+I4))/20)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="WoundsÆ" dataDxfId="10">
+    <tableColumn id="11" name="WoundsÆ" dataDxfId="11">
       <calculatedColumnFormula>1*Q4*(P4)*(1+R4)*D4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="% Base" dataDxfId="9" dataCellStyle="Percent">
+    <tableColumn id="12" name="% Base" dataDxfId="10" dataCellStyle="Percent">
       <calculatedColumnFormula>S4/$S$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="To Kill" dataDxfId="8" dataCellStyle="Percent">
+    <tableColumn id="20" name="To Kill" dataDxfId="9" dataCellStyle="Percent">
       <calculatedColumnFormula>AI10/Table1453[[#This Row],[WoundsÆ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Column3" dataDxfId="7"/>
-    <tableColumn id="14" name="Hit %" dataDxfId="6" dataCellStyle="Percent">
+    <tableColumn id="13" name="Column3" dataDxfId="8"/>
+    <tableColumn id="14" name="Hit %" dataDxfId="7" dataCellStyle="Percent">
       <calculatedColumnFormula>($AF$3)/20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Wound %" dataDxfId="5" dataCellStyle="Percent">
+    <tableColumn id="15" name="Wound %" dataDxfId="6" dataCellStyle="Percent">
       <calculatedColumnFormula>(C4/20)*IF($AI$6=1,IF(F4="X",1,0.5),1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Crit %" dataDxfId="4" dataCellStyle="Percent">
+    <tableColumn id="16" name="Crit %" dataDxfId="5" dataCellStyle="Percent">
       <calculatedColumnFormula>($AF$5/20)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="WoundÆ" dataDxfId="3">
+    <tableColumn id="18" name="WoundÆ" dataDxfId="4">
       <calculatedColumnFormula>1*X4*(W4)*(1+Y4)*D4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="% Base2" dataDxfId="2" dataCellStyle="Percent">
+    <tableColumn id="19" name="% Base2" dataDxfId="3" dataCellStyle="Percent">
       <calculatedColumnFormula>Z4/$Z$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="To Kill2" dataDxfId="1" dataCellStyle="Percent">
+    <tableColumn id="21" name="To Kill2" dataDxfId="2" dataCellStyle="Percent">
       <calculatedColumnFormula>$AI$10/Table1453[[#This Row],[WoundÆ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="Combo" dataDxfId="0" dataCellStyle="Percent">
+    <tableColumn id="22" name="Combo" dataDxfId="1" dataCellStyle="Percent">
       <calculatedColumnFormula>(Table1453[[#This Row],[% Base]]+Table1453[[#This Row],[% Base2]])/2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3191,10 +3203,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AI66"/>
+  <dimension ref="A2:AJ66"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3203,38 +3215,38 @@
     <col min="3" max="3" width="6.7109375" customWidth="1"/>
     <col min="4" max="4" width="7.140625" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="14" width="3.42578125" customWidth="1"/>
+    <col min="6" max="15" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B2" s="30" t="s">
+    <row r="2" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="P2" s="30" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="Q2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="W2" s="30" t="s">
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="X2" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="X2" s="30"/>
-      <c r="Y2" s="30"/>
-      <c r="Z2" s="30"/>
-      <c r="AA2" s="25"/>
+      <c r="Y2" s="31"/>
+      <c r="Z2" s="31"/>
+      <c r="AA2" s="31"/>
       <c r="AB2" s="25"/>
-      <c r="AE2" t="s">
+      <c r="AC2" s="25"/>
+      <c r="AF2" t="s">
         <v>8</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:35" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:36" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
@@ -3254,86 +3266,89 @@
         <v>104</v>
       </c>
       <c r="H3" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="K3" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="L3" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="M3" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="N3" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="O3" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="P3" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="Q3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="R3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="T3" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="U3" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="V3" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="W3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="X3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="X3" s="6" t="s">
+      <c r="Y3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="Y3" s="6" t="s">
+      <c r="Z3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Z3" s="6" t="s">
+      <c r="AA3" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="AA3" s="6" t="s">
+      <c r="AB3" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AB3" s="6" t="s">
+      <c r="AC3" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="AC3" s="6" t="s">
+      <c r="AD3" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AD3" s="6"/>
-      <c r="AE3" t="s">
+      <c r="AE3" s="6"/>
+      <c r="AF3" t="s">
         <v>10</v>
       </c>
-      <c r="AF3">
+      <c r="AG3">
         <v>10</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AI3" t="s">
         <v>10</v>
       </c>
-      <c r="AI3">
+      <c r="AJ3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
@@ -3354,74 +3369,75 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-      <c r="P4" s="3">
-        <f>(10+$AF$4-$AI$5)/20</f>
-        <v>0.5</v>
-      </c>
+      <c r="P4" s="1"/>
       <c r="Q4" s="3">
-        <f>(C4/20)*IF($AI$6=1,IF(F4="X",1,0.5),1)</f>
+        <f>(10+$AG$4-$AJ$5+IF(H4="X",5,0))/20</f>
         <v>0.5</v>
       </c>
       <c r="R4" s="3">
-        <f>(IF(( L4="X"),0,($AF$5+I4))/20)</f>
-        <v>0.1</v>
-      </c>
-      <c r="S4" s="5">
-        <f>1*Q4*P4*(1+R4)*D4 + IF(N4="X",D4*P4*0.25,0) + IF(M4="X",D4*P4*Q4*0.5,0)</f>
+        <f>(C4/20)*IF($AJ$6=1,IF(F4="X",1,0.5),1)</f>
+        <v>0.5</v>
+      </c>
+      <c r="S4" s="3">
+        <f>(IF(( M4="X"),0,($AG$5+J4))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="T4" s="5">
+        <f>1*R4*Q4*(1+S4)*D4 + IF(O4="X",D4*Q4*0.25,0) + IF(N4="X",D4*Q4*R4*0.5,0)</f>
         <v>0.55000000000000004</v>
       </c>
-      <c r="T4" s="3">
-        <f>S4/$S$4</f>
+      <c r="U4" s="3">
+        <f>T4/$T$4</f>
         <v>1</v>
       </c>
-      <c r="U4" s="7">
-        <f>$AI$3/S4/2</f>
+      <c r="V4" s="7">
+        <f>$AJ$3/T4/2</f>
         <v>3.6363636363636362</v>
       </c>
-      <c r="V4" s="4"/>
-      <c r="W4" s="3">
-        <f>(10+$AF$4-$AI$5)/20</f>
-        <v>0.5</v>
-      </c>
+      <c r="W4" s="4"/>
       <c r="X4" s="3">
+        <f>(10+$AG$4-$AJ$5+IF(H4="X",5,0))/20</f>
+        <v>0.5</v>
+      </c>
+      <c r="Y4" s="3">
         <f>(C4/20)</f>
         <v>0.5</v>
       </c>
-      <c r="Y4" s="3">
-        <f>(IF((OR(K4="X", L4="X")),0,($AF$5+I4))/20)</f>
-        <v>0.1</v>
-      </c>
-      <c r="Z4" s="5">
-        <f>IF(G4="X",0,1*X4*W4*(1+Y4)*D4) * IF($AI$13=1,IF(F4="X",1,0.5),1) + IF(N4="X",D4*P4*0.25,0)</f>
+      <c r="Z4" s="3">
+        <f>(IF((OR(L4="X", M4="X")),0,($AG$5+J4))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="AA4" s="5">
+        <f>IF(G4="X",0,1*Y4*X4*(1+Z4)*D4) * IF($AJ$13=1,IF(F4="X",1,0.5),1) + IF(O4="X",D4*Q4*0.25,0)</f>
         <v>0.27500000000000002</v>
       </c>
-      <c r="AA4" s="3">
-        <f>Z4/$Z$4</f>
+      <c r="AB4" s="3">
+        <f>AA4/$AA$4</f>
         <v>1</v>
       </c>
-      <c r="AB4" s="7">
-        <f>$AI$9/Z4/2</f>
+      <c r="AC4" s="7">
+        <f>$AJ$9/AA4/2</f>
         <v>7.2727272727272725</v>
       </c>
-      <c r="AC4" s="3">
-        <f>(T4+AA4)/2</f>
+      <c r="AD4" s="3">
+        <f>(U4+AB4)/2</f>
         <v>1</v>
       </c>
-      <c r="AD4" s="3"/>
-      <c r="AE4" t="s">
+      <c r="AE4" s="3"/>
+      <c r="AF4" t="s">
         <v>85</v>
       </c>
-      <c r="AF4">
+      <c r="AG4">
         <v>10</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AI4" t="s">
         <v>85</v>
       </c>
-      <c r="AI4">
+      <c r="AJ4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
@@ -3444,79 +3460,80 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
-      <c r="P5" s="3">
-        <f t="shared" ref="P5:P10" si="0">(10+$AF$4-$AI$5)/20</f>
-        <v>0.5</v>
-      </c>
+      <c r="P5" s="1"/>
       <c r="Q5" s="3">
-        <f t="shared" ref="Q5:Q10" si="1">(C5/20)*IF($AI$6=1,IF(F5="X",1,0.5),1)</f>
+        <f t="shared" ref="Q5:Q10" si="0">(10+$AG$4-$AJ$5+IF(H5="X",5,0))/20</f>
         <v>0.5</v>
       </c>
       <c r="R5" s="3">
-        <f t="shared" ref="R5:R35" si="2">(IF(( L5="X"),0,($AF$5+I5))/20)</f>
-        <v>0.1</v>
-      </c>
-      <c r="S5" s="5">
-        <f>1*Q5*P5*(1+R5)*D5 + IF(N5="X",D5*P5*0.25,0) + IF(M5="X",D5*P5*Q5*0.5,0)</f>
+        <f t="shared" ref="R5:R10" si="1">(C5/20)*IF($AJ$6=1,IF(F5="X",1,0.5),1)</f>
+        <v>0.5</v>
+      </c>
+      <c r="S5" s="3">
+        <f t="shared" ref="S5:S35" si="2">(IF(( M5="X"),0,($AG$5+J5))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="T5" s="5">
+        <f>1*R5*Q5*(1+S5)*D5 + IF(O5="X",D5*Q5*0.25,0) + IF(N5="X",D5*Q5*R5*0.5,0)</f>
         <v>0.55000000000000004</v>
       </c>
-      <c r="T5" s="3">
-        <f>S5/$S$4</f>
+      <c r="U5" s="3">
+        <f>T5/$T$4</f>
         <v>1</v>
       </c>
-      <c r="U5" s="7">
-        <f t="shared" ref="U5:U25" si="3">$AI$3/S5/2</f>
+      <c r="V5" s="7">
+        <f t="shared" ref="V5:V25" si="3">$AJ$3/T5/2</f>
         <v>3.6363636363636362</v>
       </c>
-      <c r="V5" s="4"/>
-      <c r="W5" s="3">
-        <f t="shared" ref="W5:W10" si="4">(10+$AF$4-$AI$5)/20</f>
-        <v>0.5</v>
-      </c>
+      <c r="W5" s="4"/>
       <c r="X5" s="3">
-        <f>(C5/20)*IF($AJ$13=1,IF(F5="X",1,0.5),1)</f>
+        <f t="shared" ref="X5:X10" si="4">(10+$AG$4-$AJ$5+IF(H5="X",5,0))/20</f>
         <v>0.5</v>
       </c>
       <c r="Y5" s="3">
-        <f t="shared" ref="Y5:Y35" si="5">(IF((OR(K5="X", L5="X")),0,($AF$5+I5))/20)</f>
-        <v>0.1</v>
-      </c>
-      <c r="Z5" s="5">
-        <f t="shared" ref="Z5:Z10" si="6">IF(G5="X",0,1*X5*W5*(1+Y5)*D5) * IF($AI$13=1,IF(F5="X",1,0.5),1) + IF(N5="X",D5*P5*0.25,0)</f>
+        <f>(C5/20)*IF($AK$13=1,IF(F5="X",1,0.5),1)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Z5" s="3">
+        <f t="shared" ref="Z5:Z35" si="5">(IF((OR(L5="X", M5="X")),0,($AG$5+J5))/20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="AA5" s="5">
+        <f t="shared" ref="AA5:AA10" si="6">IF(G5="X",0,1*Y5*X5*(1+Z5)*D5) * IF($AJ$13=1,IF(F5="X",1,0.5),1) + IF(O5="X",D5*Q5*0.25,0)</f>
         <v>0.27500000000000002</v>
       </c>
-      <c r="AA5" s="3">
-        <f>Z5/$Z$4</f>
+      <c r="AB5" s="3">
+        <f>AA5/$AA$4</f>
         <v>1</v>
       </c>
-      <c r="AB5" s="7">
-        <f t="shared" ref="AB5:AB16" si="7">$AI$9/Z5/2</f>
+      <c r="AC5" s="7">
+        <f t="shared" ref="AC5:AC16" si="7">$AJ$9/AA5/2</f>
         <v>7.2727272727272725</v>
       </c>
-      <c r="AC5" s="3">
-        <f t="shared" ref="AC5:AC35" si="8">(T5+AA5)/2</f>
+      <c r="AD5" s="3">
+        <f t="shared" ref="AD5:AD35" si="8">(U5+AB5)/2</f>
         <v>1</v>
       </c>
-      <c r="AD5" s="3"/>
-      <c r="AE5" t="s">
+      <c r="AE5" s="3"/>
+      <c r="AF5" t="s">
         <v>18</v>
       </c>
-      <c r="AF5">
+      <c r="AG5">
         <v>2</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AI5" t="s">
         <v>86</v>
       </c>
-      <c r="AI5">
+      <c r="AJ5">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C6" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1">
         <v>3</v>
@@ -3534,73 +3551,74 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="3">
+      <c r="P6" s="1"/>
+      <c r="Q6" s="3">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="R6" s="3">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="R6" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="S6" s="3">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="S6" s="5">
-        <f t="shared" ref="S6:S8" si="9">1*Q6*P6*(1+R6)*D6 + IF(N6="X",D6*P6*0.25,0) + IF(M6="X",D6*P6*Q6*0.5,0)</f>
-        <v>0.82500000000000007</v>
-      </c>
-      <c r="T6" s="3">
-        <f t="shared" ref="T6:T8" si="10">S6/$S$4</f>
-        <v>1.5</v>
-      </c>
-      <c r="U6" s="7">
+      <c r="T6" s="5">
+        <f t="shared" ref="T6:T8" si="9">1*R6*Q6*(1+S6)*D6 + IF(O6="X",D6*Q6*0.25,0) + IF(N6="X",D6*Q6*R6*0.5,0)</f>
+        <v>0.66000000000000014</v>
+      </c>
+      <c r="U6" s="3">
+        <f t="shared" ref="U6:U8" si="10">T6/$T$4</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="V6" s="7">
         <f t="shared" si="3"/>
-        <v>2.4242424242424239</v>
-      </c>
-      <c r="V6" s="4"/>
-      <c r="W6" s="3">
+        <v>3.0303030303030298</v>
+      </c>
+      <c r="W6" s="4"/>
+      <c r="X6" s="3">
         <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
-      <c r="X6" s="3">
-        <f>(C6/20)*IF($AJ$13=1,IF(F6="X",1,0.5),1)</f>
-        <v>0.5</v>
-      </c>
       <c r="Y6" s="3">
+        <f>(C6/20)*IF($AK$13=1,IF(F6="X",1,0.5),1)</f>
+        <v>0.4</v>
+      </c>
+      <c r="Z6" s="3">
         <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
-      <c r="Z6" s="5">
+      <c r="AA6" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AA6" s="3">
-        <f t="shared" ref="AA6:AA8" si="11">Z6/$Z$4</f>
+      <c r="AB6" s="3">
+        <f t="shared" ref="AB6:AB8" si="11">AA6/$AA$4</f>
         <v>0</v>
       </c>
-      <c r="AB6" s="7" t="e">
+      <c r="AC6" s="7" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AC6" s="3">
+      <c r="AD6" s="3">
         <f t="shared" si="8"/>
-        <v>0.75</v>
-      </c>
-      <c r="AD6" s="3"/>
-      <c r="AH6" t="s">
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AE6" s="3"/>
+      <c r="AI6" t="s">
         <v>87</v>
       </c>
-      <c r="AI6">
+      <c r="AJ6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1">
         <v>2</v>
@@ -3618,67 +3636,68 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
-      <c r="P7" s="3">
+      <c r="P7" s="1"/>
+      <c r="Q7" s="3">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="Q7" s="3">
+      <c r="R7" s="3">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="R7" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="S7" s="3">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="S7" s="5">
+      <c r="T7" s="5">
         <f t="shared" si="9"/>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="T7" s="3">
+        <v>0.66</v>
+      </c>
+      <c r="U7" s="3">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="U7" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="V7" s="7">
         <f t="shared" si="3"/>
-        <v>3.6363636363636362</v>
-      </c>
-      <c r="V7" s="4"/>
-      <c r="W7" s="3">
+        <v>3.0303030303030303</v>
+      </c>
+      <c r="W7" s="4"/>
+      <c r="X7" s="3">
         <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
-      <c r="X7" s="3">
-        <f>(C7/20)*IF($AJ$13=1,IF(F7="X",1,0.5),1)</f>
-        <v>0.5</v>
-      </c>
       <c r="Y7" s="3">
+        <f>(C7/20)*IF($AK$13=1,IF(F7="X",1,0.5),1)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Z7" s="3">
         <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
-      <c r="Z7" s="5">
+      <c r="AA7" s="5">
         <f t="shared" si="6"/>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="AA7" s="3">
+        <v>0.66</v>
+      </c>
+      <c r="AB7" s="3">
         <f t="shared" si="11"/>
-        <v>2</v>
-      </c>
-      <c r="AB7" s="7">
+        <v>2.4</v>
+      </c>
+      <c r="AC7" s="7">
         <f t="shared" si="7"/>
-        <v>3.6363636363636362</v>
-      </c>
-      <c r="AC7" s="3">
+        <v>3.0303030303030303</v>
+      </c>
+      <c r="AD7" s="3">
         <f t="shared" si="8"/>
-        <v>1.5</v>
-      </c>
-      <c r="AD7" s="3"/>
-    </row>
-    <row r="8" spans="2:35" x14ac:dyDescent="0.25">
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="AE7" s="3"/>
+    </row>
+    <row r="8" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D8" s="1">
         <v>2</v>
@@ -3696,78 +3715,83 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="P8" s="3">
+      <c r="P8" s="1"/>
+      <c r="Q8" s="3">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="Q8" s="3">
+      <c r="R8" s="3">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="R8" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="S8" s="3">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="S8" s="5">
+      <c r="T8" s="5">
         <f t="shared" si="9"/>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="T8" s="3">
+        <v>0.66</v>
+      </c>
+      <c r="U8" s="3">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="U8" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="V8" s="7">
         <f t="shared" si="3"/>
-        <v>3.6363636363636362</v>
-      </c>
-      <c r="V8" s="4"/>
-      <c r="W8" s="3">
+        <v>3.0303030303030303</v>
+      </c>
+      <c r="W8" s="4"/>
+      <c r="X8" s="3">
         <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
-      <c r="X8" s="3">
-        <f>(C8/20)*IF($AJ$13=1,IF(F8="X",1,0.5),1)</f>
-        <v>0.5</v>
-      </c>
       <c r="Y8" s="3">
+        <f>(C8/20)*IF($AK$13=1,IF(F8="X",1,0.5),1)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Z8" s="3">
         <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
-      <c r="Z8" s="5">
+      <c r="AA8" s="5">
         <f t="shared" si="6"/>
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="AA8" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="AB8" s="3">
         <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="AB8" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="AC8" s="7">
         <f t="shared" si="7"/>
-        <v>7.2727272727272725</v>
-      </c>
-      <c r="AC8" s="3">
+        <v>6.0606060606060606</v>
+      </c>
+      <c r="AD8" s="3">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="AD8" s="3"/>
-      <c r="AH8" t="s">
+        <v>1.2</v>
+      </c>
+      <c r="AE8" s="3"/>
+      <c r="AI8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="1">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D9" s="1">
         <v>1.5</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -3775,68 +3799,69 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
-      <c r="P9" s="3">
+      <c r="P9" s="1"/>
+      <c r="Q9" s="3">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="Q9" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="R9" s="3">
         <f t="shared" si="1"/>
+        <v>0.6</v>
+      </c>
+      <c r="S9" s="3">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="T9" s="5">
+        <f t="shared" ref="T9:T10" si="12">1*R9*Q9*(1+S9)*D9 + IF(O9="X",D9*Q9*0.25,0) + IF(N9="X",D9*Q9*R9*0.5,0)</f>
+        <v>0.74249999999999994</v>
+      </c>
+      <c r="U9" s="3">
+        <f t="shared" ref="U9:U10" si="13">T9/$T$4</f>
+        <v>1.3499999999999999</v>
+      </c>
+      <c r="V9" s="7">
+        <f t="shared" si="3"/>
+        <v>2.6936026936026938</v>
+      </c>
+      <c r="W9" s="4"/>
+      <c r="X9" s="3">
+        <f t="shared" si="4"/>
         <v>0.75</v>
       </c>
-      <c r="R9" s="3">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="S9" s="5">
-        <f t="shared" ref="S9:S10" si="12">1*Q9*P9*(1+R9)*D9 + IF(N9="X",D9*P9*0.25,0) + IF(M9="X",D9*P9*Q9*0.5,0)</f>
-        <v>0.61875000000000002</v>
-      </c>
-      <c r="T9" s="3">
-        <f t="shared" ref="T9:T10" si="13">S9/$S$4</f>
-        <v>1.125</v>
-      </c>
-      <c r="U9" s="7">
-        <f t="shared" si="3"/>
-        <v>3.2323232323232323</v>
-      </c>
-      <c r="V9" s="4"/>
-      <c r="W9" s="3">
-        <f t="shared" si="4"/>
-        <v>0.5</v>
-      </c>
-      <c r="X9" s="3">
-        <f t="shared" ref="X9:X10" si="14">(C9/20)*IF($AJ$13=1,IF(F9="X",1,0.5),1)</f>
-        <v>0.75</v>
-      </c>
       <c r="Y9" s="3">
+        <f t="shared" ref="Y9:Y10" si="14">(C9/20)*IF($AK$13=1,IF(F9="X",1,0.5),1)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Z9" s="3">
         <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
-      <c r="Z9" s="5">
+      <c r="AA9" s="5">
         <f t="shared" si="6"/>
-        <v>0.30937500000000001</v>
-      </c>
-      <c r="AA9" s="3">
-        <f t="shared" ref="AA9:AA10" si="15">Z9/$Z$4</f>
-        <v>1.125</v>
-      </c>
-      <c r="AB9" s="7">
+        <v>0.74249999999999994</v>
+      </c>
+      <c r="AB9" s="3">
+        <f t="shared" ref="AB9:AB10" si="15">AA9/$AA$4</f>
+        <v>2.6999999999999997</v>
+      </c>
+      <c r="AC9" s="7">
         <f t="shared" si="7"/>
-        <v>6.4646464646464645</v>
-      </c>
-      <c r="AC9" s="3">
+        <v>2.6936026936026938</v>
+      </c>
+      <c r="AD9" s="3">
         <f t="shared" si="8"/>
-        <v>1.125</v>
-      </c>
-      <c r="AD9" s="3"/>
-      <c r="AH9" t="s">
+        <v>2.0249999999999999</v>
+      </c>
+      <c r="AE9" s="3"/>
+      <c r="AI9" t="s">
         <v>47</v>
       </c>
-      <c r="AI9">
+      <c r="AJ9">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>71</v>
       </c>
@@ -3851,7 +3876,9 @@
         <v>59</v>
       </c>
       <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -3859,68 +3886,69 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
-      <c r="P10" s="3">
+      <c r="P10" s="1"/>
+      <c r="Q10" s="3">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="Q10" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="R10" s="3">
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
-      <c r="R10" s="3">
+      <c r="S10" s="3">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="S10" s="5">
+      <c r="T10" s="5">
         <f t="shared" si="12"/>
-        <v>1.2375</v>
-      </c>
-      <c r="T10" s="3">
+        <v>1.8562500000000002</v>
+      </c>
+      <c r="U10" s="3">
         <f t="shared" si="13"/>
-        <v>2.25</v>
-      </c>
-      <c r="U10" s="7">
+        <v>3.375</v>
+      </c>
+      <c r="V10" s="7">
         <f t="shared" si="3"/>
-        <v>1.6161616161616161</v>
-      </c>
-      <c r="V10" s="4"/>
-      <c r="W10" s="3">
+        <v>1.0774410774410774</v>
+      </c>
+      <c r="W10" s="4"/>
+      <c r="X10" s="3">
         <f t="shared" si="4"/>
-        <v>0.5</v>
-      </c>
-      <c r="X10" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="Y10" s="3">
         <f t="shared" si="14"/>
         <v>0.75</v>
       </c>
-      <c r="Y10" s="3">
+      <c r="Z10" s="3">
         <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
-      <c r="Z10" s="5">
+      <c r="AA10" s="5">
         <f t="shared" si="6"/>
-        <v>1.2375</v>
-      </c>
-      <c r="AA10" s="3">
+        <v>1.8562500000000002</v>
+      </c>
+      <c r="AB10" s="3">
         <f t="shared" si="15"/>
-        <v>4.5</v>
-      </c>
-      <c r="AB10" s="7">
+        <v>6.75</v>
+      </c>
+      <c r="AC10" s="7">
         <f t="shared" si="7"/>
-        <v>1.6161616161616161</v>
-      </c>
-      <c r="AC10" s="3">
+        <v>1.0774410774410774</v>
+      </c>
+      <c r="AD10" s="3">
         <f t="shared" si="8"/>
-        <v>3.375</v>
-      </c>
-      <c r="AD10" s="17"/>
-      <c r="AH10" t="s">
+        <v>5.0625</v>
+      </c>
+      <c r="AE10" s="17"/>
+      <c r="AI10" t="s">
         <v>10</v>
       </c>
-      <c r="AI10">
+      <c r="AJ10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
       <c r="D11" s="1"/>
@@ -3935,29 +3963,30 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
-      <c r="P11" s="3"/>
+      <c r="P11" s="1"/>
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="7"/>
-      <c r="V11" s="4"/>
-      <c r="W11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="4"/>
       <c r="X11" s="3"/>
       <c r="Y11" s="3"/>
-      <c r="Z11" s="5"/>
-      <c r="AA11" s="3"/>
-      <c r="AB11" s="7"/>
-      <c r="AC11" s="3"/>
-      <c r="AD11" s="17"/>
-      <c r="AH11" t="s">
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="5"/>
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="7"/>
+      <c r="AD11" s="3"/>
+      <c r="AE11" s="17"/>
+      <c r="AI11" t="s">
         <v>85</v>
       </c>
-      <c r="AI11">
+      <c r="AJ11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="2:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
@@ -3978,68 +4007,69 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
-      <c r="P12" s="3">
-        <f>IF(K12="X",1,($AF$3+H12)/20)</f>
-        <v>0.5</v>
-      </c>
+      <c r="P12" s="1"/>
       <c r="Q12" s="3">
-        <f>(C12/20)*IF($AI$6=1,0.5,1)</f>
+        <f>IF(L12="X",1,($AG$3+I12)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="R12" s="3">
+        <f>(C12/20)*IF($AJ$6=1,0.5,1)</f>
         <v>0.4</v>
       </c>
-      <c r="R12" s="3">
+      <c r="S12" s="3">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="S12" s="5">
-        <f t="shared" ref="S12:S14" si="16">((1*Q12*(P12)*D12   +   (IF(J12="X",2,1)*R12*D12)      + IF(N12="X",D12*P12*0.25,0)     ) * IF(M12="X",1.5,1) ) *      IF($AJ$6="1",0.5,1)</f>
+      <c r="T12" s="5">
+        <f t="shared" ref="T12:T14" si="16">((1*R12*(Q12)*D12   +   (IF(K12="X",2,1)*S12*D12)      + IF(O12="X",D12*Q12*0.25,0)     ) * IF(N12="X",1.5,1) ) *      IF($AK$6="1",0.5,1)</f>
         <v>0.60000000000000009</v>
       </c>
-      <c r="T12" s="3">
-        <f>S12/$S$12</f>
+      <c r="U12" s="3">
+        <f>T12/$T$12</f>
         <v>1</v>
       </c>
-      <c r="U12" s="7">
+      <c r="V12" s="7">
         <f t="shared" si="3"/>
         <v>3.333333333333333</v>
       </c>
-      <c r="V12" s="4"/>
-      <c r="W12" s="3">
-        <f>IF(K12="X",1,($AF$3+H12)/20)</f>
-        <v>0.5</v>
-      </c>
+      <c r="W12" s="4"/>
       <c r="X12" s="3">
-        <f>(C12/20)*IF($AF$13=1,IF(F12="X",1,0.5),1)</f>
+        <f>IF(L12="X",1,($AG$3+I12)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Y12" s="3">
+        <f>(C12/20)*IF($AG$13=1,IF(F12="X",1,0.5),1)</f>
         <v>0.4</v>
       </c>
-      <c r="Y12" s="3">
+      <c r="Z12" s="3">
         <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
-      <c r="Z12" s="5">
-        <f>IF(G12="X",0,((1*X12*(W12)*D12   +   (IF(J12="X",2,1)*Y12*D12)      + IF(N12="X",D12*W12*0.25,0)     ) * IF(M12="X",1.5,1) ) *      IF($AI$13=1,IF(F12="X",1,0.5),1))</f>
+      <c r="AA12" s="5">
+        <f>IF(G12="X",0,((1*Y12*(X12)*D12   +   (IF(K12="X",2,1)*Z12*D12)      + IF(O12="X",D12*X12*0.25,0)     ) * IF(N12="X",1.5,1) ) *      IF($AJ$13=1,IF(F12="X",1,0.5),1))</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="AA12" s="3">
-        <f>Z12/$Z$12</f>
+      <c r="AB12" s="3">
+        <f>AA12/$AA$12</f>
         <v>1</v>
       </c>
-      <c r="AB12" s="7">
+      <c r="AC12" s="7">
         <f t="shared" si="7"/>
         <v>6.6666666666666661</v>
       </c>
-      <c r="AC12" s="3">
+      <c r="AD12" s="3">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="AD12" s="17"/>
-      <c r="AH12" t="s">
+      <c r="AE12" s="17"/>
+      <c r="AI12" t="s">
         <v>86</v>
       </c>
-      <c r="AI12">
+      <c r="AJ12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>37</v>
       </c>
@@ -4064,68 +4094,69 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
-      <c r="P13" s="3">
-        <f t="shared" ref="P13:P35" si="17">IF(K13="X",1,($AF$3+H13)/20)</f>
-        <v>0.5</v>
-      </c>
+      <c r="P13" s="1"/>
       <c r="Q13" s="3">
-        <f t="shared" ref="Q13:Q35" si="18">(C13/20)*IF($AI$6=1,0.5,1)</f>
+        <f t="shared" ref="Q13:Q35" si="17">IF(L13="X",1,($AG$3+I13)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="R13" s="3">
+        <f t="shared" ref="R13:R35" si="18">(C13/20)*IF($AJ$6=1,0.5,1)</f>
         <v>0.35</v>
       </c>
-      <c r="R13" s="3">
+      <c r="S13" s="3">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="S13" s="5">
+      <c r="T13" s="5">
         <f t="shared" si="16"/>
         <v>0.55000000000000004</v>
       </c>
-      <c r="T13" s="3">
-        <f t="shared" ref="T13:T16" si="19">S13/$S$12</f>
+      <c r="U13" s="3">
+        <f t="shared" ref="U13:U16" si="19">T13/$T$12</f>
         <v>0.91666666666666663</v>
       </c>
-      <c r="U13" s="7">
+      <c r="V13" s="7">
         <f t="shared" si="3"/>
         <v>3.6363636363636362</v>
       </c>
-      <c r="V13" s="4"/>
-      <c r="W13" s="3">
-        <f t="shared" ref="W13:W35" si="20">IF(K13="X",1,($AF$3+H13)/20)</f>
-        <v>0.5</v>
-      </c>
+      <c r="W13" s="4"/>
       <c r="X13" s="3">
-        <f t="shared" ref="X13:X35" si="21">(C13/20)*IF($AF$13=1,IF(F13="X",1,0.5),1)</f>
+        <f t="shared" ref="X13:X35" si="20">IF(L13="X",1,($AG$3+I13)/20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Y13" s="3">
+        <f t="shared" ref="Y13:Y35" si="21">(C13/20)*IF($AG$13=1,IF(F13="X",1,0.5),1)</f>
         <v>0.35</v>
       </c>
-      <c r="Y13" s="3">
+      <c r="Z13" s="3">
         <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
-      <c r="Z13" s="5">
-        <f t="shared" ref="Z13:Z35" si="22">IF(G13="X",0,((1*X13*(W13)*D13   +   (IF(J13="X",2,1)*Y13*D13)      + IF(N13="X",D13*W13*0.25,0)     ) * IF(M13="X",1.5,1) ) *      IF($AI$13=1,IF(F13="X",1,0.5),1))</f>
+      <c r="AA13" s="5">
+        <f t="shared" ref="AA13:AA35" si="22">IF(G13="X",0,((1*Y13*(X13)*D13   +   (IF(K13="X",2,1)*Z13*D13)      + IF(O13="X",D13*X13*0.25,0)     ) * IF(N13="X",1.5,1) ) *      IF($AJ$13=1,IF(F13="X",1,0.5),1))</f>
         <v>0.55000000000000004</v>
       </c>
-      <c r="AA13" s="3">
-        <f t="shared" ref="AA13:AA25" si="23">Z13/$Z$12</f>
+      <c r="AB13" s="3">
+        <f t="shared" ref="AB13:AB25" si="23">AA13/$AA$12</f>
         <v>1.8333333333333333</v>
       </c>
-      <c r="AB13" s="7">
+      <c r="AC13" s="7">
         <f t="shared" si="7"/>
         <v>3.6363636363636362</v>
       </c>
-      <c r="AC13" s="3">
+      <c r="AD13" s="3">
         <f t="shared" si="8"/>
         <v>1.375</v>
       </c>
-      <c r="AD13" s="17"/>
-      <c r="AH13" t="s">
+      <c r="AE13" s="17"/>
+      <c r="AI13" t="s">
         <v>87</v>
       </c>
-      <c r="AI13">
+      <c r="AJ13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>58</v>
       </c>
@@ -4150,62 +4181,63 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="3">
+      <c r="P14" s="1"/>
+      <c r="Q14" s="3">
         <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
-      <c r="Q14" s="3">
+      <c r="R14" s="3">
         <f t="shared" si="18"/>
         <v>0.4</v>
       </c>
-      <c r="R14" s="3">
+      <c r="S14" s="3">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="S14" s="5">
+      <c r="T14" s="5">
         <f t="shared" si="16"/>
         <v>0.60000000000000009</v>
       </c>
-      <c r="T14" s="3">
+      <c r="U14" s="3">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="U14" s="7">
+      <c r="V14" s="7">
         <f t="shared" si="3"/>
         <v>3.333333333333333</v>
       </c>
-      <c r="V14" s="4"/>
-      <c r="W14" s="3">
+      <c r="W14" s="4"/>
+      <c r="X14" s="3">
         <f t="shared" si="20"/>
         <v>0.5</v>
       </c>
-      <c r="X14" s="3">
+      <c r="Y14" s="3">
         <f t="shared" si="21"/>
         <v>0.4</v>
       </c>
-      <c r="Y14" s="3">
+      <c r="Z14" s="3">
         <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
-      <c r="Z14" s="5">
+      <c r="AA14" s="5">
         <f t="shared" si="22"/>
         <v>0.60000000000000009</v>
       </c>
-      <c r="AA14" s="3">
+      <c r="AB14" s="3">
         <f t="shared" si="23"/>
         <v>2</v>
       </c>
-      <c r="AB14" s="7">
+      <c r="AC14" s="7">
         <f t="shared" si="7"/>
         <v>3.333333333333333</v>
       </c>
-      <c r="AC14" s="3">
+      <c r="AD14" s="3">
         <f t="shared" si="8"/>
         <v>1.5</v>
       </c>
-      <c r="AD14" s="17"/>
-    </row>
-    <row r="15" spans="2:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE14" s="17"/>
+    </row>
+    <row r="15" spans="2:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
@@ -4224,68 +4256,69 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-      <c r="L15" s="1" t="s">
+      <c r="L15" s="1"/>
+      <c r="M15" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="3">
+      <c r="P15" s="1"/>
+      <c r="Q15" s="3">
         <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
-      <c r="Q15" s="3">
+      <c r="R15" s="3">
         <f t="shared" si="18"/>
         <v>0.4</v>
       </c>
-      <c r="R15" s="3">
+      <c r="S15" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S15" s="5">
-        <f t="shared" ref="S15:S23" si="24">((1*Q15*(P15)*D15   +   (IF(J15="X",2,1)*R15*D15)      + IF(N15="X",D15*P15*0.25,0)     ) * IF(M15="X",1.5,1) ) *      IF($AJ$6="1",0.5,1)</f>
+      <c r="T15" s="5">
+        <f t="shared" ref="T15:T23" si="24">((1*R15*(Q15)*D15   +   (IF(K15="X",2,1)*S15*D15)      + IF(O15="X",D15*Q15*0.25,0)     ) * IF(N15="X",1.5,1) ) *      IF($AK$6="1",0.5,1)</f>
         <v>0.8</v>
       </c>
-      <c r="T15" s="3">
+      <c r="U15" s="3">
         <f t="shared" si="19"/>
         <v>1.3333333333333333</v>
       </c>
-      <c r="U15" s="7">
+      <c r="V15" s="7">
         <f t="shared" si="3"/>
         <v>2.5</v>
       </c>
-      <c r="V15" s="4"/>
-      <c r="W15" s="3">
+      <c r="W15" s="4"/>
+      <c r="X15" s="3">
         <f t="shared" si="20"/>
         <v>0.5</v>
       </c>
-      <c r="X15" s="3">
+      <c r="Y15" s="3">
         <f t="shared" si="21"/>
         <v>0.4</v>
       </c>
-      <c r="Y15" s="3">
+      <c r="Z15" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z15" s="5">
+      <c r="AA15" s="5">
         <f t="shared" si="22"/>
         <v>0.4</v>
       </c>
-      <c r="AA15" s="3">
+      <c r="AB15" s="3">
         <f t="shared" si="23"/>
         <v>1.3333333333333333</v>
       </c>
-      <c r="AB15" s="7">
+      <c r="AC15" s="7">
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="AC15" s="3">
+      <c r="AD15" s="3">
         <f t="shared" si="8"/>
         <v>1.3333333333333333</v>
       </c>
-      <c r="AD15" s="17"/>
-    </row>
-    <row r="16" spans="2:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE15" s="17"/>
+    </row>
+    <row r="16" spans="2:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
@@ -4303,71 +4336,72 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
-      <c r="K16" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="K16" s="1"/>
       <c r="L16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M16" s="1"/>
+      <c r="M16" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
-      <c r="P16" s="3">
+      <c r="P16" s="1"/>
+      <c r="Q16" s="3">
         <f t="shared" si="17"/>
         <v>1</v>
       </c>
-      <c r="Q16" s="3">
+      <c r="R16" s="3">
         <f t="shared" si="18"/>
         <v>0.3</v>
       </c>
-      <c r="R16" s="3">
+      <c r="S16" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S16" s="5">
+      <c r="T16" s="5">
         <f t="shared" si="24"/>
         <v>0.6</v>
       </c>
-      <c r="T16" s="3">
+      <c r="U16" s="3">
         <f t="shared" si="19"/>
         <v>0.99999999999999978</v>
       </c>
-      <c r="U16" s="7">
+      <c r="V16" s="7">
         <f t="shared" si="3"/>
         <v>3.3333333333333335</v>
       </c>
-      <c r="V16" s="4"/>
-      <c r="W16" s="3">
+      <c r="W16" s="4"/>
+      <c r="X16" s="3">
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
-      <c r="X16" s="3">
+      <c r="Y16" s="3">
         <f t="shared" si="21"/>
         <v>0.3</v>
       </c>
-      <c r="Y16" s="3">
+      <c r="Z16" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z16" s="5">
+      <c r="AA16" s="5">
         <f t="shared" si="22"/>
         <v>0.3</v>
       </c>
-      <c r="AA16" s="3">
+      <c r="AB16" s="3">
         <f t="shared" si="23"/>
         <v>0.99999999999999978</v>
       </c>
-      <c r="AB16" s="7">
+      <c r="AC16" s="7">
         <f t="shared" si="7"/>
         <v>6.666666666666667</v>
       </c>
-      <c r="AC16" s="3">
+      <c r="AD16" s="3">
         <f t="shared" si="8"/>
         <v>0.99999999999999978</v>
       </c>
-      <c r="AD16" s="17"/>
-    </row>
-    <row r="17" spans="2:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE16" s="17"/>
+    </row>
+    <row r="17" spans="2:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="2"/>
       <c r="D17" s="1"/>
@@ -4382,23 +4416,24 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
-      <c r="P17" s="3"/>
+      <c r="P17" s="1"/>
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="3"/>
-      <c r="U17" s="7"/>
-      <c r="V17" s="4"/>
-      <c r="W17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="3"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="4"/>
       <c r="X17" s="3"/>
       <c r="Y17" s="3"/>
-      <c r="Z17" s="5"/>
-      <c r="AA17" s="3"/>
-      <c r="AB17" s="18"/>
-      <c r="AC17" s="3"/>
-      <c r="AD17" s="17"/>
-    </row>
-    <row r="18" spans="2:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z17" s="3"/>
+      <c r="AA17" s="5"/>
+      <c r="AB17" s="3"/>
+      <c r="AC17" s="18"/>
+      <c r="AD17" s="3"/>
+      <c r="AE17" s="17"/>
+    </row>
+    <row r="18" spans="2:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>24</v>
       </c>
@@ -4419,62 +4454,63 @@
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
-      <c r="P18" s="3">
+      <c r="P18" s="1"/>
+      <c r="Q18" s="3">
         <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
-      <c r="Q18" s="3">
+      <c r="R18" s="3">
         <f t="shared" si="18"/>
         <v>0.5</v>
       </c>
-      <c r="R18" s="3">
+      <c r="S18" s="3">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="S18" s="5">
+      <c r="T18" s="5">
         <f t="shared" si="24"/>
         <v>1.05</v>
       </c>
-      <c r="T18" s="3">
-        <f>S18/$S$18</f>
+      <c r="U18" s="3">
+        <f>T18/$T$18</f>
         <v>1</v>
       </c>
-      <c r="U18" s="7">
+      <c r="V18" s="7">
         <f t="shared" si="3"/>
         <v>1.9047619047619047</v>
       </c>
-      <c r="V18" s="4"/>
-      <c r="W18" s="3">
+      <c r="W18" s="4"/>
+      <c r="X18" s="3">
         <f t="shared" si="20"/>
         <v>0.5</v>
       </c>
-      <c r="X18" s="3">
+      <c r="Y18" s="3">
         <f t="shared" si="21"/>
         <v>0.5</v>
       </c>
-      <c r="Y18" s="3">
+      <c r="Z18" s="3">
         <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
-      <c r="Z18" s="5">
+      <c r="AA18" s="5">
         <f t="shared" si="22"/>
         <v>0.52500000000000002</v>
       </c>
-      <c r="AA18" s="3">
+      <c r="AB18" s="3">
         <f t="shared" si="23"/>
         <v>1.7499999999999998</v>
       </c>
-      <c r="AB18" s="18">
-        <f>$AI$9/Z18</f>
+      <c r="AC18" s="18">
+        <f>$AJ$9/AA18</f>
         <v>7.6190476190476186</v>
       </c>
-      <c r="AC18" s="3">
+      <c r="AD18" s="3">
         <f t="shared" si="8"/>
         <v>1.375</v>
       </c>
-      <c r="AD18" s="17"/>
-    </row>
-    <row r="19" spans="2:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE18" s="17"/>
+    </row>
+    <row r="19" spans="2:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>25</v>
       </c>
@@ -4497,62 +4533,63 @@
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
-      <c r="P19" s="3">
+      <c r="P19" s="1"/>
+      <c r="Q19" s="3">
         <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
-      <c r="Q19" s="3">
+      <c r="R19" s="3">
         <f t="shared" si="18"/>
         <v>0.4</v>
       </c>
-      <c r="R19" s="3">
+      <c r="S19" s="3">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="S19" s="5">
+      <c r="T19" s="5">
         <f t="shared" si="24"/>
         <v>0.90000000000000013</v>
       </c>
-      <c r="T19" s="3">
-        <f t="shared" ref="T19:T25" si="25">S19/$S$18</f>
+      <c r="U19" s="3">
+        <f t="shared" ref="U19:U25" si="25">T19/$T$18</f>
         <v>0.85714285714285721</v>
       </c>
-      <c r="U19" s="7">
+      <c r="V19" s="7">
         <f t="shared" si="3"/>
         <v>2.2222222222222219</v>
       </c>
-      <c r="V19" s="4"/>
-      <c r="W19" s="3">
+      <c r="W19" s="4"/>
+      <c r="X19" s="3">
         <f t="shared" si="20"/>
         <v>0.5</v>
       </c>
-      <c r="X19" s="3">
+      <c r="Y19" s="3">
         <f t="shared" si="21"/>
         <v>0.4</v>
       </c>
-      <c r="Y19" s="3">
+      <c r="Z19" s="3">
         <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
-      <c r="Z19" s="5">
+      <c r="AA19" s="5">
         <f t="shared" si="22"/>
         <v>0.45000000000000007</v>
       </c>
-      <c r="AA19" s="3">
+      <c r="AB19" s="3">
         <f t="shared" si="23"/>
         <v>1.5</v>
       </c>
-      <c r="AB19" s="18">
-        <f t="shared" ref="AB19:AB35" si="26">$AI$9/Z19</f>
+      <c r="AC19" s="18">
+        <f t="shared" ref="AC19:AC35" si="26">$AJ$9/AA19</f>
         <v>8.8888888888888875</v>
       </c>
-      <c r="AC19" s="3">
+      <c r="AD19" s="3">
         <f t="shared" si="8"/>
         <v>1.1785714285714286</v>
       </c>
-      <c r="AD19" s="17"/>
-    </row>
-    <row r="20" spans="2:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE19" s="17"/>
+    </row>
+    <row r="20" spans="2:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>26</v>
       </c>
@@ -4575,62 +4612,63 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
-      <c r="P20" s="3">
+      <c r="P20" s="1"/>
+      <c r="Q20" s="3">
         <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
-      <c r="Q20" s="3">
+      <c r="R20" s="3">
         <f t="shared" si="18"/>
         <v>0.4</v>
       </c>
-      <c r="R20" s="3">
+      <c r="S20" s="3">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="S20" s="5">
+      <c r="T20" s="5">
         <f t="shared" si="24"/>
         <v>0.90000000000000013</v>
       </c>
-      <c r="T20" s="3">
+      <c r="U20" s="3">
         <f t="shared" si="25"/>
         <v>0.85714285714285721</v>
       </c>
-      <c r="U20" s="7">
+      <c r="V20" s="7">
         <f t="shared" si="3"/>
         <v>2.2222222222222219</v>
       </c>
-      <c r="V20" s="4"/>
-      <c r="W20" s="3">
+      <c r="W20" s="4"/>
+      <c r="X20" s="3">
         <f t="shared" si="20"/>
         <v>0.5</v>
       </c>
-      <c r="X20" s="3">
+      <c r="Y20" s="3">
         <f t="shared" si="21"/>
         <v>0.4</v>
       </c>
-      <c r="Y20" s="3">
+      <c r="Z20" s="3">
         <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
-      <c r="Z20" s="5">
+      <c r="AA20" s="5">
         <f t="shared" si="22"/>
         <v>0.90000000000000013</v>
       </c>
-      <c r="AA20" s="3">
+      <c r="AB20" s="3">
         <f t="shared" si="23"/>
         <v>3</v>
       </c>
-      <c r="AB20" s="18">
+      <c r="AC20" s="18">
         <f t="shared" si="26"/>
         <v>4.4444444444444438</v>
       </c>
-      <c r="AC20" s="3">
+      <c r="AD20" s="3">
         <f t="shared" si="8"/>
         <v>1.9285714285714286</v>
       </c>
-      <c r="AD20" s="17"/>
-    </row>
-    <row r="21" spans="2:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE20" s="17"/>
+    </row>
+    <row r="21" spans="2:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>51</v>
       </c>
@@ -4655,62 +4693,63 @@
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
-      <c r="P21" s="3">
+      <c r="P21" s="1"/>
+      <c r="Q21" s="3">
         <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
-      <c r="Q21" s="3">
+      <c r="R21" s="3">
         <f t="shared" si="18"/>
         <v>0.6</v>
       </c>
-      <c r="R21" s="3">
+      <c r="S21" s="3">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="S21" s="5">
+      <c r="T21" s="5">
         <f t="shared" si="24"/>
         <v>0.8</v>
       </c>
-      <c r="T21" s="3">
+      <c r="U21" s="3">
         <f t="shared" si="25"/>
         <v>0.76190476190476186</v>
       </c>
-      <c r="U21" s="7">
+      <c r="V21" s="7">
         <f t="shared" si="3"/>
         <v>2.5</v>
       </c>
-      <c r="V21" s="4"/>
-      <c r="W21" s="3">
+      <c r="W21" s="4"/>
+      <c r="X21" s="3">
         <f t="shared" si="20"/>
         <v>0.5</v>
       </c>
-      <c r="X21" s="3">
+      <c r="Y21" s="3">
         <f t="shared" si="21"/>
         <v>0.6</v>
       </c>
-      <c r="Y21" s="3">
+      <c r="Z21" s="3">
         <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
-      <c r="Z21" s="5">
+      <c r="AA21" s="5">
         <f t="shared" si="22"/>
         <v>0.8</v>
       </c>
-      <c r="AA21" s="3">
+      <c r="AB21" s="3">
         <f t="shared" si="23"/>
         <v>2.6666666666666665</v>
       </c>
-      <c r="AB21" s="18">
+      <c r="AC21" s="18">
         <f t="shared" si="26"/>
         <v>5</v>
       </c>
-      <c r="AC21" s="3">
+      <c r="AD21" s="3">
         <f t="shared" si="8"/>
         <v>1.7142857142857142</v>
       </c>
-      <c r="AD21" s="17"/>
-    </row>
-    <row r="22" spans="2:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE21" s="17"/>
+    </row>
+    <row r="22" spans="2:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>27</v>
       </c>
@@ -4728,71 +4767,72 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
-      <c r="K22" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="K22" s="1"/>
       <c r="L22" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M22" s="1"/>
+      <c r="M22" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
-      <c r="P22" s="3">
+      <c r="P22" s="1"/>
+      <c r="Q22" s="3">
         <f t="shared" si="17"/>
         <v>1</v>
       </c>
-      <c r="Q22" s="3">
+      <c r="R22" s="3">
         <f t="shared" si="18"/>
         <v>0.5</v>
       </c>
-      <c r="R22" s="3">
+      <c r="S22" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S22" s="5">
+      <c r="T22" s="5">
         <f t="shared" si="24"/>
         <v>1</v>
       </c>
-      <c r="T22" s="3">
+      <c r="U22" s="3">
         <f t="shared" si="25"/>
         <v>0.95238095238095233</v>
       </c>
-      <c r="U22" s="7">
+      <c r="V22" s="7">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="V22" s="4"/>
-      <c r="W22" s="3">
+      <c r="W22" s="4"/>
+      <c r="X22" s="3">
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
-      <c r="X22" s="3">
+      <c r="Y22" s="3">
         <f t="shared" si="21"/>
         <v>0.5</v>
       </c>
-      <c r="Y22" s="3">
+      <c r="Z22" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z22" s="5">
+      <c r="AA22" s="5">
         <f t="shared" si="22"/>
         <v>0.5</v>
       </c>
-      <c r="AA22" s="3">
+      <c r="AB22" s="3">
         <f t="shared" si="23"/>
         <v>1.6666666666666665</v>
       </c>
-      <c r="AB22" s="18">
+      <c r="AC22" s="18">
         <f t="shared" si="26"/>
         <v>8</v>
       </c>
-      <c r="AC22" s="3">
+      <c r="AD22" s="3">
         <f t="shared" si="8"/>
         <v>1.3095238095238093</v>
       </c>
-      <c r="AD22" s="17"/>
-    </row>
-    <row r="23" spans="2:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE22" s="17"/>
+    </row>
+    <row r="23" spans="2:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>28</v>
       </c>
@@ -4807,76 +4847,77 @@
         <v>59</v>
       </c>
       <c r="G23" s="1"/>
-      <c r="H23" s="1">
+      <c r="H23" s="1"/>
+      <c r="I23" s="1">
         <v>5</v>
       </c>
-      <c r="I23" s="1">
+      <c r="J23" s="1">
         <v>4</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
-      <c r="P23" s="3">
+      <c r="P23" s="1"/>
+      <c r="Q23" s="3">
         <f t="shared" si="17"/>
         <v>0.75</v>
       </c>
-      <c r="Q23" s="3">
+      <c r="R23" s="3">
         <f t="shared" si="18"/>
         <v>0.8</v>
       </c>
-      <c r="R23" s="3">
+      <c r="S23" s="3">
         <f t="shared" si="2"/>
         <v>0.3</v>
       </c>
-      <c r="S23" s="5">
+      <c r="T23" s="5">
         <f t="shared" si="24"/>
         <v>1.2000000000000002</v>
       </c>
-      <c r="T23" s="3">
+      <c r="U23" s="3">
         <f t="shared" si="25"/>
         <v>1.142857142857143</v>
       </c>
-      <c r="U23" s="7">
+      <c r="V23" s="7">
         <f t="shared" si="3"/>
         <v>1.6666666666666665</v>
       </c>
-      <c r="V23" s="4"/>
-      <c r="W23" s="3">
+      <c r="W23" s="4"/>
+      <c r="X23" s="3">
         <f t="shared" si="20"/>
         <v>0.75</v>
       </c>
-      <c r="X23" s="3">
+      <c r="Y23" s="3">
         <f t="shared" si="21"/>
         <v>0.8</v>
       </c>
-      <c r="Y23" s="3">
+      <c r="Z23" s="3">
         <f t="shared" si="5"/>
         <v>0.3</v>
       </c>
-      <c r="Z23" s="5">
+      <c r="AA23" s="5">
         <f t="shared" si="22"/>
         <v>1.2000000000000002</v>
       </c>
-      <c r="AA23" s="3">
+      <c r="AB23" s="3">
         <f t="shared" si="23"/>
         <v>4</v>
       </c>
-      <c r="AB23" s="18">
+      <c r="AC23" s="18">
         <f t="shared" si="26"/>
         <v>3.333333333333333</v>
       </c>
-      <c r="AC23" s="3">
+      <c r="AD23" s="3">
         <f t="shared" si="8"/>
         <v>2.5714285714285716</v>
       </c>
-      <c r="AD23" s="17"/>
-    </row>
-    <row r="24" spans="2:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE23" s="17"/>
+    </row>
+    <row r="24" spans="2:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>29</v>
       </c>
@@ -4897,62 +4938,63 @@
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
-      <c r="P24" s="3">
+      <c r="P24" s="1"/>
+      <c r="Q24" s="3">
         <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
-      <c r="Q24" s="3">
+      <c r="R24" s="3">
         <f t="shared" si="18"/>
         <v>0.5</v>
       </c>
-      <c r="R24" s="3">
+      <c r="S24" s="3">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="S24" s="5">
-        <f t="shared" ref="S24:S25" si="27">((1*Q24*(P24)*D24   +   (IF(J24="X",2,1)*R24*D24)      + IF(N24="X",D24*P24*0.25,0)     ) * IF(M24="X",1.5,1) ) *      IF($AJ$6="1",0.5,1)</f>
+      <c r="T24" s="5">
+        <f t="shared" ref="T24:T25" si="27">((1*R24*(Q24)*D24   +   (IF(K24="X",2,1)*S24*D24)      + IF(O24="X",D24*Q24*0.25,0)     ) * IF(N24="X",1.5,1) ) *      IF($AK$6="1",0.5,1)</f>
         <v>1.75</v>
       </c>
-      <c r="T24" s="3">
+      <c r="U24" s="3">
         <f t="shared" si="25"/>
         <v>1.6666666666666665</v>
       </c>
-      <c r="U24" s="7">
+      <c r="V24" s="7">
         <f t="shared" si="3"/>
         <v>1.1428571428571428</v>
       </c>
-      <c r="V24" s="4"/>
-      <c r="W24" s="3">
+      <c r="W24" s="4"/>
+      <c r="X24" s="3">
         <f t="shared" si="20"/>
         <v>0.5</v>
       </c>
-      <c r="X24" s="3">
+      <c r="Y24" s="3">
         <f t="shared" si="21"/>
         <v>0.5</v>
       </c>
-      <c r="Y24" s="3">
+      <c r="Z24" s="3">
         <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
-      <c r="Z24" s="5">
+      <c r="AA24" s="5">
         <f t="shared" si="22"/>
         <v>0.875</v>
       </c>
-      <c r="AA24" s="3">
+      <c r="AB24" s="3">
         <f t="shared" si="23"/>
         <v>2.9166666666666661</v>
       </c>
-      <c r="AB24" s="18">
+      <c r="AC24" s="18">
         <f t="shared" si="26"/>
         <v>4.5714285714285712</v>
       </c>
-      <c r="AC24" s="3">
+      <c r="AD24" s="3">
         <f t="shared" si="8"/>
         <v>2.2916666666666661</v>
       </c>
-      <c r="AD24" s="17"/>
-    </row>
-    <row r="25" spans="2:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE24" s="17"/>
+    </row>
+    <row r="25" spans="2:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>30</v>
       </c>
@@ -4971,68 +5013,69 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
-      <c r="L25" s="1" t="s">
+      <c r="L25" s="1"/>
+      <c r="M25" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
-      <c r="P25" s="3">
+      <c r="P25" s="1"/>
+      <c r="Q25" s="3">
         <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
-      <c r="Q25" s="3">
+      <c r="R25" s="3">
         <f t="shared" si="18"/>
         <v>0.4</v>
       </c>
-      <c r="R25" s="3">
+      <c r="S25" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S25" s="5">
+      <c r="T25" s="5">
         <f t="shared" si="27"/>
         <v>1.2000000000000002</v>
       </c>
-      <c r="T25" s="3">
+      <c r="U25" s="3">
         <f t="shared" si="25"/>
         <v>1.142857142857143</v>
       </c>
-      <c r="U25" s="7">
+      <c r="V25" s="7">
         <f t="shared" si="3"/>
         <v>1.6666666666666665</v>
       </c>
-      <c r="V25" s="4"/>
-      <c r="W25" s="3">
+      <c r="W25" s="4"/>
+      <c r="X25" s="3">
         <f t="shared" si="20"/>
         <v>0.5</v>
       </c>
-      <c r="X25" s="3">
+      <c r="Y25" s="3">
         <f t="shared" si="21"/>
         <v>0.4</v>
       </c>
-      <c r="Y25" s="3">
+      <c r="Z25" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z25" s="5">
+      <c r="AA25" s="5">
         <f t="shared" si="22"/>
         <v>0.60000000000000009</v>
       </c>
-      <c r="AA25" s="3">
+      <c r="AB25" s="3">
         <f t="shared" si="23"/>
         <v>2</v>
       </c>
-      <c r="AB25" s="18">
+      <c r="AC25" s="18">
         <f t="shared" si="26"/>
         <v>6.6666666666666661</v>
       </c>
-      <c r="AC25" s="3">
+      <c r="AD25" s="3">
         <f t="shared" si="8"/>
         <v>1.5714285714285716</v>
       </c>
-      <c r="AD25" s="17"/>
-    </row>
-    <row r="26" spans="2:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE25" s="17"/>
+    </row>
+    <row r="26" spans="2:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="2"/>
       <c r="D26" s="1"/>
@@ -5047,23 +5090,24 @@
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
-      <c r="P26" s="3"/>
+      <c r="P26" s="1"/>
       <c r="Q26" s="3"/>
       <c r="R26" s="3"/>
-      <c r="S26" s="5"/>
-      <c r="T26" s="3"/>
-      <c r="U26" s="7"/>
-      <c r="V26" s="4"/>
-      <c r="W26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="3"/>
+      <c r="V26" s="7"/>
+      <c r="W26" s="4"/>
       <c r="X26" s="3"/>
       <c r="Y26" s="3"/>
-      <c r="Z26" s="5"/>
-      <c r="AA26" s="3"/>
-      <c r="AB26" s="18"/>
-      <c r="AC26" s="3"/>
-      <c r="AD26" s="17"/>
-    </row>
-    <row r="27" spans="2:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z26" s="3"/>
+      <c r="AA26" s="5"/>
+      <c r="AB26" s="3"/>
+      <c r="AC26" s="18"/>
+      <c r="AD26" s="3"/>
+      <c r="AE26" s="17"/>
+    </row>
+    <row r="27" spans="2:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>31</v>
       </c>
@@ -5086,62 +5130,63 @@
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
-      <c r="P27" s="3">
+      <c r="P27" s="1"/>
+      <c r="Q27" s="3">
         <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
-      <c r="Q27" s="3">
+      <c r="R27" s="3">
         <f t="shared" si="18"/>
         <v>0.6</v>
       </c>
-      <c r="R27" s="3">
+      <c r="S27" s="3">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="S27" s="5">
-        <f>((1*Q27*(P27)*D27   +   (IF(J27="X",2,1)*R27*D27)      + IF(N27="X",D27*P27*0.25,0)     ) * IF(M27="X",1.5,1) ) *      IF($AJ$6="1",0.5,1)</f>
+      <c r="T27" s="5">
+        <f>((1*R27*(Q27)*D27   +   (IF(K27="X",2,1)*S27*D27)      + IF(O27="X",D27*Q27*0.25,0)     ) * IF(N27="X",1.5,1) ) *      IF($AK$6="1",0.5,1)</f>
         <v>1.6</v>
       </c>
-      <c r="T27" s="3">
-        <f>S27/$S$27</f>
+      <c r="U27" s="3">
+        <f>T27/$T$27</f>
         <v>1</v>
       </c>
-      <c r="U27" s="7">
-        <f t="shared" ref="U27" si="28">$AI$9/S27</f>
+      <c r="V27" s="7">
+        <f t="shared" ref="V27" si="28">$AJ$9/T27</f>
         <v>2.5</v>
       </c>
-      <c r="V27" s="4"/>
-      <c r="W27" s="3">
+      <c r="W27" s="4"/>
+      <c r="X27" s="3">
         <f t="shared" si="20"/>
         <v>0.5</v>
       </c>
-      <c r="X27" s="3">
+      <c r="Y27" s="3">
         <f t="shared" si="21"/>
         <v>0.6</v>
       </c>
-      <c r="Y27" s="3">
+      <c r="Z27" s="3">
         <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
-      <c r="Z27" s="5">
+      <c r="AA27" s="5">
         <f t="shared" si="22"/>
         <v>0.8</v>
       </c>
-      <c r="AA27" s="3">
-        <f>Z27/$Z$27</f>
+      <c r="AB27" s="3">
+        <f>AA27/$AA$27</f>
         <v>1</v>
       </c>
-      <c r="AB27" s="18">
+      <c r="AC27" s="18">
         <f t="shared" si="26"/>
         <v>5</v>
       </c>
-      <c r="AC27" s="3">
+      <c r="AD27" s="3">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="AD27" s="17"/>
-    </row>
-    <row r="28" spans="2:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE27" s="17"/>
+    </row>
+    <row r="28" spans="2:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>32</v>
       </c>
@@ -5159,71 +5204,72 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
-      <c r="K28" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="K28" s="1"/>
       <c r="L28" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M28" s="1"/>
+      <c r="M28" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
-      <c r="P28" s="3">
+      <c r="P28" s="1"/>
+      <c r="Q28" s="3">
         <f t="shared" si="17"/>
         <v>1</v>
       </c>
-      <c r="Q28" s="3">
+      <c r="R28" s="3">
         <f t="shared" si="18"/>
         <v>0.6</v>
       </c>
-      <c r="R28" s="3">
+      <c r="S28" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S28" s="5">
-        <f t="shared" ref="S28:S35" si="29">((1*Q28*(P28)*D28   +   (IF(J28="X",2,1)*R28*D28)      + IF(N28="X",D28*P28*0.25,0)     ) * IF(M28="X",1.5,1) ) *      IF($AJ$6="1",0.5,1)</f>
+      <c r="T28" s="5">
+        <f t="shared" ref="T28:T35" si="29">((1*R28*(Q28)*D28   +   (IF(K28="X",2,1)*S28*D28)      + IF(O28="X",D28*Q28*0.25,0)     ) * IF(N28="X",1.5,1) ) *      IF($AK$6="1",0.5,1)</f>
         <v>1.2</v>
       </c>
-      <c r="T28" s="3">
-        <f t="shared" ref="T28:T35" si="30">S28/$S$27</f>
+      <c r="U28" s="3">
+        <f t="shared" ref="U28:U35" si="30">T28/$T$27</f>
         <v>0.74999999999999989</v>
       </c>
-      <c r="U28" s="7">
-        <f t="shared" ref="U28:U35" si="31">$AI$9/S28</f>
+      <c r="V28" s="7">
+        <f t="shared" ref="V28:V35" si="31">$AJ$9/T28</f>
         <v>3.3333333333333335</v>
       </c>
-      <c r="V28" s="4"/>
-      <c r="W28" s="3">
+      <c r="W28" s="4"/>
+      <c r="X28" s="3">
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
-      <c r="X28" s="3">
+      <c r="Y28" s="3">
         <f t="shared" si="21"/>
         <v>0.6</v>
       </c>
-      <c r="Y28" s="3">
+      <c r="Z28" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z28" s="5">
+      <c r="AA28" s="5">
         <f t="shared" si="22"/>
         <v>0.6</v>
       </c>
-      <c r="AA28" s="3">
-        <f t="shared" ref="AA28:AA35" si="32">Z28/$Z$27</f>
+      <c r="AB28" s="3">
+        <f t="shared" ref="AB28:AB35" si="32">AA28/$AA$27</f>
         <v>0.74999999999999989</v>
       </c>
-      <c r="AB28" s="18">
+      <c r="AC28" s="18">
         <f t="shared" si="26"/>
         <v>6.666666666666667</v>
       </c>
-      <c r="AC28" s="3">
+      <c r="AD28" s="3">
         <f t="shared" si="8"/>
         <v>0.74999999999999989</v>
       </c>
-      <c r="AD28" s="3"/>
-    </row>
-    <row r="29" spans="2:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE28" s="3"/>
+    </row>
+    <row r="29" spans="2:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>33</v>
       </c>
@@ -5246,62 +5292,63 @@
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
-      <c r="P29" s="3">
+      <c r="P29" s="1"/>
+      <c r="Q29" s="3">
         <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
-      <c r="Q29" s="3">
+      <c r="R29" s="3">
         <f t="shared" si="18"/>
         <v>0.7</v>
       </c>
-      <c r="R29" s="3">
+      <c r="S29" s="3">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="S29" s="5">
+      <c r="T29" s="5">
         <f t="shared" si="29"/>
         <v>1.3499999999999999</v>
       </c>
-      <c r="T29" s="3">
+      <c r="U29" s="3">
         <f t="shared" si="30"/>
         <v>0.84374999999999989</v>
       </c>
-      <c r="U29" s="7">
+      <c r="V29" s="7">
         <f t="shared" si="31"/>
         <v>2.9629629629629632</v>
       </c>
-      <c r="V29" s="4"/>
-      <c r="W29" s="3">
+      <c r="W29" s="4"/>
+      <c r="X29" s="3">
         <f t="shared" si="20"/>
         <v>0.5</v>
       </c>
-      <c r="X29" s="3">
+      <c r="Y29" s="3">
         <f t="shared" si="21"/>
         <v>0.7</v>
       </c>
-      <c r="Y29" s="3">
+      <c r="Z29" s="3">
         <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
-      <c r="Z29" s="5">
+      <c r="AA29" s="5">
         <f t="shared" si="22"/>
         <v>1.3499999999999999</v>
       </c>
-      <c r="AA29" s="3">
+      <c r="AB29" s="3">
         <f t="shared" si="32"/>
         <v>1.6874999999999998</v>
       </c>
-      <c r="AB29" s="18">
+      <c r="AC29" s="18">
         <f t="shared" si="26"/>
         <v>2.9629629629629632</v>
       </c>
-      <c r="AC29" s="3">
+      <c r="AD29" s="3">
         <f t="shared" si="8"/>
         <v>1.2656249999999998</v>
       </c>
-      <c r="AD29" s="17"/>
-    </row>
-    <row r="30" spans="2:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE29" s="17"/>
+    </row>
+    <row r="30" spans="2:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>34</v>
       </c>
@@ -5319,71 +5366,72 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
-      <c r="K30" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="K30" s="1"/>
       <c r="L30" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M30" s="1"/>
+      <c r="M30" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
-      <c r="P30" s="3">
+      <c r="P30" s="1"/>
+      <c r="Q30" s="3">
         <f t="shared" si="17"/>
         <v>1</v>
       </c>
-      <c r="Q30" s="3">
+      <c r="R30" s="3">
         <f t="shared" si="18"/>
         <v>0.5</v>
       </c>
-      <c r="R30" s="3">
+      <c r="S30" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S30" s="5">
+      <c r="T30" s="5">
         <f t="shared" si="29"/>
         <v>1</v>
       </c>
-      <c r="T30" s="3">
+      <c r="U30" s="3">
         <f t="shared" si="30"/>
         <v>0.625</v>
       </c>
-      <c r="U30" s="7">
+      <c r="V30" s="7">
         <f t="shared" si="31"/>
         <v>4</v>
       </c>
-      <c r="V30" s="4"/>
-      <c r="W30" s="3">
+      <c r="W30" s="4"/>
+      <c r="X30" s="3">
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
-      <c r="X30" s="3">
+      <c r="Y30" s="3">
         <f t="shared" si="21"/>
         <v>0.5</v>
       </c>
-      <c r="Y30" s="3">
+      <c r="Z30" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z30" s="5">
+      <c r="AA30" s="5">
         <f t="shared" si="22"/>
         <v>0.5</v>
       </c>
-      <c r="AA30" s="3">
+      <c r="AB30" s="3">
         <f t="shared" si="32"/>
         <v>0.625</v>
       </c>
-      <c r="AB30" s="18">
+      <c r="AC30" s="18">
         <f t="shared" si="26"/>
         <v>8</v>
       </c>
-      <c r="AC30" s="3">
+      <c r="AD30" s="3">
         <f t="shared" si="8"/>
         <v>0.625</v>
       </c>
-      <c r="AD30" s="3"/>
-    </row>
-    <row r="31" spans="2:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE30" s="3"/>
+    </row>
+    <row r="31" spans="2:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>70</v>
       </c>
@@ -5401,71 +5449,72 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
-      <c r="K31" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="K31" s="1"/>
       <c r="L31" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M31" s="1"/>
+      <c r="M31" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
-      <c r="P31" s="3">
+      <c r="P31" s="1"/>
+      <c r="Q31" s="3">
         <f t="shared" si="17"/>
         <v>1</v>
       </c>
-      <c r="Q31" s="3">
+      <c r="R31" s="3">
         <f t="shared" si="18"/>
         <v>0.4</v>
       </c>
-      <c r="R31" s="3">
+      <c r="S31" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S31" s="5">
+      <c r="T31" s="5">
         <f t="shared" si="29"/>
         <v>1.2000000000000002</v>
       </c>
-      <c r="T31" s="3">
+      <c r="U31" s="3">
         <f t="shared" si="30"/>
         <v>0.75000000000000011</v>
       </c>
-      <c r="U31" s="7">
+      <c r="V31" s="7">
         <f t="shared" si="31"/>
         <v>3.333333333333333</v>
       </c>
-      <c r="V31" s="4"/>
-      <c r="W31" s="3">
+      <c r="W31" s="4"/>
+      <c r="X31" s="3">
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
-      <c r="X31" s="3">
+      <c r="Y31" s="3">
         <f t="shared" si="21"/>
         <v>0.4</v>
       </c>
-      <c r="Y31" s="3">
+      <c r="Z31" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z31" s="5">
+      <c r="AA31" s="5">
         <f t="shared" si="22"/>
         <v>0.60000000000000009</v>
       </c>
-      <c r="AA31" s="3">
+      <c r="AB31" s="3">
         <f t="shared" si="32"/>
         <v>0.75000000000000011</v>
       </c>
-      <c r="AB31" s="18">
+      <c r="AC31" s="18">
         <f t="shared" si="26"/>
         <v>6.6666666666666661</v>
       </c>
-      <c r="AC31" s="3">
+      <c r="AD31" s="3">
         <f t="shared" si="8"/>
         <v>0.75000000000000011</v>
       </c>
-      <c r="AD31" s="17"/>
-    </row>
-    <row r="32" spans="2:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AE31" s="17"/>
+    </row>
+    <row r="32" spans="2:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>36</v>
       </c>
@@ -5488,62 +5537,63 @@
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
-      <c r="P32" s="3">
+      <c r="P32" s="1"/>
+      <c r="Q32" s="3">
         <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
-      <c r="Q32" s="3">
+      <c r="R32" s="3">
         <f t="shared" si="18"/>
         <v>0.4</v>
       </c>
-      <c r="R32" s="3">
+      <c r="S32" s="3">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="S32" s="5">
+      <c r="T32" s="5">
         <f t="shared" si="29"/>
         <v>1.5</v>
       </c>
-      <c r="T32" s="3">
+      <c r="U32" s="3">
         <f t="shared" si="30"/>
         <v>0.9375</v>
       </c>
-      <c r="U32" s="7">
+      <c r="V32" s="7">
         <f t="shared" si="31"/>
         <v>2.6666666666666665</v>
       </c>
-      <c r="V32" s="4"/>
-      <c r="W32" s="3">
+      <c r="W32" s="4"/>
+      <c r="X32" s="3">
         <f t="shared" si="20"/>
         <v>0.5</v>
       </c>
-      <c r="X32" s="3">
+      <c r="Y32" s="3">
         <f t="shared" si="21"/>
         <v>0.4</v>
       </c>
-      <c r="Y32" s="3">
+      <c r="Z32" s="3">
         <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
-      <c r="Z32" s="5">
+      <c r="AA32" s="5">
         <f t="shared" si="22"/>
         <v>0.75</v>
       </c>
-      <c r="AA32" s="3">
+      <c r="AB32" s="3">
         <f t="shared" si="32"/>
         <v>0.9375</v>
       </c>
-      <c r="AB32" s="18">
+      <c r="AC32" s="18">
         <f t="shared" si="26"/>
         <v>5.333333333333333</v>
       </c>
-      <c r="AC32" s="3">
+      <c r="AD32" s="3">
         <f t="shared" si="8"/>
         <v>0.9375</v>
       </c>
-      <c r="AD32" s="17"/>
-    </row>
-    <row r="33" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AE32" s="17"/>
+    </row>
+    <row r="33" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="1" t="s">
         <v>72</v>
@@ -5563,68 +5613,69 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
-      <c r="L33" s="1" t="s">
+      <c r="L33" s="1"/>
+      <c r="M33" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M33" s="1"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
-      <c r="P33" s="3">
+      <c r="P33" s="1"/>
+      <c r="Q33" s="3">
         <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
-      <c r="Q33" s="3">
+      <c r="R33" s="3">
         <f t="shared" si="18"/>
         <v>0.5</v>
       </c>
-      <c r="R33" s="3">
+      <c r="S33" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S33" s="5">
+      <c r="T33" s="5">
         <f t="shared" si="29"/>
         <v>1.75</v>
       </c>
-      <c r="T33" s="3">
+      <c r="U33" s="3">
         <f t="shared" si="30"/>
         <v>1.09375</v>
       </c>
-      <c r="U33" s="7">
+      <c r="V33" s="7">
         <f t="shared" si="31"/>
         <v>2.2857142857142856</v>
       </c>
-      <c r="V33" s="4"/>
-      <c r="W33" s="3">
+      <c r="W33" s="4"/>
+      <c r="X33" s="3">
         <f t="shared" si="20"/>
         <v>0.5</v>
       </c>
-      <c r="X33" s="3">
+      <c r="Y33" s="3">
         <f t="shared" si="21"/>
         <v>0.5</v>
       </c>
-      <c r="Y33" s="3">
+      <c r="Z33" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z33" s="5">
+      <c r="AA33" s="5">
         <f t="shared" si="22"/>
         <v>0.875</v>
       </c>
-      <c r="AA33" s="3">
+      <c r="AB33" s="3">
         <f t="shared" si="32"/>
         <v>1.09375</v>
       </c>
-      <c r="AB33" s="18">
+      <c r="AC33" s="18">
         <f t="shared" si="26"/>
         <v>4.5714285714285712</v>
       </c>
-      <c r="AC33" s="3">
+      <c r="AD33" s="3">
         <f t="shared" si="8"/>
         <v>1.09375</v>
       </c>
-      <c r="AD33" s="17"/>
-    </row>
-    <row r="34" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AE33" s="17"/>
+    </row>
+    <row r="34" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="8" t="s">
         <v>73</v>
@@ -5646,62 +5697,63 @@
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
-      <c r="P34" s="3">
+      <c r="P34" s="1"/>
+      <c r="Q34" s="3">
         <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
-      <c r="Q34" s="3">
+      <c r="R34" s="3">
         <f t="shared" si="18"/>
         <v>0.6</v>
       </c>
-      <c r="R34" s="3">
+      <c r="S34" s="3">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="S34" s="5">
+      <c r="T34" s="5">
         <f t="shared" si="29"/>
         <v>1.6</v>
       </c>
-      <c r="T34" s="3">
+      <c r="U34" s="3">
         <f t="shared" si="30"/>
         <v>1</v>
       </c>
-      <c r="U34" s="7">
+      <c r="V34" s="7">
         <f t="shared" si="31"/>
         <v>2.5</v>
       </c>
-      <c r="V34" s="4"/>
-      <c r="W34" s="3">
+      <c r="W34" s="4"/>
+      <c r="X34" s="3">
         <f t="shared" si="20"/>
         <v>0.5</v>
       </c>
-      <c r="X34" s="3">
+      <c r="Y34" s="3">
         <f t="shared" si="21"/>
         <v>0.6</v>
       </c>
-      <c r="Y34" s="3">
+      <c r="Z34" s="3">
         <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
-      <c r="Z34" s="5">
+      <c r="AA34" s="5">
         <f t="shared" si="22"/>
         <v>0.8</v>
       </c>
-      <c r="AA34" s="3">
+      <c r="AB34" s="3">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
-      <c r="AB34" s="18">
+      <c r="AC34" s="18">
         <f t="shared" si="26"/>
         <v>5</v>
       </c>
-      <c r="AC34" s="3">
+      <c r="AD34" s="3">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="AD34" s="17"/>
-    </row>
-    <row r="35" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AE34" s="17"/>
+    </row>
+    <row r="35" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="8" t="s">
         <v>35</v>
@@ -5720,71 +5772,72 @@
       <c r="H35" s="8"/>
       <c r="I35" s="8"/>
       <c r="J35" s="8"/>
-      <c r="K35" s="8" t="s">
-        <v>59</v>
-      </c>
+      <c r="K35" s="8"/>
       <c r="L35" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="M35" s="8"/>
+      <c r="M35" s="8" t="s">
+        <v>59</v>
+      </c>
       <c r="N35" s="8"/>
       <c r="O35" s="8"/>
-      <c r="P35" s="3">
+      <c r="P35" s="8"/>
+      <c r="Q35" s="3">
         <f t="shared" si="17"/>
         <v>1</v>
       </c>
-      <c r="Q35" s="3">
+      <c r="R35" s="3">
         <f t="shared" si="18"/>
         <v>0.4</v>
       </c>
-      <c r="R35" s="3">
+      <c r="S35" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S35" s="5">
+      <c r="T35" s="5">
         <f t="shared" si="29"/>
         <v>1.2000000000000002</v>
       </c>
-      <c r="T35" s="3">
+      <c r="U35" s="3">
         <f t="shared" si="30"/>
         <v>0.75000000000000011</v>
       </c>
-      <c r="U35" s="7">
+      <c r="V35" s="7">
         <f t="shared" si="31"/>
         <v>3.333333333333333</v>
       </c>
-      <c r="V35" s="4"/>
-      <c r="W35" s="3">
+      <c r="W35" s="4"/>
+      <c r="X35" s="3">
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
-      <c r="X35" s="3">
+      <c r="Y35" s="3">
         <f t="shared" si="21"/>
         <v>0.4</v>
       </c>
-      <c r="Y35" s="3">
+      <c r="Z35" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z35" s="5">
+      <c r="AA35" s="5">
         <f t="shared" si="22"/>
         <v>0.60000000000000009</v>
       </c>
-      <c r="AA35" s="3">
+      <c r="AB35" s="3">
         <f t="shared" si="32"/>
         <v>0.75000000000000011</v>
       </c>
-      <c r="AB35" s="18">
+      <c r="AC35" s="18">
         <f t="shared" si="26"/>
         <v>6.6666666666666661</v>
       </c>
-      <c r="AC35" s="3">
+      <c r="AD35" s="3">
         <f t="shared" si="8"/>
         <v>0.75000000000000011</v>
       </c>
-      <c r="AD35" s="17"/>
-    </row>
-    <row r="36" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AE35" s="17"/>
+    </row>
+    <row r="36" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="8"/>
       <c r="C36" s="9"/>
@@ -5800,23 +5853,24 @@
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
       <c r="O36" s="8"/>
-      <c r="P36" s="3"/>
+      <c r="P36" s="8"/>
       <c r="Q36" s="3"/>
       <c r="R36" s="3"/>
-      <c r="S36" s="5"/>
-      <c r="T36" s="3"/>
-      <c r="U36" s="7"/>
-      <c r="V36" s="4"/>
-      <c r="W36" s="3"/>
+      <c r="S36" s="3"/>
+      <c r="T36" s="5"/>
+      <c r="U36" s="3"/>
+      <c r="V36" s="7"/>
+      <c r="W36" s="4"/>
       <c r="X36" s="3"/>
       <c r="Y36" s="3"/>
-      <c r="Z36" s="5"/>
-      <c r="AA36" s="3"/>
-      <c r="AB36" s="18"/>
-      <c r="AC36" s="3"/>
-      <c r="AD36" s="17"/>
-    </row>
-    <row r="37" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z36" s="3"/>
+      <c r="AA36" s="5"/>
+      <c r="AB36" s="3"/>
+      <c r="AC36" s="18"/>
+      <c r="AD36" s="3"/>
+      <c r="AE36" s="17"/>
+    </row>
+    <row r="37" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
       <c r="B37" s="8"/>
       <c r="C37" s="9"/>
@@ -5832,23 +5886,24 @@
       <c r="M37" s="8"/>
       <c r="N37" s="8"/>
       <c r="O37" s="8"/>
-      <c r="P37" s="3"/>
+      <c r="P37" s="8"/>
       <c r="Q37" s="3"/>
       <c r="R37" s="3"/>
-      <c r="S37" s="5"/>
-      <c r="T37" s="3"/>
-      <c r="U37" s="7"/>
-      <c r="V37" s="4"/>
-      <c r="W37" s="3"/>
+      <c r="S37" s="3"/>
+      <c r="T37" s="5"/>
+      <c r="U37" s="3"/>
+      <c r="V37" s="7"/>
+      <c r="W37" s="4"/>
       <c r="X37" s="3"/>
       <c r="Y37" s="3"/>
-      <c r="Z37" s="5"/>
-      <c r="AA37" s="3"/>
-      <c r="AB37" s="18"/>
-      <c r="AC37" s="3"/>
-      <c r="AD37" s="17"/>
-    </row>
-    <row r="38" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z37" s="3"/>
+      <c r="AA37" s="5"/>
+      <c r="AB37" s="3"/>
+      <c r="AC37" s="18"/>
+      <c r="AD37" s="3"/>
+      <c r="AE37" s="17"/>
+    </row>
+    <row r="38" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="13"/>
       <c r="B38" s="8"/>
       <c r="C38" s="9"/>
@@ -5864,23 +5919,24 @@
       <c r="M38" s="8"/>
       <c r="N38" s="8"/>
       <c r="O38" s="8"/>
-      <c r="P38" s="3"/>
+      <c r="P38" s="8"/>
       <c r="Q38" s="3"/>
       <c r="R38" s="3"/>
-      <c r="S38" s="5"/>
-      <c r="T38" s="3"/>
-      <c r="U38" s="7"/>
-      <c r="V38" s="4"/>
-      <c r="W38" s="3"/>
+      <c r="S38" s="3"/>
+      <c r="T38" s="5"/>
+      <c r="U38" s="3"/>
+      <c r="V38" s="7"/>
+      <c r="W38" s="4"/>
       <c r="X38" s="3"/>
       <c r="Y38" s="3"/>
-      <c r="Z38" s="5"/>
-      <c r="AA38" s="3"/>
-      <c r="AB38" s="18"/>
-      <c r="AC38" s="3"/>
-      <c r="AD38" s="17"/>
-    </row>
-    <row r="39" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z38" s="3"/>
+      <c r="AA38" s="5"/>
+      <c r="AB38" s="3"/>
+      <c r="AC38" s="18"/>
+      <c r="AD38" s="3"/>
+      <c r="AE38" s="17"/>
+    </row>
+    <row r="39" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39" s="8"/>
       <c r="C39" s="9"/>
@@ -5896,23 +5952,24 @@
       <c r="M39" s="8"/>
       <c r="N39" s="8"/>
       <c r="O39" s="8"/>
-      <c r="P39" s="3"/>
+      <c r="P39" s="8"/>
       <c r="Q39" s="3"/>
       <c r="R39" s="3"/>
-      <c r="S39" s="5"/>
-      <c r="T39" s="3"/>
-      <c r="U39" s="7"/>
-      <c r="V39" s="4"/>
-      <c r="W39" s="3"/>
+      <c r="S39" s="3"/>
+      <c r="T39" s="5"/>
+      <c r="U39" s="3"/>
+      <c r="V39" s="7"/>
+      <c r="W39" s="4"/>
       <c r="X39" s="3"/>
       <c r="Y39" s="3"/>
-      <c r="Z39" s="5"/>
-      <c r="AA39" s="3"/>
-      <c r="AB39" s="18"/>
-      <c r="AC39" s="17"/>
+      <c r="Z39" s="3"/>
+      <c r="AA39" s="5"/>
+      <c r="AB39" s="3"/>
+      <c r="AC39" s="18"/>
       <c r="AD39" s="17"/>
-    </row>
-    <row r="40" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AE39" s="17"/>
+    </row>
+    <row r="40" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
       <c r="B40" s="8"/>
       <c r="C40" s="9"/>
@@ -5928,23 +5985,24 @@
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
-      <c r="P40" s="3"/>
+      <c r="P40" s="1"/>
       <c r="Q40" s="3"/>
       <c r="R40" s="3"/>
-      <c r="S40" s="5"/>
-      <c r="T40" s="3"/>
-      <c r="U40" s="17"/>
-      <c r="V40" s="4"/>
-      <c r="W40" s="3"/>
+      <c r="S40" s="3"/>
+      <c r="T40" s="5"/>
+      <c r="U40" s="3"/>
+      <c r="V40" s="17"/>
+      <c r="W40" s="4"/>
       <c r="X40" s="3"/>
       <c r="Y40" s="3"/>
-      <c r="Z40" s="5"/>
-      <c r="AA40" s="3"/>
-      <c r="AB40" s="18"/>
-      <c r="AC40" s="17"/>
+      <c r="Z40" s="3"/>
+      <c r="AA40" s="5"/>
+      <c r="AB40" s="3"/>
+      <c r="AC40" s="18"/>
       <c r="AD40" s="17"/>
-    </row>
-    <row r="41" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AE40" s="17"/>
+    </row>
+    <row r="41" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
       <c r="B41" s="8"/>
       <c r="C41" s="9"/>
@@ -5959,24 +6017,25 @@
       <c r="L41" s="8"/>
       <c r="M41" s="8"/>
       <c r="N41" s="8"/>
-      <c r="O41" s="10"/>
+      <c r="O41" s="8"/>
       <c r="P41" s="10"/>
       <c r="Q41" s="10"/>
       <c r="R41" s="10"/>
       <c r="S41" s="10"/>
-      <c r="T41" s="11"/>
-      <c r="U41" s="12"/>
-      <c r="V41" s="10"/>
+      <c r="T41" s="10"/>
+      <c r="U41" s="11"/>
+      <c r="V41" s="12"/>
       <c r="W41" s="10"/>
       <c r="X41" s="10"/>
       <c r="Y41" s="10"/>
       <c r="Z41" s="10"/>
-      <c r="AA41" s="11"/>
-      <c r="AB41" s="10"/>
-      <c r="AC41" s="14"/>
+      <c r="AA41" s="10"/>
+      <c r="AB41" s="11"/>
+      <c r="AC41" s="10"/>
       <c r="AD41" s="14"/>
-    </row>
-    <row r="42" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AE41" s="14"/>
+    </row>
+    <row r="42" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
       <c r="B42" s="8"/>
       <c r="C42" s="9"/>
@@ -5991,24 +6050,25 @@
       <c r="L42" s="8"/>
       <c r="M42" s="8"/>
       <c r="N42" s="8"/>
-      <c r="O42" s="10"/>
+      <c r="O42" s="8"/>
       <c r="P42" s="10"/>
       <c r="Q42" s="10"/>
       <c r="R42" s="10"/>
       <c r="S42" s="10"/>
-      <c r="T42" s="11"/>
-      <c r="U42" s="12"/>
-      <c r="V42" s="10"/>
+      <c r="T42" s="10"/>
+      <c r="U42" s="11"/>
+      <c r="V42" s="12"/>
       <c r="W42" s="10"/>
       <c r="X42" s="10"/>
       <c r="Y42" s="10"/>
       <c r="Z42" s="10"/>
-      <c r="AA42" s="11"/>
-      <c r="AB42" s="10"/>
-      <c r="AC42" s="14"/>
+      <c r="AA42" s="10"/>
+      <c r="AB42" s="11"/>
+      <c r="AC42" s="10"/>
       <c r="AD42" s="14"/>
-    </row>
-    <row r="43" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AE42" s="14"/>
+    </row>
+    <row r="43" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
       <c r="B43" s="8"/>
       <c r="C43" s="9"/>
@@ -6023,52 +6083,53 @@
       <c r="L43" s="8"/>
       <c r="M43" s="8"/>
       <c r="N43" s="8"/>
-      <c r="O43" s="10"/>
+      <c r="O43" s="8"/>
       <c r="P43" s="10"/>
       <c r="Q43" s="10"/>
       <c r="R43" s="10"/>
       <c r="S43" s="10"/>
-      <c r="T43" s="11"/>
-      <c r="U43" s="12"/>
-      <c r="V43" s="10"/>
+      <c r="T43" s="10"/>
+      <c r="U43" s="11"/>
+      <c r="V43" s="12"/>
       <c r="W43" s="10"/>
       <c r="X43" s="10"/>
       <c r="Y43" s="10"/>
       <c r="Z43" s="10"/>
-      <c r="AA43" s="11"/>
-      <c r="AB43" s="10"/>
-      <c r="AC43" s="14"/>
+      <c r="AA43" s="10"/>
+      <c r="AB43" s="11"/>
+      <c r="AC43" s="10"/>
       <c r="AD43" s="14"/>
-    </row>
-    <row r="44" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AE43" s="14"/>
+    </row>
+    <row r="44" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>
       <c r="B44" s="8"/>
       <c r="C44" s="9"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
     </row>
-    <row r="45" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="15"/>
       <c r="B45" s="8"/>
       <c r="C45" s="9"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
     </row>
-    <row r="46" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
       <c r="B46" s="8"/>
       <c r="C46" s="9"/>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
     </row>
-    <row r="47" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
       <c r="B47" s="8"/>
       <c r="C47" s="9"/>
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
     </row>
-    <row r="48" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="13"/>
       <c r="B48" s="8"/>
       <c r="C48" s="9"/>
@@ -6203,10 +6264,10 @@
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="X2:AA2"/>
   </mergeCells>
-  <conditionalFormatting sqref="AD34">
+  <conditionalFormatting sqref="AE34">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -6218,7 +6279,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA41:AA43 T41:T43 U4:U39 AB4:AB39">
+  <conditionalFormatting sqref="AB41:AB43 U41:U43 V4:V39 AC4:AC39">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -6230,7 +6291,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z41:Z43 S41:S43 AA4:AA39 T4:T39">
+  <conditionalFormatting sqref="AA41:AA43 T41:T43 AB4:AB39 U4:U39">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -6242,7 +6303,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB41:AB43 AD31:AD33 AC36:AD39 AC4:AD4 AD35 AD5:AD28 AC5:AC35">
+  <conditionalFormatting sqref="AC41:AC43 AE31:AE33 AD36:AE39 AD4:AE4 AE35 AE5:AE28 AD5:AD35">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -6254,7 +6315,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD30">
+  <conditionalFormatting sqref="AE30">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -6278,7 +6339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AJ68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
@@ -6292,24 +6353,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="Q2" s="30" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="Q2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="X2" s="30" t="s">
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="X2" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="Y2" s="30"/>
-      <c r="Z2" s="30"/>
-      <c r="AA2" s="30"/>
+      <c r="Y2" s="31"/>
+      <c r="Z2" s="31"/>
+      <c r="AA2" s="31"/>
       <c r="AB2" s="26"/>
       <c r="AC2" s="26"/>
       <c r="AF2" t="s">
@@ -9043,7 +9104,7 @@
       <c r="D38" s="8">
         <v>3</v>
       </c>
-      <c r="E38" s="31" t="s">
+      <c r="E38" s="30" t="s">
         <v>139</v>
       </c>
       <c r="F38" s="8" t="s">
@@ -9620,7 +9681,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC40 V40">
+  <conditionalFormatting sqref="V40 AC40">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -9632,7 +9693,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U40 AB40">
+  <conditionalFormatting sqref="AB40 U40">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -9681,24 +9742,24 @@
   <sheetData>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="R2" s="30" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="R2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
-      <c r="Y2" s="30" t="s">
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
+      <c r="Y2" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="Z2" s="30"/>
-      <c r="AA2" s="30"/>
-      <c r="AB2" s="30"/>
+      <c r="Z2" s="31"/>
+      <c r="AA2" s="31"/>
+      <c r="AB2" s="31"/>
       <c r="AC2" s="21"/>
       <c r="AD2" s="21"/>
       <c r="AG2" t="s">
@@ -12260,7 +12321,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD30 W30">
+  <conditionalFormatting sqref="W30 AD30">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -12272,7 +12333,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC30 V30">
+  <conditionalFormatting sqref="V30 AC30">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -12296,7 +12357,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD34 W34">
+  <conditionalFormatting sqref="W34 AD34">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -12308,7 +12369,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC34 V34">
+  <conditionalFormatting sqref="V34 AC34">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -12357,24 +12418,24 @@
   <sheetData>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="P2" s="30" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="P2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="W2" s="30" t="s">
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="W2" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="X2" s="30"/>
-      <c r="Y2" s="30"/>
-      <c r="Z2" s="30"/>
+      <c r="X2" s="31"/>
+      <c r="Y2" s="31"/>
+      <c r="Z2" s="31"/>
       <c r="AA2" s="24"/>
       <c r="AB2" s="24"/>
       <c r="AE2" t="s">
@@ -14993,7 +15054,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB31 U31">
+  <conditionalFormatting sqref="U31 AB31">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -15005,7 +15066,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA31 T31">
+  <conditionalFormatting sqref="T31 AA31">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -15029,7 +15090,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB35 U35">
+  <conditionalFormatting sqref="U35 AB35">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -15041,7 +15102,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA35 T35">
+  <conditionalFormatting sqref="T35 AA35">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0.5"/>

</xml_diff>